<commit_message>
Jurisdiction area - added desc: used by >among others< RCG LDF
Description update: Jurisdiction area - added desc: used by >among others< RCG LDF
v1.18.4
</commit_message>
<xml_diff>
--- a/Documents/RDBES Data Model.xlsx
+++ b/Documents/RDBES Data Model.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="17430" windowHeight="5595" tabRatio="747" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="17430" windowHeight="5595"/>
   </bookViews>
   <sheets>
-    <sheet name="Model v1.18.3" sheetId="1" r:id="rId1"/>
+    <sheet name="Model v1.18.4" sheetId="1" r:id="rId1"/>
     <sheet name="Design" sheetId="5" r:id="rId2"/>
     <sheet name="Temporal Event" sheetId="21" r:id="rId3"/>
     <sheet name="Location" sheetId="20" r:id="rId4"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3020" uniqueCount="1176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3020" uniqueCount="1178">
   <si>
     <t>Design Table (DE)</t>
   </si>
@@ -3006,9 +3006,6 @@
   </si>
   <si>
     <t>LEjurisdArea</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dominant Area belonging to a country or a part of an area used by Long Distance Fisheries. </t>
   </si>
   <si>
     <t>SAjurisdictionArea</t>
@@ -3547,25 +3544,6 @@
   </si>
   <si>
     <t xml:space="preserve">Mesh size (mm).  The following: LLD, LLS, LHM, LHP, LL, FPO cannot insert mesh size. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indicating the sampling scheme type code list: 'Regional Routine', 'Regional Pilot', 'National Routine', 'National Pilot', 'Research project' or 'DCF'. Routine is continued maybe with updates each year. A pilot is a test of a routine so it is done for the first time for a short periode. Research is all other studies/projects. </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> Sampling scheme type code list: 
-'DCF R-CFM' 
-'Regional Routine', 'Regional Pilot', 'National Routine', 'National Pilot'</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">. </t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">Date when of the gear start. "YYYY-MM-DD" (UTC). date and time of shooting (active) or last setting (passive) of the gear. </t>
@@ -3872,6 +3850,115 @@
         <scheme val="minor"/>
       </rPr>
       <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Indicating the sampling scheme type code list: 'Regional Routine', 'Regional Pilot', 'National Routine', 'National Pilot' or 'Research project'. Routine is continued maybe with updates each year. A pilot is a test of a routine so it is done for the first time for a short periode. Research is all other studies/projects. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> Sampling scheme type code list: 
+'Regional Routine', 'Regional Pilot', 'National Routine', 'National Pilot'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Area belonging to a country or a part of an area </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">among others </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">used by Long Distance Fisheries. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Area belonging to a country or a part of an area </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>among</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">others </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">used by Long Distance Fisheries. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dominant Area belonging to a country or a part of an area </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">among others </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">used by Long Distance Fisheries. </t>
     </r>
   </si>
 </sst>
@@ -4588,8 +4675,8 @@
   </sheetPr>
   <dimension ref="A1:AI112"/>
   <sheetViews>
-    <sheetView showZeros="0" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="V10" sqref="V10"/>
+    <sheetView showZeros="0" tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5024,7 +5111,6 @@
       <c r="C7" s="43" t="str">
         <f>IF(ISBLANK(Design!A5)=TRUE, Design!L5, "")</f>
         <v xml:space="preserve"> Sampling scheme type code list: 
-'DCF R-CFM' 
 'Regional Routine', 'Regional Pilot', 'National Routine', 'National Pilot'. </v>
       </c>
       <c r="E7" s="18">
@@ -5948,7 +6034,7 @@
         <v>The number of fish measured in this stratum</v>
       </c>
     </row>
-    <row r="17" spans="9:35" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="9:35" ht="47.25" x14ac:dyDescent="0.25">
       <c r="I17" s="18" t="str">
         <f>IF(ISBLANK('Temporal Event'!A2)=TRUE, 'Temporal Event'!B2, "")</f>
         <v/>
@@ -8774,8 +8860,8 @@
   </sheetPr>
   <dimension ref="A1:XFD61"/>
   <sheetViews>
-    <sheetView topLeftCell="G13" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView topLeftCell="F30" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8810,7 +8896,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="84" t="s">
-        <v>1171</v>
+        <v>1168</v>
       </c>
       <c r="F1" s="26" t="s">
         <v>134</v>
@@ -8843,7 +8929,7 @@
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E2" s="27" t="s">
         <v>3</v>
@@ -8877,7 +8963,7 @@
         <v>267</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E3" s="27" t="s">
         <v>122</v>
@@ -8913,7 +8999,7 @@
         <v>267</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E4" s="27" t="s">
         <v>288</v>
@@ -8949,7 +9035,7 @@
         <v>267</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E5" s="27" t="s">
         <v>680</v>
@@ -8983,7 +9069,7 @@
       </c>
       <c r="C6" s="27"/>
       <c r="D6" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E6" s="27" t="s">
         <v>87</v>
@@ -9019,7 +9105,7 @@
         <v>267</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E7" s="27" t="s">
         <v>260</v>
@@ -9055,7 +9141,7 @@
         <v>267</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E8" s="27" t="s">
         <v>653</v>
@@ -9091,7 +9177,7 @@
         <v>267</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E9" s="27" t="s">
         <v>976</v>
@@ -9159,22 +9245,22 @@
         <v>688</v>
       </c>
       <c r="F11" s="36" t="s">
+        <v>1072</v>
+      </c>
+      <c r="G11" s="36" t="s">
         <v>1073</v>
       </c>
-      <c r="G11" s="36" t="s">
-        <v>1074</v>
-      </c>
       <c r="H11" s="36" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
       <c r="I11" s="36" t="s">
         <v>11</v>
       </c>
       <c r="J11" s="36" t="s">
-        <v>1165</v>
+        <v>1162</v>
       </c>
       <c r="K11" s="36" t="s">
-        <v>1153</v>
+        <v>1150</v>
       </c>
       <c r="L11" s="36" t="s">
         <v>683</v>
@@ -9571,10 +9657,10 @@
         <v>11</v>
       </c>
       <c r="J23" s="49" t="s">
-        <v>1157</v>
+        <v>1154</v>
       </c>
       <c r="K23" s="36" t="s">
-        <v>1158</v>
+        <v>1155</v>
       </c>
       <c r="L23" s="36" t="s">
         <v>199</v>
@@ -9657,10 +9743,10 @@
         <v>969</v>
       </c>
       <c r="F26" s="35" t="s">
+        <v>1075</v>
+      </c>
+      <c r="G26" s="35" t="s">
         <v>1076</v>
-      </c>
-      <c r="G26" s="35" t="s">
-        <v>1077</v>
       </c>
       <c r="H26" s="36" t="s">
         <v>10</v>
@@ -9672,7 +9758,7 @@
         <v>14</v>
       </c>
       <c r="K26" s="36" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="L26" s="36" t="s">
         <v>971</v>
@@ -9706,7 +9792,7 @@
         <v>14</v>
       </c>
       <c r="K27" s="36" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="L27" s="36" t="s">
         <v>202</v>
@@ -9740,7 +9826,7 @@
         <v>14</v>
       </c>
       <c r="K28" s="36" t="s">
-        <v>1173</v>
+        <v>1170</v>
       </c>
       <c r="L28" s="36" t="s">
         <v>203</v>
@@ -9756,16 +9842,16 @@
         <v>20</v>
       </c>
       <c r="E29" s="35" t="s">
+        <v>987</v>
+      </c>
+      <c r="F29" s="35" t="s">
+        <v>1074</v>
+      </c>
+      <c r="G29" s="35" t="s">
+        <v>1074</v>
+      </c>
+      <c r="H29" s="35" t="s">
         <v>988</v>
-      </c>
-      <c r="F29" s="35" t="s">
-        <v>1075</v>
-      </c>
-      <c r="G29" s="35" t="s">
-        <v>1075</v>
-      </c>
-      <c r="H29" s="35" t="s">
-        <v>989</v>
       </c>
       <c r="I29" s="35" t="s">
         <v>11</v>
@@ -9774,10 +9860,10 @@
         <v>14</v>
       </c>
       <c r="K29" s="36" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="L29" s="36" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="M29" s="70"/>
       <c r="N29" s="70"/>
@@ -9808,7 +9894,7 @@
         <v>14</v>
       </c>
       <c r="K30" s="35" t="s">
-        <v>985</v>
+        <v>1177</v>
       </c>
       <c r="L30" s="35" t="s">
         <v>980</v>
@@ -9842,7 +9928,7 @@
         <v>14</v>
       </c>
       <c r="K31" s="36" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="L31" s="36" t="s">
         <v>721</v>
@@ -9876,7 +9962,7 @@
         <v>14</v>
       </c>
       <c r="K32" s="36" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="L32" s="36" t="s">
         <v>173</v>
@@ -9892,7 +9978,7 @@
         <v>24</v>
       </c>
       <c r="E33" s="35" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="F33" s="35" t="s">
         <v>761</v>
@@ -9910,7 +9996,7 @@
         <v>14</v>
       </c>
       <c r="K33" s="36" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="L33" s="36" t="s">
         <v>174</v>
@@ -9944,7 +10030,7 @@
         <v>14</v>
       </c>
       <c r="K34" s="36" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="L34" s="36" t="s">
         <v>101</v>
@@ -9976,7 +10062,7 @@
       </c>
       <c r="J35" s="36"/>
       <c r="K35" s="36" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="L35" s="36" t="s">
         <v>39</v>
@@ -10010,7 +10096,7 @@
         <v>14</v>
       </c>
       <c r="K36" s="36" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="L36" s="36" t="s">
         <v>40</v>
@@ -10042,7 +10128,7 @@
       </c>
       <c r="J37" s="36"/>
       <c r="K37" s="36" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="L37" s="36" t="s">
         <v>175</v>
@@ -10092,10 +10178,10 @@
         <v>30</v>
       </c>
       <c r="E39" s="35" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="F39" s="35" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="G39" s="35" t="s">
         <v>763</v>
@@ -10110,7 +10196,7 @@
         <v>14</v>
       </c>
       <c r="K39" s="36" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="L39" s="36"/>
       <c r="M39" s="70"/>
@@ -10221,10 +10307,10 @@
         <v>736</v>
       </c>
       <c r="F43" s="35" t="s">
+        <v>1077</v>
+      </c>
+      <c r="G43" s="35" t="s">
         <v>1078</v>
-      </c>
-      <c r="G43" s="35" t="s">
-        <v>1079</v>
       </c>
       <c r="H43" s="36" t="s">
         <v>187</v>
@@ -10253,10 +10339,10 @@
         <v>154</v>
       </c>
       <c r="F44" s="35" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="G44" s="36" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="H44" s="36" t="s">
         <v>187</v>
@@ -10332,10 +10418,10 @@
       </c>
       <c r="J46" s="64"/>
       <c r="K46" s="63" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="L46" s="63" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="M46" s="55"/>
       <c r="N46" s="55"/>
@@ -10447,10 +10533,10 @@
         <v>828</v>
       </c>
       <c r="F50" s="35" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="G50" s="35" t="s">
-        <v>1084</v>
+        <v>1083</v>
       </c>
       <c r="H50" s="36" t="s">
         <v>187</v>
@@ -10479,10 +10565,10 @@
         <v>829</v>
       </c>
       <c r="F51" s="35" t="s">
+        <v>1081</v>
+      </c>
+      <c r="G51" s="36" t="s">
         <v>1082</v>
-      </c>
-      <c r="G51" s="36" t="s">
-        <v>1083</v>
       </c>
       <c r="H51" s="36" t="s">
         <v>187</v>
@@ -10509,10 +10595,10 @@
         <v>818</v>
       </c>
       <c r="F52" s="35" t="s">
+        <v>1034</v>
+      </c>
+      <c r="G52" s="35" t="s">
         <v>1035</v>
-      </c>
-      <c r="G52" s="35" t="s">
-        <v>1036</v>
       </c>
       <c r="H52" s="36" t="s">
         <v>10</v>
@@ -10630,7 +10716,7 @@
     </row>
     <row r="57" spans="1:16384" x14ac:dyDescent="0.25">
       <c r="A57" s="83" t="s">
-        <v>1169</v>
+        <v>1166</v>
       </c>
       <c r="B57" s="83"/>
       <c r="C57" s="83"/>
@@ -27126,7 +27212,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="84" t="s">
-        <v>1171</v>
+        <v>1168</v>
       </c>
       <c r="F1" s="26" t="s">
         <v>134</v>
@@ -27159,7 +27245,7 @@
       </c>
       <c r="C2" s="31"/>
       <c r="D2" s="31" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E2" s="31" t="s">
         <v>208</v>
@@ -27193,7 +27279,7 @@
         <v>265</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E3" s="31" t="s">
         <v>3</v>
@@ -27229,7 +27315,7 @@
         <v>265</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E4" s="31" t="s">
         <v>90</v>
@@ -27265,7 +27351,7 @@
         <v>265</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E5" s="31" t="s">
         <v>288</v>
@@ -27299,7 +27385,7 @@
         <v>265</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E6" s="31" t="s">
         <v>274</v>
@@ -27333,7 +27419,7 @@
         <v>265</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E7" s="31" t="s">
         <v>260</v>
@@ -27363,7 +27449,7 @@
       <c r="B8" s="31"/>
       <c r="C8" s="31"/>
       <c r="D8" s="31" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E8" s="31" t="s">
         <v>681</v>
@@ -27382,7 +27468,7 @@
       </c>
       <c r="J8" s="31"/>
       <c r="K8" s="31" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="L8" s="31" t="s">
         <v>682</v>
@@ -27503,7 +27589,7 @@
         <v>665</v>
       </c>
       <c r="F12" s="35" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="G12" s="35" t="s">
         <v>666</v>
@@ -27553,7 +27639,7 @@
       </c>
       <c r="J13" s="53"/>
       <c r="K13" s="76" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="L13" s="76" t="s">
         <v>526</v>
@@ -27575,7 +27661,7 @@
         <v>667</v>
       </c>
       <c r="F14" s="60" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="G14" s="60" t="s">
         <v>669</v>
@@ -27746,10 +27832,10 @@
         <v>614</v>
       </c>
       <c r="F19" s="53" t="s">
+        <v>1111</v>
+      </c>
+      <c r="G19" s="53" t="s">
         <v>1112</v>
-      </c>
-      <c r="G19" s="53" t="s">
-        <v>1113</v>
       </c>
       <c r="H19" s="53" t="s">
         <v>10</v>
@@ -27880,10 +27966,10 @@
         <v>736</v>
       </c>
       <c r="F23" s="35" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="G23" s="35" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="H23" s="36" t="s">
         <v>187</v>
@@ -27913,10 +27999,10 @@
         <v>154</v>
       </c>
       <c r="F24" s="35" t="s">
+        <v>1117</v>
+      </c>
+      <c r="G24" s="36" t="s">
         <v>1118</v>
-      </c>
-      <c r="G24" s="36" t="s">
-        <v>1119</v>
       </c>
       <c r="H24" s="36" t="s">
         <v>187</v>
@@ -28113,10 +28199,10 @@
         <v>828</v>
       </c>
       <c r="F30" s="35" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="G30" s="35" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="H30" s="36" t="s">
         <v>187</v>
@@ -28146,10 +28232,10 @@
         <v>829</v>
       </c>
       <c r="F31" s="35" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="G31" s="36" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="H31" s="36" t="s">
         <v>187</v>
@@ -28177,10 +28263,10 @@
         <v>818</v>
       </c>
       <c r="F32" s="35" t="s">
+        <v>1036</v>
+      </c>
+      <c r="G32" s="35" t="s">
         <v>1037</v>
-      </c>
-      <c r="G32" s="35" t="s">
-        <v>1038</v>
       </c>
       <c r="H32" s="36" t="s">
         <v>10</v>
@@ -28365,8 +28451,8 @@
   </sheetPr>
   <dimension ref="A1:V60"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView topLeftCell="E18" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28399,7 +28485,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="85" t="s">
-        <v>1171</v>
+        <v>1168</v>
       </c>
       <c r="F1" s="41" t="s">
         <v>134</v>
@@ -28432,7 +28518,7 @@
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E2" s="27" t="s">
         <v>653</v>
@@ -28466,7 +28552,7 @@
         <v>770</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E3" s="27" t="s">
         <v>208</v>
@@ -28579,7 +28665,7 @@
         <v>3</v>
       </c>
       <c r="E6" s="60" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="F6" s="36" t="s">
         <v>795</v>
@@ -28743,13 +28829,13 @@
         <v>7</v>
       </c>
       <c r="E10" s="60" t="s">
+        <v>1138</v>
+      </c>
+      <c r="F10" s="60" t="s">
         <v>1139</v>
       </c>
-      <c r="F10" s="60" t="s">
+      <c r="G10" s="60" t="s">
         <v>1140</v>
-      </c>
-      <c r="G10" s="60" t="s">
-        <v>1141</v>
       </c>
       <c r="H10" s="60" t="s">
         <v>10</v>
@@ -28761,7 +28847,7 @@
         <v>14</v>
       </c>
       <c r="K10" s="36" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="L10" s="36" t="s">
         <v>689</v>
@@ -28847,7 +28933,7 @@
         <v>14</v>
       </c>
       <c r="K12" s="53" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="L12" s="53" t="s">
         <v>662</v>
@@ -29067,7 +29153,7 @@
         <v>14</v>
       </c>
       <c r="K17" s="36" t="s">
-        <v>1170</v>
+        <v>1167</v>
       </c>
       <c r="L17" s="36" t="s">
         <v>21</v>
@@ -29094,10 +29180,10 @@
         <v>969</v>
       </c>
       <c r="F18" s="79" t="s">
+        <v>996</v>
+      </c>
+      <c r="G18" s="79" t="s">
         <v>997</v>
-      </c>
-      <c r="G18" s="79" t="s">
-        <v>998</v>
       </c>
       <c r="H18" s="36" t="s">
         <v>10</v>
@@ -29193,7 +29279,7 @@
         <v>14</v>
       </c>
       <c r="K20" s="36" t="s">
-        <v>1174</v>
+        <v>1171</v>
       </c>
       <c r="L20" s="36" t="s">
         <v>203</v>
@@ -29217,16 +29303,16 @@
         <v>18</v>
       </c>
       <c r="E21" s="36" t="s">
+        <v>987</v>
+      </c>
+      <c r="F21" s="36" t="s">
+        <v>1108</v>
+      </c>
+      <c r="G21" s="36" t="s">
+        <v>1108</v>
+      </c>
+      <c r="H21" s="36" t="s">
         <v>988</v>
-      </c>
-      <c r="F21" s="36" t="s">
-        <v>1109</v>
-      </c>
-      <c r="G21" s="36" t="s">
-        <v>1109</v>
-      </c>
-      <c r="H21" s="36" t="s">
-        <v>989</v>
       </c>
       <c r="I21" s="36" t="s">
         <v>11</v>
@@ -29235,10 +29321,10 @@
         <v>14</v>
       </c>
       <c r="K21" s="36" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="L21" s="36" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="M21" s="55"/>
       <c r="N21" s="55"/>
@@ -29262,10 +29348,10 @@
         <v>979</v>
       </c>
       <c r="F22" s="36" t="s">
+        <v>985</v>
+      </c>
+      <c r="G22" s="36" t="s">
         <v>986</v>
-      </c>
-      <c r="G22" s="36" t="s">
-        <v>987</v>
       </c>
       <c r="H22" s="36" t="s">
         <v>10</v>
@@ -29277,7 +29363,7 @@
         <v>14</v>
       </c>
       <c r="K22" s="36" t="s">
-        <v>980</v>
+        <v>1176</v>
       </c>
       <c r="L22" s="36" t="s">
         <v>980</v>
@@ -29377,7 +29463,7 @@
       <c r="U24" s="55"/>
       <c r="V24" s="55"/>
     </row>
-    <row r="25" spans="1:22" s="24" customFormat="1" ht="108.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" s="24" customFormat="1" ht="96.75" x14ac:dyDescent="0.25">
       <c r="A25" s="36"/>
       <c r="B25" s="36"/>
       <c r="C25" s="36"/>
@@ -29647,7 +29733,7 @@
       </c>
       <c r="J31" s="60"/>
       <c r="K31" s="36" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="L31" s="36" t="s">
         <v>218</v>
@@ -29687,7 +29773,7 @@
       </c>
       <c r="J32" s="60"/>
       <c r="K32" s="36" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="L32" s="36" t="s">
         <v>219</v>
@@ -29794,10 +29880,10 @@
         <v>736</v>
       </c>
       <c r="F35" s="35" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="G35" s="35" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="H35" s="36" t="s">
         <v>187</v>
@@ -29834,10 +29920,10 @@
         <v>154</v>
       </c>
       <c r="F36" s="35" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="G36" s="36" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="H36" s="36" t="s">
         <v>187</v>
@@ -30038,10 +30124,10 @@
         <v>818</v>
       </c>
       <c r="F41" s="35" t="s">
+        <v>1038</v>
+      </c>
+      <c r="G41" s="35" t="s">
         <v>1039</v>
-      </c>
-      <c r="G41" s="35" t="s">
-        <v>1040</v>
       </c>
       <c r="H41" s="36" t="s">
         <v>10</v>
@@ -30165,7 +30251,7 @@
       </c>
       <c r="J44" s="60"/>
       <c r="K44" s="36" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="L44" s="36" t="s">
         <v>218</v>
@@ -30205,7 +30291,7 @@
       </c>
       <c r="J45" s="60"/>
       <c r="K45" s="36" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="L45" s="36" t="s">
         <v>219</v>
@@ -30643,7 +30729,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="84" t="s">
-        <v>1171</v>
+        <v>1168</v>
       </c>
       <c r="F1" s="26" t="s">
         <v>134</v>
@@ -30676,7 +30762,7 @@
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E2" s="27" t="s">
         <v>296</v>
@@ -30710,7 +30796,7 @@
         <v>267</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E3" s="27" t="s">
         <v>653</v>
@@ -30868,10 +30954,10 @@
         <v>656</v>
       </c>
       <c r="F8" s="60" t="s">
+        <v>1041</v>
+      </c>
+      <c r="G8" s="60" t="s">
         <v>1042</v>
-      </c>
-      <c r="G8" s="60" t="s">
-        <v>1043</v>
       </c>
       <c r="H8" s="60" t="s">
         <v>10</v>
@@ -30964,10 +31050,10 @@
         <v>733</v>
       </c>
       <c r="F11" s="60" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="G11" s="36" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="H11" s="60" t="s">
         <v>187</v>
@@ -30992,10 +31078,10 @@
         <v>735</v>
       </c>
       <c r="F12" s="36" t="s">
+        <v>1044</v>
+      </c>
+      <c r="G12" s="36" t="s">
         <v>1045</v>
-      </c>
-      <c r="G12" s="36" t="s">
-        <v>1046</v>
       </c>
       <c r="H12" s="36" t="s">
         <v>10</v>
@@ -31058,7 +31144,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="84" t="s">
-        <v>1171</v>
+        <v>1168</v>
       </c>
       <c r="F1" s="26" t="s">
         <v>134</v>
@@ -31091,7 +31177,7 @@
       </c>
       <c r="C2" s="32"/>
       <c r="D2" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E2" s="32" t="s">
         <v>4</v>
@@ -31127,7 +31213,7 @@
         <v>267</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E3" s="32" t="s">
         <v>227</v>
@@ -31163,7 +31249,7 @@
         <v>267</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E4" s="27" t="s">
         <v>296</v>
@@ -31228,13 +31314,13 @@
         <v>2</v>
       </c>
       <c r="E6" s="36" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="F6" s="60" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="G6" s="60" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="H6" s="60" t="s">
         <v>13</v>
@@ -31244,7 +31330,7 @@
       </c>
       <c r="J6" s="60"/>
       <c r="K6" s="36" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="L6" s="36" t="s">
         <v>232</v>
@@ -31338,7 +31424,7 @@
         <v>14</v>
       </c>
       <c r="K9" s="36" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="L9" s="60" t="s">
         <v>247</v>
@@ -31449,10 +31535,10 @@
         <v>656</v>
       </c>
       <c r="F13" s="60" t="s">
+        <v>1056</v>
+      </c>
+      <c r="G13" s="60" t="s">
         <v>1057</v>
-      </c>
-      <c r="G13" s="60" t="s">
-        <v>1058</v>
       </c>
       <c r="H13" s="60" t="s">
         <v>10</v>
@@ -31541,10 +31627,10 @@
         <v>736</v>
       </c>
       <c r="F16" s="35" t="s">
+        <v>1059</v>
+      </c>
+      <c r="G16" s="35" t="s">
         <v>1060</v>
-      </c>
-      <c r="G16" s="35" t="s">
-        <v>1061</v>
       </c>
       <c r="H16" s="36" t="s">
         <v>187</v>
@@ -31571,10 +31657,10 @@
         <v>154</v>
       </c>
       <c r="F17" s="35" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="G17" s="36" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="H17" s="36" t="s">
         <v>187</v>
@@ -31694,8 +31780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31729,7 +31815,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="84" t="s">
-        <v>1171</v>
+        <v>1168</v>
       </c>
       <c r="F1" s="26" t="s">
         <v>134</v>
@@ -31762,7 +31848,7 @@
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E2" s="27" t="s">
         <v>135</v>
@@ -31877,10 +31963,10 @@
         <v>14</v>
       </c>
       <c r="K5" s="54" t="s">
-        <v>1148</v>
+        <v>1173</v>
       </c>
       <c r="L5" s="54" t="s">
-        <v>1149</v>
+        <v>1174</v>
       </c>
     </row>
     <row r="6" spans="1:12" s="11" customFormat="1" ht="12" x14ac:dyDescent="0.2">
@@ -32590,7 +32676,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="84" t="s">
-        <v>1171</v>
+        <v>1168</v>
       </c>
       <c r="F1" s="26" t="s">
         <v>134</v>
@@ -32623,7 +32709,7 @@
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E2" s="27" t="s">
         <v>260</v>
@@ -32657,7 +32743,7 @@
         <v>267</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E3" s="27" t="s">
         <v>851</v>
@@ -32691,7 +32777,7 @@
         <v>267</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E4" s="27" t="s">
         <v>131</v>
@@ -32725,7 +32811,7 @@
         <v>267</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E5" s="27" t="s">
         <v>337</v>
@@ -33069,10 +33155,10 @@
         <v>736</v>
       </c>
       <c r="F16" s="35" t="s">
-        <v>1126</v>
+        <v>1125</v>
       </c>
       <c r="G16" s="35" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="H16" s="36" t="s">
         <v>187</v>
@@ -33099,10 +33185,10 @@
         <v>154</v>
       </c>
       <c r="F17" s="35" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="G17" s="36" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="H17" s="36" t="s">
         <v>187</v>
@@ -33174,10 +33260,10 @@
       </c>
       <c r="J19" s="36"/>
       <c r="K19" s="36" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="L19" s="36" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="20" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -33281,10 +33367,10 @@
         <v>828</v>
       </c>
       <c r="F23" s="35" t="s">
+        <v>1121</v>
+      </c>
+      <c r="G23" s="35" t="s">
         <v>1122</v>
-      </c>
-      <c r="G23" s="35" t="s">
-        <v>1123</v>
       </c>
       <c r="H23" s="36" t="s">
         <v>187</v>
@@ -33311,10 +33397,10 @@
         <v>829</v>
       </c>
       <c r="F24" s="35" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="G24" s="36" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="H24" s="36" t="s">
         <v>187</v>
@@ -33339,10 +33425,10 @@
         <v>818</v>
       </c>
       <c r="F25" s="35" t="s">
+        <v>1028</v>
+      </c>
+      <c r="G25" s="35" t="s">
         <v>1029</v>
-      </c>
-      <c r="G25" s="35" t="s">
-        <v>1030</v>
       </c>
       <c r="H25" s="36" t="s">
         <v>10</v>
@@ -33447,7 +33533,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="84" t="s">
-        <v>1171</v>
+        <v>1168</v>
       </c>
       <c r="F1" s="26" t="s">
         <v>134</v>
@@ -33480,7 +33566,7 @@
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E2" s="27" t="s">
         <v>131</v>
@@ -33516,7 +33602,7 @@
         <v>267</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E3" s="27" t="s">
         <v>851</v>
@@ -33676,10 +33762,10 @@
         <v>748</v>
       </c>
       <c r="F8" s="35" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="G8" s="35" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="H8" s="35" t="s">
         <v>10</v>
@@ -33892,10 +33978,10 @@
         <v>736</v>
       </c>
       <c r="F15" s="35" t="s">
+        <v>1088</v>
+      </c>
+      <c r="G15" s="35" t="s">
         <v>1089</v>
-      </c>
-      <c r="G15" s="35" t="s">
-        <v>1090</v>
       </c>
       <c r="H15" s="36" t="s">
         <v>187</v>
@@ -33922,10 +34008,10 @@
         <v>737</v>
       </c>
       <c r="F16" s="35" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="G16" s="36" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="H16" s="36" t="s">
         <v>187</v>
@@ -34104,10 +34190,10 @@
         <v>828</v>
       </c>
       <c r="F22" s="35" t="s">
+        <v>1092</v>
+      </c>
+      <c r="G22" s="35" t="s">
         <v>1093</v>
-      </c>
-      <c r="G22" s="35" t="s">
-        <v>1094</v>
       </c>
       <c r="H22" s="36" t="s">
         <v>187</v>
@@ -34134,10 +34220,10 @@
         <v>829</v>
       </c>
       <c r="F23" s="35" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="G23" s="36" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="H23" s="36" t="s">
         <v>187</v>
@@ -34162,10 +34248,10 @@
         <v>818</v>
       </c>
       <c r="F24" s="35" t="s">
+        <v>1030</v>
+      </c>
+      <c r="G24" s="35" t="s">
         <v>1031</v>
-      </c>
-      <c r="G24" s="35" t="s">
-        <v>1032</v>
       </c>
       <c r="H24" s="36" t="s">
         <v>10</v>
@@ -34304,7 +34390,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="84" t="s">
-        <v>1171</v>
+        <v>1168</v>
       </c>
       <c r="F1" s="26" t="s">
         <v>134</v>
@@ -34337,7 +34423,7 @@
       </c>
       <c r="C2" s="66"/>
       <c r="D2" s="28" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E2" s="28" t="s">
         <v>851</v>
@@ -34371,7 +34457,7 @@
         <v>267</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E3" s="28" t="s">
         <v>135</v>
@@ -34449,10 +34535,10 @@
         <v>11</v>
       </c>
       <c r="J5" s="82" t="s">
-        <v>1156</v>
+        <v>1153</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
       <c r="L5" s="7" t="s">
         <v>146</v>
@@ -34535,7 +34621,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="84" t="s">
-        <v>1171</v>
+        <v>1168</v>
       </c>
       <c r="F1" s="26" t="s">
         <v>134</v>
@@ -34568,7 +34654,7 @@
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E2" s="27" t="s">
         <v>337</v>
@@ -34604,7 +34690,7 @@
         <v>267</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E3" s="27" t="s">
         <v>851</v>
@@ -34640,7 +34726,7 @@
         <v>267</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E4" s="27" t="s">
         <v>261</v>
@@ -34676,7 +34762,7 @@
         <v>267</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E5" s="27" t="s">
         <v>260</v>
@@ -34780,16 +34866,16 @@
         <v>687</v>
       </c>
       <c r="H8" s="36" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
       <c r="I8" s="36" t="s">
         <v>11</v>
       </c>
       <c r="J8" s="36" t="s">
-        <v>1165</v>
+        <v>1162</v>
       </c>
       <c r="K8" s="36" t="s">
-        <v>1159</v>
+        <v>1156</v>
       </c>
       <c r="L8" s="36" t="s">
         <v>683</v>
@@ -35020,10 +35106,10 @@
         <v>736</v>
       </c>
       <c r="F16" s="35" t="s">
+        <v>1129</v>
+      </c>
+      <c r="G16" s="35" t="s">
         <v>1130</v>
-      </c>
-      <c r="G16" s="35" t="s">
-        <v>1131</v>
       </c>
       <c r="H16" s="36" t="s">
         <v>187</v>
@@ -35050,10 +35136,10 @@
         <v>154</v>
       </c>
       <c r="F17" s="35" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="G17" s="36" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="H17" s="36" t="s">
         <v>187</v>
@@ -35234,10 +35320,10 @@
         <v>828</v>
       </c>
       <c r="F23" s="35" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="G23" s="35" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="H23" s="36" t="s">
         <v>187</v>
@@ -35264,10 +35350,10 @@
         <v>829</v>
       </c>
       <c r="F24" s="35" t="s">
+        <v>1133</v>
+      </c>
+      <c r="G24" s="36" t="s">
         <v>1134</v>
-      </c>
-      <c r="G24" s="36" t="s">
-        <v>1135</v>
       </c>
       <c r="H24" s="36" t="s">
         <v>187</v>
@@ -35345,7 +35431,7 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="83" t="s">
-        <v>1167</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="29" spans="1:12" s="5" customFormat="1" x14ac:dyDescent="0.25">
@@ -35377,7 +35463,7 @@
   </sheetPr>
   <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="K26" sqref="K26:L26"/>
     </sheetView>
   </sheetViews>
@@ -35410,7 +35496,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="84" t="s">
-        <v>1171</v>
+        <v>1168</v>
       </c>
       <c r="F1" s="26" t="s">
         <v>134</v>
@@ -35443,7 +35529,7 @@
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E2" s="86" t="s">
         <v>288</v>
@@ -35475,7 +35561,7 @@
       </c>
       <c r="C3" s="27"/>
       <c r="D3" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E3" s="27" t="s">
         <v>111</v>
@@ -35507,7 +35593,7 @@
       </c>
       <c r="C4" s="27"/>
       <c r="D4" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E4" s="27" t="s">
         <v>343</v>
@@ -35539,7 +35625,7 @@
       </c>
       <c r="C5" s="27"/>
       <c r="D5" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E5" s="27" t="s">
         <v>114</v>
@@ -35573,7 +35659,7 @@
       </c>
       <c r="C6" s="27"/>
       <c r="D6" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E6" s="27" t="s">
         <v>851</v>
@@ -35607,7 +35693,7 @@
       </c>
       <c r="C7" s="27"/>
       <c r="D7" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E7" s="27" t="s">
         <v>128</v>
@@ -35641,7 +35727,7 @@
       </c>
       <c r="C8" s="27"/>
       <c r="D8" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E8" s="27" t="s">
         <v>260</v>
@@ -35707,22 +35793,22 @@
         <v>688</v>
       </c>
       <c r="F10" s="36" t="s">
+        <v>990</v>
+      </c>
+      <c r="G10" s="36" t="s">
         <v>991</v>
       </c>
-      <c r="G10" s="36" t="s">
-        <v>992</v>
-      </c>
       <c r="H10" s="36" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
       <c r="I10" s="36" t="s">
         <v>11</v>
       </c>
       <c r="J10" s="36" t="s">
-        <v>1166</v>
+        <v>1163</v>
       </c>
       <c r="K10" s="36" t="s">
-        <v>1153</v>
+        <v>1150</v>
       </c>
       <c r="L10" s="36"/>
     </row>
@@ -35968,7 +36054,7 @@
         <v>60</v>
       </c>
       <c r="K18" s="36" t="s">
-        <v>1138</v>
+        <v>1137</v>
       </c>
       <c r="L18" s="36" t="s">
         <v>159</v>
@@ -36214,10 +36300,10 @@
       </c>
       <c r="J26" s="36"/>
       <c r="K26" s="49" t="s">
-        <v>1151</v>
+        <v>1148</v>
       </c>
       <c r="L26" s="49" t="s">
-        <v>1151</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="27" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.25">
@@ -36231,10 +36317,10 @@
         <v>736</v>
       </c>
       <c r="F27" s="35" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="G27" s="35" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="H27" s="36" t="s">
         <v>187</v>
@@ -36261,10 +36347,10 @@
         <v>154</v>
       </c>
       <c r="F28" s="35" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="G28" s="36" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="H28" s="36" t="s">
         <v>187</v>
@@ -36443,10 +36529,10 @@
         <v>828</v>
       </c>
       <c r="F34" s="35" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="G34" s="35" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="H34" s="36" t="s">
         <v>187</v>
@@ -36473,10 +36559,10 @@
         <v>829</v>
       </c>
       <c r="F35" s="35" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="G35" s="36" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="H35" s="36" t="s">
         <v>187</v>
@@ -36501,10 +36587,10 @@
         <v>818</v>
       </c>
       <c r="F36" s="35" t="s">
+        <v>992</v>
+      </c>
+      <c r="G36" s="35" t="s">
         <v>993</v>
-      </c>
-      <c r="G36" s="35" t="s">
-        <v>994</v>
       </c>
       <c r="H36" s="36" t="s">
         <v>10</v>
@@ -36568,7 +36654,7 @@
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="83" t="s">
-        <v>1168</v>
+        <v>1165</v>
       </c>
       <c r="B39" s="67"/>
       <c r="C39" s="67"/>
@@ -36628,8 +36714,8 @@
   </sheetPr>
   <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView topLeftCell="D26" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36663,7 +36749,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="84" t="s">
-        <v>1171</v>
+        <v>1168</v>
       </c>
       <c r="F1" s="26" t="s">
         <v>134</v>
@@ -36696,7 +36782,7 @@
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E2" s="30" t="s">
         <v>128</v>
@@ -36730,7 +36816,7 @@
         <v>267</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E3" s="30" t="s">
         <v>288</v>
@@ -36762,7 +36848,7 @@
       </c>
       <c r="C4" s="27"/>
       <c r="D4" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E4" s="30" t="s">
         <v>851</v>
@@ -37127,10 +37213,10 @@
       </c>
       <c r="J15" s="35"/>
       <c r="K15" s="36" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="L15" s="36" t="s">
-        <v>1150</v>
+        <v>1147</v>
       </c>
       <c r="M15" s="70"/>
     </row>
@@ -37247,7 +37333,7 @@
       </c>
       <c r="J19" s="35"/>
       <c r="K19" s="36" t="s">
-        <v>1160</v>
+        <v>1157</v>
       </c>
       <c r="L19" s="36" t="s">
         <v>92</v>
@@ -37278,7 +37364,7 @@
       </c>
       <c r="J20" s="35"/>
       <c r="K20" s="36" t="s">
-        <v>1161</v>
+        <v>1158</v>
       </c>
       <c r="L20" s="36" t="s">
         <v>93</v>
@@ -37309,7 +37395,7 @@
       </c>
       <c r="J21" s="35"/>
       <c r="K21" s="36" t="s">
-        <v>1162</v>
+        <v>1159</v>
       </c>
       <c r="L21" s="36" t="s">
         <v>94</v>
@@ -37340,7 +37426,7 @@
       </c>
       <c r="J22" s="35"/>
       <c r="K22" s="36" t="s">
-        <v>1163</v>
+        <v>1160</v>
       </c>
       <c r="L22" s="36" t="s">
         <v>95</v>
@@ -37371,7 +37457,7 @@
       </c>
       <c r="J23" s="35"/>
       <c r="K23" s="36" t="s">
-        <v>1164</v>
+        <v>1161</v>
       </c>
       <c r="L23" s="36" t="s">
         <v>96</v>
@@ -37389,10 +37475,10 @@
         <v>969</v>
       </c>
       <c r="F24" s="35" t="s">
+        <v>998</v>
+      </c>
+      <c r="G24" s="35" t="s">
         <v>999</v>
-      </c>
-      <c r="G24" s="35" t="s">
-        <v>1000</v>
       </c>
       <c r="H24" s="35" t="s">
         <v>10</v>
@@ -37404,7 +37490,7 @@
         <v>14</v>
       </c>
       <c r="K24" s="36" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="L24" s="36" t="s">
         <v>971</v>
@@ -37437,7 +37523,7 @@
         <v>14</v>
       </c>
       <c r="K25" s="36" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="L25" s="36" t="s">
         <v>228</v>
@@ -37470,7 +37556,7 @@
         <v>14</v>
       </c>
       <c r="K26" s="36" t="s">
-        <v>1175</v>
+        <v>1172</v>
       </c>
       <c r="L26" s="36" t="s">
         <v>178</v>
@@ -37485,16 +37571,16 @@
         <v>23</v>
       </c>
       <c r="E27" s="35" t="s">
+        <v>987</v>
+      </c>
+      <c r="F27" s="35" t="s">
+        <v>1047</v>
+      </c>
+      <c r="G27" s="35" t="s">
+        <v>1047</v>
+      </c>
+      <c r="H27" s="35" t="s">
         <v>988</v>
-      </c>
-      <c r="F27" s="35" t="s">
-        <v>1048</v>
-      </c>
-      <c r="G27" s="35" t="s">
-        <v>1048</v>
-      </c>
-      <c r="H27" s="35" t="s">
-        <v>989</v>
       </c>
       <c r="I27" s="35" t="s">
         <v>11</v>
@@ -37503,10 +37589,10 @@
         <v>14</v>
       </c>
       <c r="K27" s="36" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="L27" s="36" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="M27" s="70"/>
     </row>
@@ -37536,7 +37622,7 @@
         <v>14</v>
       </c>
       <c r="K28" s="35" t="s">
-        <v>980</v>
+        <v>1175</v>
       </c>
       <c r="L28" s="35" t="s">
         <v>980</v>
@@ -37761,10 +37847,10 @@
       </c>
       <c r="J35" s="35"/>
       <c r="K35" s="36" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="L35" s="36" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="M35" s="70"/>
     </row>
@@ -37873,13 +37959,13 @@
         <v>35</v>
       </c>
       <c r="E39" s="35" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="F39" s="35" t="s">
         <v>738</v>
       </c>
       <c r="G39" s="35" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="H39" s="35" t="s">
         <v>10</v>
@@ -37891,7 +37977,7 @@
         <v>14</v>
       </c>
       <c r="K39" s="36" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="L39" s="36"/>
       <c r="M39" s="70"/>
@@ -37920,7 +38006,7 @@
       </c>
       <c r="J40" s="35"/>
       <c r="K40" s="36" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="L40" s="36"/>
       <c r="M40" s="70"/>
@@ -38013,10 +38099,10 @@
       </c>
       <c r="J43" s="35"/>
       <c r="K43" s="36" t="s">
-        <v>1172</v>
+        <v>1169</v>
       </c>
       <c r="L43" s="36" t="s">
-        <v>1152</v>
+        <v>1149</v>
       </c>
       <c r="M43" s="70"/>
     </row>
@@ -38031,10 +38117,10 @@
         <v>736</v>
       </c>
       <c r="F44" s="35" t="s">
+        <v>1048</v>
+      </c>
+      <c r="G44" s="35" t="s">
         <v>1049</v>
-      </c>
-      <c r="G44" s="35" t="s">
-        <v>1050</v>
       </c>
       <c r="H44" s="36" t="s">
         <v>187</v>
@@ -38062,10 +38148,10 @@
         <v>154</v>
       </c>
       <c r="F45" s="35" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="G45" s="36" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="H45" s="36" t="s">
         <v>187</v>
@@ -38250,10 +38336,10 @@
         <v>828</v>
       </c>
       <c r="F51" s="35" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="G51" s="35" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="H51" s="36" t="s">
         <v>187</v>
@@ -38281,10 +38367,10 @@
         <v>829</v>
       </c>
       <c r="F52" s="35" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="G52" s="36" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="H52" s="36" t="s">
         <v>187</v>
@@ -38310,10 +38396,10 @@
         <v>818</v>
       </c>
       <c r="F53" s="35" t="s">
+        <v>994</v>
+      </c>
+      <c r="G53" s="35" t="s">
         <v>995</v>
-      </c>
-      <c r="G53" s="35" t="s">
-        <v>996</v>
       </c>
       <c r="H53" s="36" t="s">
         <v>10</v>
@@ -38502,7 +38588,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="84" t="s">
-        <v>1171</v>
+        <v>1168</v>
       </c>
       <c r="F1" s="26" t="s">
         <v>134</v>
@@ -38535,7 +38621,7 @@
       </c>
       <c r="C2" s="30"/>
       <c r="D2" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E2" s="30" t="s">
         <v>274</v>
@@ -38569,7 +38655,7 @@
         <v>770</v>
       </c>
       <c r="D3" s="27" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="E3" s="30" t="s">
         <v>851</v>
@@ -38682,7 +38768,7 @@
         <v>14</v>
       </c>
       <c r="K6" s="36" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="L6" s="36" t="s">
         <v>506</v>
@@ -39076,10 +39162,10 @@
         <v>736</v>
       </c>
       <c r="F19" s="35" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="G19" s="35" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="H19" s="36" t="s">
         <v>187</v>
@@ -39106,10 +39192,10 @@
         <v>154</v>
       </c>
       <c r="F20" s="35" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="G20" s="36" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="H20" s="36" t="s">
         <v>187</v>
@@ -39320,10 +39406,10 @@
         <v>828</v>
       </c>
       <c r="F27" s="35" t="s">
+        <v>1097</v>
+      </c>
+      <c r="G27" s="35" t="s">
         <v>1098</v>
-      </c>
-      <c r="G27" s="35" t="s">
-        <v>1099</v>
       </c>
       <c r="H27" s="36" t="s">
         <v>187</v>
@@ -39350,10 +39436,10 @@
         <v>829</v>
       </c>
       <c r="F28" s="35" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="G28" s="36" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="H28" s="36" t="s">
         <v>187</v>
@@ -39378,10 +39464,10 @@
         <v>818</v>
       </c>
       <c r="F29" s="35" t="s">
+        <v>1032</v>
+      </c>
+      <c r="G29" s="35" t="s">
         <v>1033</v>
-      </c>
-      <c r="G29" s="35" t="s">
-        <v>1034</v>
       </c>
       <c r="H29" s="36" t="s">
         <v>10</v>
@@ -39440,27 +39526,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
-    <TaxCatchAllLabel xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
-    <TaxKeywordTaxHTField xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100584B29A9F606E64BBE0B94B46ABEDBD5" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ad12f995843361ff338b3798f1f5f41c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4d5313c0-c1e6-4122-afa9-da1ccdba405d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8fda66a02b6b5d1f39f2000ab0f58af4" ns2:_="">
     <xsd:import namespace="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
@@ -39632,31 +39697,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60949D59-0B5B-44ED-ACEF-9231A5F5D889}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04CD8B6C-25F0-471A-A724-387AC1B5060F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
+    <TaxCatchAllLabel xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
+    <TaxKeywordTaxHTField xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F67F35D-1CDD-4110-B6CE-1A6865489AEE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -39672,4 +39734,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04CD8B6C-25F0-471A-A724-387AC1B5060F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60949D59-0B5B-44ED-ACEF-9231A5F5D889}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated SA uk1 and uk2
</commit_message>
<xml_diff>
--- a/Documents/RDBES Data Model.xlsx
+++ b/Documents/RDBES Data Model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="23115" windowHeight="13515" tabRatio="747" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="23115" windowHeight="13515" tabRatio="747" firstSheet="6" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Model v1.18.3" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3180" uniqueCount="1229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3180" uniqueCount="1231">
   <si>
     <t>Design Table (DE)</t>
   </si>
@@ -4184,6 +4184,53 @@
   </si>
   <si>
     <t>RS_MethodForMeasurement</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Uk1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Uk2</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Uk1</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, Uk2</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -12507,8 +12554,8 @@
   </sheetPr>
   <dimension ref="A1:W60"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12610,7 +12657,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>766</v>
+        <v>1230</v>
       </c>
       <c r="D3" s="27" t="s">
         <v>997</v>
@@ -12682,7 +12729,7 @@
       <c r="A5" s="36"/>
       <c r="B5" s="57"/>
       <c r="C5" s="36" t="s">
-        <v>264</v>
+        <v>1229</v>
       </c>
       <c r="D5" s="53">
         <v>2</v>
@@ -16010,7 +16057,7 @@
   </sheetPr>
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
@@ -24204,12 +24251,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
+    <TaxCatchAllLabel xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
+    <TaxKeywordTaxHTField xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -24385,21 +24435,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
-    <TaxCatchAllLabel xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
-    <TaxKeywordTaxHTField xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04CD8B6C-25F0-471A-A724-387AC1B5060F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60949D59-0B5B-44ED-ACEF-9231A5F5D889}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -24423,17 +24478,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60949D59-0B5B-44ED-ACEF-9231A5F5D889}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04CD8B6C-25F0-471A-A724-387AC1B5060F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
UK2 is inserted again
UK2 is inserted again because it is fundamental for ensuring subsamples are correctly refering to only one sample record.
</commit_message>
<xml_diff>
--- a/Documents/RDBES Data Model.xlsx
+++ b/Documents/RDBES Data Model.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\git\RDBES\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profile\Henrik K\Documents\GitHub\RDBESpublic\RDBES\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="23115" windowHeight="13515" tabRatio="747" firstSheet="6" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="23115" windowHeight="13515" tabRatio="747" firstSheet="5" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Model v1.18.3" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3180" uniqueCount="1231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3180" uniqueCount="1230">
   <si>
     <t>Design Table (DE)</t>
   </si>
@@ -4203,33 +4203,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Uk2</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Uk1</t>
-    </r>
-    <r>
-      <rPr>
-        <strike/>
-        <sz val="9"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, Uk2</t>
+      <t xml:space="preserve"> Uk2</t>
     </r>
   </si>
 </sst>
@@ -12555,7 +12529,7 @@
   <dimension ref="A1:W60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12657,7 +12631,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>1230</v>
+        <v>766</v>
       </c>
       <c r="D3" s="27" t="s">
         <v>997</v>
@@ -24251,18 +24225,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
-    <TaxCatchAllLabel xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
-    <TaxKeywordTaxHTField xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100584B29A9F606E64BBE0B94B46ABEDBD5" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ad12f995843361ff338b3798f1f5f41c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4d5313c0-c1e6-4122-afa9-da1ccdba405d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8fda66a02b6b5d1f39f2000ab0f58af4" ns2:_="">
     <xsd:import namespace="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
@@ -24434,6 +24396,18 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
+    <TaxCatchAllLabel xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
+    <TaxKeywordTaxHTField xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -24444,22 +24418,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60949D59-0B5B-44ED-ACEF-9231A5F5D889}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F67F35D-1CDD-4110-B6CE-1A6865489AEE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -24477,6 +24435,22 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60949D59-0B5B-44ED-ACEF-9231A5F5D889}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04CD8B6C-25F0-471A-A724-387AC1B5060F}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Minor correction ver 1.19.1 Field: OSlocationType is removed from pos. 21
In table 'Onshore Event' the field: Sampling location type, OSlocationType, was previously moved from position 21 to 6, but the field was not deleted in pos. 21. Now it as been deleted and appear only in position 6.
</commit_message>
<xml_diff>
--- a/Documents/RDBES Data Model.xlsx
+++ b/Documents/RDBES Data Model.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20374"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20375"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profile\Henrik K\Documents\GitHub\RDBES_Core_Group\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5191D9EC-E00B-49EA-B433-617D071147F6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09473E9C-8DF1-4635-90F5-9796328A6ECB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="17430" windowHeight="5595" tabRatio="781" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="17430" windowHeight="5595" tabRatio="781" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Model v1.19" sheetId="1" r:id="rId1"/>
+    <sheet name="Model v1.19.1" sheetId="1" r:id="rId1"/>
     <sheet name="Design" sheetId="5" r:id="rId2"/>
     <sheet name="Temporal Event" sheetId="21" r:id="rId3"/>
     <sheet name="Location" sheetId="20" r:id="rId4"/>
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3462" uniqueCount="1304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3403" uniqueCount="1304">
   <si>
     <t>Design Table (DE)</t>
   </si>
@@ -4398,7 +4398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -4595,6 +4595,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4949,7 +4950,9 @@
   </sheetPr>
   <dimension ref="A1:AI112"/>
   <sheetViews>
-    <sheetView showZeros="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0"/>
+    <sheetView showZeros="0" topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
@@ -7205,7 +7208,7 @@
         <v>Conversion factor between measured weight and live weight.</v>
       </c>
     </row>
-    <row r="32" spans="9:35" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="32" spans="9:35" x14ac:dyDescent="0.5">
       <c r="I32" s="17">
         <f>IF(ISBLANK(Location!A4)=TRUE, Location!B4, "")</f>
         <v>0</v>
@@ -7651,7 +7654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="8:27" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="41" spans="8:27" x14ac:dyDescent="0.5">
       <c r="H41" s="48"/>
       <c r="I41" s="48">
         <f>IF(ISBLANK(Location!A27)=TRUE, Location!B27, "")</f>
@@ -7696,7 +7699,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="8:27" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="42" spans="8:27" x14ac:dyDescent="0.5">
       <c r="H42" s="48"/>
       <c r="I42" s="48"/>
       <c r="J42" s="42" t="str">
@@ -8103,8 +8106,8 @@
         <v>OSselectionMethod</v>
       </c>
       <c r="O54" s="36" t="str">
-        <f>IF(ISBLANK('Onshore Event'!A24)=TRUE, 'Onshore Event'!M24, "")</f>
-        <v>Type of location</v>
+        <f>IF(ISBLANK('Onshore Event'!#REF!)=TRUE, 'Onshore Event'!#REF!, "")</f>
+        <v/>
       </c>
       <c r="P54" s="18"/>
       <c r="R54" s="20">
@@ -8128,8 +8131,8 @@
       <c r="L55" s="17"/>
       <c r="M55" s="18"/>
       <c r="N55" s="20" t="str">
-        <f>IF(ISBLANK('Onshore Event'!A24)=TRUE, 'Onshore Event'!F24, "")</f>
-        <v>OSlocationType</v>
+        <f>IF(ISBLANK('Onshore Event'!#REF!)=TRUE, 'Onshore Event'!#REF!, "")</f>
+        <v/>
       </c>
       <c r="O55" s="36" t="str">
         <f>IF(ISBLANK('Onshore Event'!#REF!)=TRUE, 'Onshore Event'!#REF!, "")</f>
@@ -8161,11 +8164,11 @@
       <c r="L56" s="17"/>
       <c r="M56" s="18"/>
       <c r="N56" s="20" t="str">
-        <f>IF(ISBLANK('Onshore Event'!A25)=TRUE, 'Onshore Event'!F25, "")</f>
+        <f>IF(ISBLANK('Onshore Event'!A24)=TRUE, 'Onshore Event'!F24, "")</f>
         <v>OSselectionMethodCluster</v>
       </c>
       <c r="O56" s="36" t="str">
-        <f>IF(ISBLANK('Onshore Event'!A25)=TRUE, 'Onshore Event'!M25, "")</f>
+        <f>IF(ISBLANK('Onshore Event'!A24)=TRUE, 'Onshore Event'!M24, "")</f>
         <v>The method of selecting clusters</v>
       </c>
       <c r="P56" s="18"/>
@@ -8198,11 +8201,11 @@
       <c r="L57" s="17"/>
       <c r="M57" s="18"/>
       <c r="N57" s="20" t="str">
-        <f>IF(ISBLANK('Onshore Event'!A26)=TRUE, 'Onshore Event'!F26, "")</f>
+        <f>IF(ISBLANK('Onshore Event'!A25)=TRUE, 'Onshore Event'!F25, "")</f>
         <v>OSnumberTotalClusters</v>
       </c>
       <c r="O57" s="36" t="str">
-        <f>IF(ISBLANK('Onshore Event'!A26)=TRUE, 'Onshore Event'!M26, "")</f>
+        <f>IF(ISBLANK('Onshore Event'!A25)=TRUE, 'Onshore Event'!M25, "")</f>
         <v>Total number of clusters in that level of the sampling hierarchy</v>
       </c>
       <c r="P57" s="18"/>
@@ -8235,11 +8238,11 @@
       <c r="L58" s="17"/>
       <c r="M58" s="18"/>
       <c r="N58" s="20" t="str">
-        <f>IF(ISBLANK('Onshore Event'!A27)=TRUE, 'Onshore Event'!F27, "")</f>
+        <f>IF(ISBLANK('Onshore Event'!A26)=TRUE, 'Onshore Event'!F26, "")</f>
         <v>OSnumberSampledClusters</v>
       </c>
       <c r="O58" s="36" t="str">
-        <f>IF(ISBLANK('Onshore Event'!A27)=TRUE, 'Onshore Event'!M27, "")</f>
+        <f>IF(ISBLANK('Onshore Event'!A26)=TRUE, 'Onshore Event'!M26, "")</f>
         <v>Total number of clusters sampled</v>
       </c>
       <c r="P58" s="18"/>
@@ -8301,11 +8304,11 @@
       <c r="L60" s="17"/>
       <c r="M60" s="18"/>
       <c r="N60" s="20" t="str">
-        <f>IF(ISBLANK('Onshore Event'!A31)=TRUE, 'Onshore Event'!F31, "")</f>
+        <f>IF(ISBLANK('Onshore Event'!A30)=TRUE, 'Onshore Event'!F30, "")</f>
         <v>OSreasonNotSampled</v>
       </c>
       <c r="O60" s="36" t="str">
-        <f>IF(ISBLANK('Onshore Event'!A31)=TRUE, 'Onshore Event'!M31, "")</f>
+        <f>IF(ISBLANK('Onshore Event'!A30)=TRUE, 'Onshore Event'!M30, "")</f>
         <v>Reason for not sampling</v>
       </c>
       <c r="P60" s="18"/>
@@ -8333,11 +8336,11 @@
       <c r="L61" s="17"/>
       <c r="M61" s="18"/>
       <c r="N61" s="20">
-        <f>IF(ISBLANK('Onshore Event'!A32)=TRUE, 'Onshore Event'!F32, "")</f>
+        <f>IF(ISBLANK('Onshore Event'!A31)=TRUE, 'Onshore Event'!F31, "")</f>
         <v>0</v>
       </c>
       <c r="O61" s="20">
-        <f>IF(ISBLANK('Onshore Event'!A32)=TRUE, 'Onshore Event'!M32, "")</f>
+        <f>IF(ISBLANK('Onshore Event'!A31)=TRUE, 'Onshore Event'!M31, "")</f>
         <v>0</v>
       </c>
       <c r="P61" s="18"/>
@@ -8423,7 +8426,7 @@
       <c r="Y64" s="19"/>
       <c r="Z64" s="19"/>
     </row>
-    <row r="65" spans="10:26" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="65" spans="10:26" x14ac:dyDescent="0.5">
       <c r="J65" s="43" t="str">
         <f>IF(ISBLANK(Location!A18)=TRUE, Location!F18, "")</f>
         <v>LOselectionMethod</v>
@@ -29099,7 +29102,7 @@
       <c r="U6" s="51"/>
       <c r="V6" s="51"/>
     </row>
-    <row r="7" spans="1:22" s="41" customFormat="1" ht="35.65" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:22" s="41" customFormat="1" ht="24" x14ac:dyDescent="0.45">
       <c r="A7" s="12"/>
       <c r="B7" s="11"/>
       <c r="C7" s="11"/>
@@ -30796,7 +30799,7 @@
       <c r="U46" s="51"/>
       <c r="V46" s="51"/>
     </row>
-    <row r="47" spans="1:22" ht="35.65" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:22" ht="24" x14ac:dyDescent="0.45">
       <c r="A47" s="12"/>
       <c r="B47" s="11"/>
       <c r="C47" s="11"/>
@@ -31688,7 +31691,7 @@
       </c>
       <c r="M14" s="35"/>
     </row>
-    <row r="15" spans="1:22" ht="35.65" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:22" ht="24" x14ac:dyDescent="0.45">
       <c r="A15" s="52"/>
       <c r="B15" s="52"/>
       <c r="C15" s="52"/>
@@ -32029,7 +32032,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="51" customFormat="1" ht="58.9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" s="51" customFormat="1" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A7" s="35"/>
       <c r="B7" s="56" t="s">
         <v>1097</v>
@@ -32744,7 +32747,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -39309,7 +39312,7 @@
       </c>
       <c r="N36" s="90"/>
     </row>
-    <row r="37" spans="1:14" ht="24" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A37" s="4"/>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
@@ -40184,9 +40187,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:O34"/>
+  <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -40482,9 +40487,7 @@
     </row>
     <row r="9" spans="1:15" s="88" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A9" s="12"/>
-      <c r="B9" s="34" t="s">
-        <v>1256</v>
-      </c>
+      <c r="B9" s="34"/>
       <c r="C9" s="34"/>
       <c r="D9" s="34">
         <v>6</v>
@@ -40510,8 +40513,12 @@
       <c r="K9" s="102" t="s">
         <v>1041</v>
       </c>
-      <c r="L9" s="59"/>
-      <c r="M9" s="59"/>
+      <c r="L9" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="M9" s="35" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A10" s="15"/>
@@ -40971,87 +40978,83 @@
       <c r="A24" s="15"/>
       <c r="B24" s="34"/>
       <c r="C24" s="34"/>
-      <c r="D24" s="34">
+      <c r="D24" s="106">
         <v>21</v>
       </c>
       <c r="E24" s="34" t="s">
-        <v>62</v>
+        <v>1170</v>
       </c>
       <c r="F24" s="34" t="s">
-        <v>432</v>
+        <v>336</v>
       </c>
       <c r="G24" s="34" t="s">
-        <v>433</v>
+        <v>338</v>
       </c>
       <c r="H24" s="34" t="s">
         <v>10</v>
       </c>
       <c r="I24" s="34" t="s">
-        <v>17</v>
-      </c>
-      <c r="J24" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="J24" s="35" t="s">
         <v>14</v>
       </c>
       <c r="K24" s="34" t="s">
-        <v>1041</v>
+        <v>1020</v>
       </c>
       <c r="L24" s="35" t="s">
-        <v>151</v>
+        <v>524</v>
       </c>
       <c r="M24" s="35" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.45">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" s="2" customFormat="1" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A25" s="15"/>
       <c r="B25" s="34"/>
       <c r="C25" s="34"/>
-      <c r="D25" s="34">
+      <c r="D25" s="106">
         <v>22</v>
       </c>
       <c r="E25" s="34" t="s">
-        <v>1170</v>
+        <v>1171</v>
       </c>
       <c r="F25" s="34" t="s">
-        <v>336</v>
+        <v>822</v>
       </c>
       <c r="G25" s="34" t="s">
-        <v>338</v>
+        <v>804</v>
       </c>
       <c r="H25" s="34" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="I25" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="J25" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="K25" s="34" t="s">
-        <v>1020</v>
-      </c>
+      <c r="J25" s="34"/>
+      <c r="K25" s="34"/>
       <c r="L25" s="35" t="s">
-        <v>524</v>
+        <v>266</v>
       </c>
       <c r="M25" s="35" t="s">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" s="2" customFormat="1" ht="35.65" x14ac:dyDescent="0.45">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" s="2" customFormat="1" ht="24" x14ac:dyDescent="0.45">
       <c r="A26" s="15"/>
       <c r="B26" s="34"/>
       <c r="C26" s="34"/>
-      <c r="D26" s="34">
+      <c r="D26" s="106">
         <v>23</v>
       </c>
       <c r="E26" s="34" t="s">
-        <v>1171</v>
+        <v>1172</v>
       </c>
       <c r="F26" s="34" t="s">
-        <v>822</v>
+        <v>776</v>
       </c>
       <c r="G26" s="34" t="s">
-        <v>804</v>
+        <v>788</v>
       </c>
       <c r="H26" s="34" t="s">
         <v>13</v>
@@ -41062,30 +41065,30 @@
       <c r="J26" s="34"/>
       <c r="K26" s="34"/>
       <c r="L26" s="35" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="M26" s="35" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
     </row>
     <row r="27" spans="1:13" s="2" customFormat="1" ht="24" x14ac:dyDescent="0.45">
-      <c r="A27" s="15"/>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34">
+      <c r="A27" s="12"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="106">
         <v>24</v>
       </c>
       <c r="E27" s="34" t="s">
-        <v>1172</v>
+        <v>698</v>
       </c>
       <c r="F27" s="34" t="s">
-        <v>776</v>
+        <v>954</v>
       </c>
       <c r="G27" s="34" t="s">
-        <v>788</v>
-      </c>
-      <c r="H27" s="34" t="s">
-        <v>13</v>
+        <v>955</v>
+      </c>
+      <c r="H27" s="35" t="s">
+        <v>148</v>
       </c>
       <c r="I27" s="34" t="s">
         <v>87</v>
@@ -41093,27 +41096,27 @@
       <c r="J27" s="34"/>
       <c r="K27" s="34"/>
       <c r="L27" s="35" t="s">
-        <v>268</v>
+        <v>831</v>
       </c>
       <c r="M27" s="35" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" s="2" customFormat="1" ht="24" x14ac:dyDescent="0.45">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" s="23" customFormat="1" ht="24" x14ac:dyDescent="0.45">
       <c r="A28" s="12"/>
       <c r="B28" s="35"/>
       <c r="C28" s="35"/>
-      <c r="D28" s="34">
+      <c r="D28" s="106">
         <v>25</v>
       </c>
       <c r="E28" s="34" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="F28" s="34" t="s">
-        <v>954</v>
-      </c>
-      <c r="G28" s="34" t="s">
-        <v>955</v>
+        <v>953</v>
+      </c>
+      <c r="G28" s="35" t="s">
+        <v>956</v>
       </c>
       <c r="H28" s="35" t="s">
         <v>148</v>
@@ -41124,111 +41127,80 @@
       <c r="J28" s="34"/>
       <c r="K28" s="34"/>
       <c r="L28" s="35" t="s">
-        <v>831</v>
-      </c>
-      <c r="M28" s="35" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" s="23" customFormat="1" ht="24" x14ac:dyDescent="0.45">
+        <v>832</v>
+      </c>
+      <c r="M28" s="35"/>
+    </row>
+    <row r="29" spans="1:13" s="2" customFormat="1" ht="24" x14ac:dyDescent="0.45">
       <c r="A29" s="12"/>
       <c r="B29" s="35"/>
       <c r="C29" s="35"/>
-      <c r="D29" s="34">
+      <c r="D29" s="106">
         <v>26</v>
       </c>
       <c r="E29" s="34" t="s">
-        <v>699</v>
+        <v>689</v>
       </c>
       <c r="F29" s="34" t="s">
-        <v>953</v>
-      </c>
-      <c r="G29" s="35" t="s">
-        <v>956</v>
+        <v>891</v>
+      </c>
+      <c r="G29" s="34" t="s">
+        <v>892</v>
       </c>
       <c r="H29" s="35" t="s">
-        <v>148</v>
+        <v>10</v>
       </c>
       <c r="I29" s="34" t="s">
-        <v>87</v>
-      </c>
-      <c r="J29" s="34"/>
-      <c r="K29" s="34"/>
+        <v>96</v>
+      </c>
+      <c r="J29" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="K29" s="34" t="s">
+        <v>1015</v>
+      </c>
       <c r="L29" s="35" t="s">
-        <v>832</v>
-      </c>
-      <c r="M29" s="35"/>
-    </row>
-    <row r="30" spans="1:13" s="2" customFormat="1" ht="24" x14ac:dyDescent="0.45">
-      <c r="A30" s="12"/>
-      <c r="B30" s="35"/>
-      <c r="C30" s="35"/>
-      <c r="D30" s="34">
+        <v>1042</v>
+      </c>
+      <c r="M29" s="34"/>
+    </row>
+    <row r="30" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="15"/>
+      <c r="B30" s="34"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="106">
         <v>27</v>
       </c>
-      <c r="E30" s="34" t="s">
-        <v>689</v>
-      </c>
-      <c r="F30" s="34" t="s">
-        <v>891</v>
-      </c>
-      <c r="G30" s="34" t="s">
-        <v>892</v>
+      <c r="E30" s="35" t="s">
+        <v>255</v>
+      </c>
+      <c r="F30" s="35" t="s">
+        <v>337</v>
+      </c>
+      <c r="G30" s="35" t="s">
+        <v>339</v>
       </c>
       <c r="H30" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="I30" s="34" t="s">
-        <v>96</v>
-      </c>
-      <c r="J30" s="34" t="s">
+      <c r="I30" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="J30" s="35" t="s">
         <v>14</v>
       </c>
       <c r="K30" s="34" t="s">
-        <v>1015</v>
+        <v>1021</v>
       </c>
       <c r="L30" s="35" t="s">
-        <v>1042</v>
-      </c>
-      <c r="M30" s="34"/>
-    </row>
-    <row r="31" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="15"/>
-      <c r="B31" s="34"/>
-      <c r="C31" s="34"/>
-      <c r="D31" s="34">
-        <v>28</v>
-      </c>
-      <c r="E31" s="35" t="s">
         <v>255</v>
       </c>
-      <c r="F31" s="35" t="s">
-        <v>337</v>
-      </c>
-      <c r="G31" s="35" t="s">
-        <v>339</v>
-      </c>
-      <c r="H31" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="I31" s="35" t="s">
-        <v>87</v>
-      </c>
-      <c r="J31" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="K31" s="34" t="s">
-        <v>1021</v>
-      </c>
-      <c r="L31" s="35" t="s">
+      <c r="M30" s="35" t="s">
         <v>255</v>
       </c>
-      <c r="M31" s="35" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.45">
-      <c r="D34" s="28" t="s">
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.45">
+      <c r="D33" s="28" t="s">
         <v>239</v>
       </c>
     </row>
@@ -41238,6 +41210,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
+    <TaxCatchAllLabel xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
+    <TaxKeywordTaxHTField xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100584B29A9F606E64BBE0B94B46ABEDBD5" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ad12f995843361ff338b3798f1f5f41c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4d5313c0-c1e6-4122-afa9-da1ccdba405d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8fda66a02b6b5d1f39f2000ab0f58af4" ns2:_="">
     <xsd:import namespace="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
@@ -41409,28 +41402,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60949D59-0B5B-44ED-ACEF-9231A5F5D889}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
-    <TaxCatchAllLabel xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
-    <TaxKeywordTaxHTField xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04CD8B6C-25F0-471A-A724-387AC1B5060F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F67F35D-1CDD-4110-B6CE-1A6865489AEE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -41446,28 +41442,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04CD8B6C-25F0-471A-A724-387AC1B5060F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60949D59-0B5B-44ED-ACEF-9231A5F5D889}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
SelectionMethod is replacing RS_SelectionMethod. V19.1.2
SelectionMethod is replacing RS_SelectionMethod.
</commit_message>
<xml_diff>
--- a/Documents/RDBES Data Model.xlsx
+++ b/Documents/RDBES Data Model.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profile\Henrik K\Documents\GitHub\RDBES_Core_Group\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09473E9C-8DF1-4635-90F5-9796328A6ECB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F1B5C4-C717-4170-8BE8-3CA106829E24}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="17430" windowHeight="5595" tabRatio="781" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="17430" windowHeight="5595" tabRatio="781" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Model v1.19.1" sheetId="1" r:id="rId1"/>
+    <sheet name="Model v1.19.2" sheetId="1" r:id="rId1"/>
     <sheet name="Design" sheetId="5" r:id="rId2"/>
     <sheet name="Temporal Event" sheetId="21" r:id="rId3"/>
     <sheet name="Location" sheetId="20" r:id="rId4"/>
@@ -3276,9 +3276,6 @@
     <t>RS_Sampler</t>
   </si>
   <si>
-    <t>RS_SelectionMethod</t>
-  </si>
-  <si>
     <t>RS_ReasonForNotSampling</t>
   </si>
   <si>
@@ -4148,6 +4145,9 @@
   </si>
   <si>
     <t xml:space="preserve">This overview will not be maintained with the new fields, but it is kept for its overview value </t>
+  </si>
+  <si>
+    <t>SelectionMethod</t>
   </si>
 </sst>
 </file>
@@ -4950,7 +4950,7 @@
   </sheetPr>
   <dimension ref="A1:AI112"/>
   <sheetViews>
-    <sheetView showZeros="0" topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView showZeros="0" tabSelected="1" topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
@@ -5002,7 +5002,7 @@
     </row>
     <row r="2" spans="1:35" ht="21" x14ac:dyDescent="0.65">
       <c r="B2" s="105" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="D2" s="19"/>
       <c r="L2" s="17"/>
@@ -9527,7 +9527,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>929</v>
@@ -9542,11 +9542,11 @@
         <v>11</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="K11" s="12"/>
       <c r="L11" s="12" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="M11" s="12" t="s">
         <v>577</v>
@@ -9582,10 +9582,10 @@
         <v>1015</v>
       </c>
       <c r="L12" s="35" t="s">
+        <v>1094</v>
+      </c>
+      <c r="M12" s="35" t="s">
         <v>1095</v>
-      </c>
-      <c r="M12" s="35" t="s">
-        <v>1096</v>
       </c>
       <c r="N12" s="51"/>
     </row>
@@ -9648,10 +9648,10 @@
       <c r="J14" s="35"/>
       <c r="K14" s="34"/>
       <c r="L14" s="35" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="M14" s="35" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="N14" s="101"/>
     </row>
@@ -9663,7 +9663,7 @@
         <v>6</v>
       </c>
       <c r="E15" s="35" t="s">
-        <v>1199</v>
+        <v>1198</v>
       </c>
       <c r="F15" s="35" t="s">
         <v>757</v>
@@ -9680,10 +9680,10 @@
       <c r="J15" s="35"/>
       <c r="K15" s="34"/>
       <c r="L15" s="35" t="s">
+        <v>1285</v>
+      </c>
+      <c r="M15" s="35" t="s">
         <v>1286</v>
-      </c>
-      <c r="M15" s="35" t="s">
-        <v>1287</v>
       </c>
       <c r="N15" s="51"/>
     </row>
@@ -9731,7 +9731,7 @@
         <v>8</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="F17" s="34" t="s">
         <v>362</v>
@@ -9853,7 +9853,7 @@
         <v>14</v>
       </c>
       <c r="K20" s="34" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="L20" s="35" t="s">
         <v>240</v>
@@ -9871,13 +9871,13 @@
         <v>12</v>
       </c>
       <c r="E21" s="35" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="F21" s="35" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="G21" s="35" t="s">
-        <v>1232</v>
+        <v>1231</v>
       </c>
       <c r="H21" s="35" t="s">
         <v>10</v>
@@ -9887,7 +9887,7 @@
       </c>
       <c r="J21" s="35"/>
       <c r="K21" s="34" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="L21" s="35" t="s">
         <v>92</v>
@@ -9901,19 +9901,19 @@
       <c r="A22" s="12"/>
       <c r="B22" s="12"/>
       <c r="C22" s="35" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="D22" s="35">
         <v>13</v>
       </c>
       <c r="E22" s="35" t="s">
+        <v>1232</v>
+      </c>
+      <c r="F22" s="35" t="s">
         <v>1233</v>
       </c>
-      <c r="F22" s="35" t="s">
-        <v>1234</v>
-      </c>
       <c r="G22" s="35" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="H22" s="35" t="s">
         <v>10</v>
@@ -9953,7 +9953,7 @@
         <v>14</v>
       </c>
       <c r="K23" s="34" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="L23" s="35" t="s">
         <v>78</v>
@@ -9992,7 +9992,7 @@
         <v>1003</v>
       </c>
       <c r="L24" s="35" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="M24" s="35" t="s">
         <v>158</v>
@@ -10071,7 +10071,7 @@
         <v>18</v>
       </c>
       <c r="E27" s="35" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="F27" s="34" t="s">
         <v>932</v>
@@ -10089,7 +10089,7 @@
         <v>14</v>
       </c>
       <c r="K27" s="34" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="L27" s="35" t="s">
         <v>866</v>
@@ -10125,7 +10125,7 @@
         <v>14</v>
       </c>
       <c r="K28" s="34" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="L28" s="35" t="s">
         <v>872</v>
@@ -10161,10 +10161,10 @@
         <v>14</v>
       </c>
       <c r="K29" s="34" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="L29" s="35" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="M29" s="35" t="s">
         <v>162</v>
@@ -10197,13 +10197,13 @@
         <v>14</v>
       </c>
       <c r="K30" s="34" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="L30" s="35" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="M30" s="35" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="N30" s="66"/>
     </row>
@@ -10233,10 +10233,10 @@
         <v>14</v>
       </c>
       <c r="K31" s="34" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="L31" s="34" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="M31" s="34" t="s">
         <v>846</v>
@@ -10269,10 +10269,10 @@
         <v>14</v>
       </c>
       <c r="K32" s="34" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="L32" s="35" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="M32" s="35" t="s">
         <v>612</v>
@@ -10305,7 +10305,7 @@
         <v>14</v>
       </c>
       <c r="K33" s="34" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="L33" s="35" t="s">
         <v>873</v>
@@ -10341,7 +10341,7 @@
         <v>14</v>
       </c>
       <c r="K34" s="34" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="L34" s="35" t="s">
         <v>874</v>
@@ -10377,7 +10377,7 @@
         <v>14</v>
       </c>
       <c r="K35" s="34" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="L35" s="35" t="s">
         <v>875</v>
@@ -10445,7 +10445,7 @@
         <v>14</v>
       </c>
       <c r="K37" s="34" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="L37" s="35" t="s">
         <v>877</v>
@@ -10513,7 +10513,7 @@
         <v>14</v>
       </c>
       <c r="K39" s="34" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="L39" s="35" t="s">
         <v>94</v>
@@ -10549,7 +10549,7 @@
         <v>14</v>
       </c>
       <c r="K40" s="34" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="L40" s="35" t="s">
         <v>879</v>
@@ -10595,7 +10595,7 @@
         <v>33</v>
       </c>
       <c r="E42" s="35" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="F42" s="35" t="s">
         <v>823</v>
@@ -10627,7 +10627,7 @@
         <v>34</v>
       </c>
       <c r="E43" s="35" t="s">
-        <v>1201</v>
+        <v>1200</v>
       </c>
       <c r="F43" s="34" t="s">
         <v>777</v>
@@ -10741,7 +10741,7 @@
         <v>14</v>
       </c>
       <c r="K46" s="34" t="s">
-        <v>1020</v>
+        <v>1303</v>
       </c>
       <c r="L46" s="35" t="s">
         <v>163</v>
@@ -10791,7 +10791,7 @@
         <v>39</v>
       </c>
       <c r="E48" s="34" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="F48" s="34" t="s">
         <v>341</v>
@@ -10809,7 +10809,7 @@
         <v>14</v>
       </c>
       <c r="K48" s="34" t="s">
-        <v>1020</v>
+        <v>1303</v>
       </c>
       <c r="L48" s="35" t="s">
         <v>524</v>
@@ -10827,7 +10827,7 @@
         <v>40</v>
       </c>
       <c r="E49" s="34" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="F49" s="34" t="s">
         <v>824</v>
@@ -10859,7 +10859,7 @@
         <v>41</v>
       </c>
       <c r="E50" s="34" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="F50" s="34" t="s">
         <v>778</v>
@@ -11004,7 +11004,7 @@
         <v>14</v>
       </c>
       <c r="K54" s="34" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="L54" s="35" t="s">
         <v>255</v>
@@ -11040,7 +11040,7 @@
         <v>14</v>
       </c>
       <c r="K55" s="34" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="L55" s="35" t="s">
         <v>544</v>
@@ -27945,10 +27945,10 @@
         <v>1015</v>
       </c>
       <c r="L11" s="35" t="s">
+        <v>1094</v>
+      </c>
+      <c r="M11" s="35" t="s">
         <v>1095</v>
-      </c>
-      <c r="M11" s="35" t="s">
-        <v>1096</v>
       </c>
       <c r="N11" s="63"/>
       <c r="O11" s="63"/>
@@ -27963,7 +27963,7 @@
         <v>4</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>1202</v>
+        <v>1201</v>
       </c>
       <c r="F12" s="34" t="s">
         <v>967</v>
@@ -27981,7 +27981,7 @@
         <v>14</v>
       </c>
       <c r="K12" s="34" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="L12" s="35" t="s">
         <v>839</v>
@@ -28002,7 +28002,7 @@
         <v>5</v>
       </c>
       <c r="E13" s="56" t="s">
-        <v>1203</v>
+        <v>1202</v>
       </c>
       <c r="F13" s="56" t="s">
         <v>685</v>
@@ -28018,7 +28018,7 @@
       </c>
       <c r="J13" s="49"/>
       <c r="K13" s="34" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="L13" s="70" t="s">
         <v>882</v>
@@ -28039,7 +28039,7 @@
         <v>6</v>
       </c>
       <c r="E14" s="56" t="s">
-        <v>1204</v>
+        <v>1203</v>
       </c>
       <c r="F14" s="56" t="s">
         <v>966</v>
@@ -28057,7 +28057,7 @@
         <v>14</v>
       </c>
       <c r="K14" s="34" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="L14" s="70" t="s">
         <v>565</v>
@@ -28076,7 +28076,7 @@
         <v>7</v>
       </c>
       <c r="E15" s="49" t="s">
-        <v>1205</v>
+        <v>1204</v>
       </c>
       <c r="F15" s="35" t="s">
         <v>758</v>
@@ -28093,7 +28093,7 @@
       <c r="J15" s="49"/>
       <c r="K15" s="34"/>
       <c r="L15" s="49" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="M15" s="35" t="s">
         <v>120</v>
@@ -28146,7 +28146,7 @@
         <v>9</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="F17" s="34" t="s">
         <v>365</v>
@@ -28216,7 +28216,7 @@
         <v>11</v>
       </c>
       <c r="E19" s="49" t="s">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="F19" s="49" t="s">
         <v>968</v>
@@ -28251,7 +28251,7 @@
         <v>12</v>
       </c>
       <c r="E20" s="49" t="s">
-        <v>1207</v>
+        <v>1206</v>
       </c>
       <c r="F20" s="49" t="s">
         <v>592</v>
@@ -28286,7 +28286,7 @@
         <v>13</v>
       </c>
       <c r="E21" s="49" t="s">
-        <v>1208</v>
+        <v>1207</v>
       </c>
       <c r="F21" s="35" t="s">
         <v>825</v>
@@ -28319,7 +28319,7 @@
         <v>14</v>
       </c>
       <c r="E22" s="49" t="s">
-        <v>1209</v>
+        <v>1208</v>
       </c>
       <c r="F22" s="34" t="s">
         <v>779</v>
@@ -28418,7 +28418,7 @@
         <v>17</v>
       </c>
       <c r="E25" s="49" t="s">
-        <v>1210</v>
+        <v>1209</v>
       </c>
       <c r="F25" s="56" t="s">
         <v>413</v>
@@ -28436,7 +28436,7 @@
         <v>14</v>
       </c>
       <c r="K25" s="15" t="s">
-        <v>1020</v>
+        <v>1303</v>
       </c>
       <c r="L25" s="35" t="s">
         <v>211</v>
@@ -28488,7 +28488,7 @@
         <v>19</v>
       </c>
       <c r="E27" s="34" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="F27" s="34" t="s">
         <v>345</v>
@@ -28506,7 +28506,7 @@
         <v>14</v>
       </c>
       <c r="K27" s="15" t="s">
-        <v>1020</v>
+        <v>1303</v>
       </c>
       <c r="L27" s="35" t="s">
         <v>524</v>
@@ -28525,7 +28525,7 @@
         <v>20</v>
       </c>
       <c r="E28" s="34" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="F28" s="34" t="s">
         <v>826</v>
@@ -28558,7 +28558,7 @@
         <v>21</v>
       </c>
       <c r="E29" s="34" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="F29" s="34" t="s">
         <v>780</v>
@@ -28706,7 +28706,7 @@
         <v>14</v>
       </c>
       <c r="K33" s="15" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="L33" s="35" t="s">
         <v>255</v>
@@ -29070,7 +29070,7 @@
         <v>3</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>1211</v>
+        <v>1210</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>673</v>
@@ -29131,10 +29131,10 @@
         <v>1015</v>
       </c>
       <c r="L7" s="35" t="s">
+        <v>1094</v>
+      </c>
+      <c r="M7" s="35" t="s">
         <v>1095</v>
-      </c>
-      <c r="M7" s="35" t="s">
-        <v>1096</v>
       </c>
       <c r="N7" s="51"/>
       <c r="O7" s="60"/>
@@ -29171,7 +29171,7 @@
       <c r="J8" s="56"/>
       <c r="K8" s="56"/>
       <c r="L8" s="35" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="M8" s="35" t="s">
         <v>98</v>
@@ -29214,7 +29214,7 @@
         <v>14</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="L9" s="12" t="s">
         <v>584</v>
@@ -29260,7 +29260,7 @@
         <v>14</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="L10" s="12" t="s">
         <v>997</v>
@@ -29281,18 +29281,18 @@
     <row r="11" spans="1:22" s="51" customFormat="1" ht="24" x14ac:dyDescent="0.45">
       <c r="A11" s="35"/>
       <c r="B11" s="56" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="C11" s="56"/>
       <c r="D11" s="52"/>
       <c r="E11" s="56" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="F11" s="56" t="s">
+        <v>1296</v>
+      </c>
+      <c r="G11" s="56" t="s">
         <v>1297</v>
-      </c>
-      <c r="G11" s="56" t="s">
-        <v>1298</v>
       </c>
       <c r="H11" s="56" t="s">
         <v>10</v>
@@ -29304,10 +29304,10 @@
         <v>14</v>
       </c>
       <c r="K11" s="56" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="L11" s="35" t="s">
-        <v>1129</v>
+        <v>1128</v>
       </c>
       <c r="M11" s="35"/>
     </row>
@@ -29339,10 +29339,10 @@
         <v>14</v>
       </c>
       <c r="K12" s="56" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="L12" s="35" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="M12" s="35" t="s">
         <v>171</v>
@@ -29356,7 +29356,7 @@
         <v>9</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>1212</v>
+        <v>1211</v>
       </c>
       <c r="F13" s="11" t="s">
         <v>560</v>
@@ -29374,7 +29374,7 @@
         <v>14</v>
       </c>
       <c r="K13" s="11" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="L13" s="87" t="s">
         <v>884</v>
@@ -29402,7 +29402,7 @@
         <v>10</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>1213</v>
+        <v>1212</v>
       </c>
       <c r="F14" s="11" t="s">
         <v>548</v>
@@ -29420,7 +29420,7 @@
         <v>14</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="L14" s="87" t="s">
         <v>697</v>
@@ -29466,7 +29466,7 @@
         <v>14</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="L15" s="12" t="s">
         <v>835</v>
@@ -29512,7 +29512,7 @@
         <v>14</v>
       </c>
       <c r="K16" s="11" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="L16" s="12" t="s">
         <v>173</v>
@@ -29558,7 +29558,7 @@
         <v>14</v>
       </c>
       <c r="K17" s="11" t="s">
-        <v>1053</v>
+        <v>1052</v>
       </c>
       <c r="L17" s="12" t="s">
         <v>19</v>
@@ -29604,10 +29604,10 @@
         <v>14</v>
       </c>
       <c r="K18" s="11" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="L18" s="12" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="M18" s="12" t="s">
         <v>20</v>
@@ -29630,7 +29630,7 @@
         <v>15</v>
       </c>
       <c r="E19" s="95" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="F19" s="95" t="s">
         <v>861</v>
@@ -29648,7 +29648,7 @@
         <v>14</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="L19" s="96" t="s">
         <v>836</v>
@@ -29692,7 +29692,7 @@
         <v>14</v>
       </c>
       <c r="K20" s="11" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="L20" s="12" t="s">
         <v>713</v>
@@ -29736,10 +29736,10 @@
         <v>14</v>
       </c>
       <c r="K21" s="11" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="L21" s="12" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="M21" s="12" t="s">
         <v>162</v>
@@ -29780,13 +29780,13 @@
         <v>14</v>
       </c>
       <c r="K22" s="11" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="L22" s="12" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="M22" s="12" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="N22" s="51"/>
       <c r="O22" s="51"/>
@@ -29824,10 +29824,10 @@
         <v>14</v>
       </c>
       <c r="K23" s="11" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="L23" s="12" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="M23" s="12" t="s">
         <v>846</v>
@@ -29868,10 +29868,10 @@
         <v>14</v>
       </c>
       <c r="K24" s="11" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="L24" s="12" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="M24" s="12" t="s">
         <v>612</v>
@@ -29912,7 +29912,7 @@
         <v>14</v>
       </c>
       <c r="K25" s="11" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="L25" s="12" t="s">
         <v>714</v>
@@ -29956,7 +29956,7 @@
         <v>14</v>
       </c>
       <c r="K26" s="11" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="L26" s="12" t="s">
         <v>715</v>
@@ -30000,7 +30000,7 @@
         <v>14</v>
       </c>
       <c r="K27" s="11" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="L27" s="12" t="s">
         <v>716</v>
@@ -30084,7 +30084,7 @@
         <v>14</v>
       </c>
       <c r="K29" s="11" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="L29" s="12" t="s">
         <v>718</v>
@@ -30168,7 +30168,7 @@
         <v>14</v>
       </c>
       <c r="K31" s="11" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="L31" s="12" t="s">
         <v>683</v>
@@ -30194,7 +30194,7 @@
         <v>28</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>1214</v>
+        <v>1213</v>
       </c>
       <c r="F32" s="11" t="s">
         <v>538</v>
@@ -30211,7 +30211,7 @@
       <c r="J32" s="11"/>
       <c r="K32" s="11"/>
       <c r="L32" s="12" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="M32" s="12" t="s">
         <v>176</v>
@@ -30234,7 +30234,7 @@
         <v>29</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>1217</v>
+        <v>1216</v>
       </c>
       <c r="F33" s="11" t="s">
         <v>537</v>
@@ -30251,7 +30251,7 @@
       <c r="J33" s="11"/>
       <c r="K33" s="11"/>
       <c r="L33" s="12" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="M33" s="12" t="s">
         <v>177</v>
@@ -30274,7 +30274,7 @@
         <v>30</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>1215</v>
+        <v>1214</v>
       </c>
       <c r="F34" s="12" t="s">
         <v>827</v>
@@ -30314,7 +30314,7 @@
         <v>31</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>1216</v>
+        <v>1215</v>
       </c>
       <c r="F35" s="15" t="s">
         <v>781</v>
@@ -30452,7 +30452,7 @@
         <v>14</v>
       </c>
       <c r="K38" s="11" t="s">
-        <v>1020</v>
+        <v>1303</v>
       </c>
       <c r="L38" s="12" t="s">
         <v>180</v>
@@ -30518,7 +30518,7 @@
         <v>36</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>1218</v>
+        <v>1217</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>515</v>
@@ -30536,7 +30536,7 @@
         <v>14</v>
       </c>
       <c r="K40" s="11" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="L40" s="12" t="s">
         <v>181</v>
@@ -30657,7 +30657,7 @@
         <v>14</v>
       </c>
       <c r="K43" s="11" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="L43" s="12" t="s">
         <v>687</v>
@@ -30701,7 +30701,7 @@
         <v>14</v>
       </c>
       <c r="K44" s="11" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="L44" s="11" t="s">
         <v>688</v>
@@ -30727,7 +30727,7 @@
         <v>41</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>1219</v>
+        <v>1218</v>
       </c>
       <c r="F45" s="11" t="s">
         <v>532</v>
@@ -30767,7 +30767,7 @@
         <v>42</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="F46" s="11" t="s">
         <v>533</v>
@@ -30807,13 +30807,13 @@
         <v>43</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="F47" s="56" t="s">
+        <v>1289</v>
+      </c>
+      <c r="G47" s="56" t="s">
         <v>1290</v>
-      </c>
-      <c r="G47" s="56" t="s">
-        <v>1291</v>
       </c>
       <c r="H47" s="11" t="s">
         <v>148</v>
@@ -31174,7 +31174,7 @@
   <dimension ref="A1:V17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -31337,20 +31337,20 @@
     <row r="5" spans="1:22" s="23" customFormat="1" ht="58.9" x14ac:dyDescent="0.45">
       <c r="A5" s="45"/>
       <c r="B5" s="56" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="C5" s="56"/>
       <c r="D5" s="52">
         <v>2</v>
       </c>
       <c r="E5" s="56" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="F5" s="56" t="s">
+        <v>1298</v>
+      </c>
+      <c r="G5" s="56" t="s">
         <v>1299</v>
-      </c>
-      <c r="G5" s="56" t="s">
-        <v>1300</v>
       </c>
       <c r="H5" s="56" t="s">
         <v>10</v>
@@ -31362,19 +31362,19 @@
         <v>14</v>
       </c>
       <c r="K5" s="56" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="L5" s="35" t="s">
-        <v>1245</v>
+        <v>1244</v>
       </c>
       <c r="M5" s="35" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="6" spans="1:22" s="2" customFormat="1" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A6" s="12"/>
       <c r="B6" s="56" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="C6" s="56"/>
       <c r="D6" s="52">
@@ -31384,10 +31384,10 @@
         <v>22</v>
       </c>
       <c r="F6" s="56" t="s">
+        <v>1124</v>
+      </c>
+      <c r="G6" s="56" t="s">
         <v>1125</v>
-      </c>
-      <c r="G6" s="56" t="s">
-        <v>1126</v>
       </c>
       <c r="H6" s="56" t="s">
         <v>10</v>
@@ -31399,13 +31399,13 @@
         <v>14</v>
       </c>
       <c r="K6" s="56" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="L6" s="35" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="M6" s="35" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
       <c r="N6" s="51"/>
       <c r="O6" s="51"/>
@@ -31427,13 +31427,13 @@
         <v>4</v>
       </c>
       <c r="E7" s="56" t="s">
-        <v>1136</v>
+        <v>1135</v>
       </c>
       <c r="F7" s="56" t="s">
+        <v>1133</v>
+      </c>
+      <c r="G7" s="56" t="s">
         <v>1134</v>
-      </c>
-      <c r="G7" s="56" t="s">
-        <v>1135</v>
       </c>
       <c r="H7" s="56" t="s">
         <v>13</v>
@@ -31444,7 +31444,7 @@
       <c r="J7" s="56"/>
       <c r="K7" s="35"/>
       <c r="L7" s="35" t="s">
-        <v>1137</v>
+        <v>1136</v>
       </c>
       <c r="M7" s="35" t="s">
         <v>552</v>
@@ -31489,13 +31489,13 @@
         <v>6</v>
       </c>
       <c r="E9" s="56" t="s">
+        <v>1137</v>
+      </c>
+      <c r="F9" s="56" t="s">
         <v>1138</v>
       </c>
-      <c r="F9" s="56" t="s">
+      <c r="G9" s="56" t="s">
         <v>1139</v>
-      </c>
-      <c r="G9" s="56" t="s">
-        <v>1140</v>
       </c>
       <c r="H9" s="56" t="s">
         <v>10</v>
@@ -31507,10 +31507,10 @@
         <v>14</v>
       </c>
       <c r="K9" s="35" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="L9" s="35" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="M9" s="35" t="s">
         <v>441</v>
@@ -31519,7 +31519,7 @@
     <row r="10" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A10" s="56"/>
       <c r="B10" s="56" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="C10" s="56"/>
       <c r="D10" s="52">
@@ -31529,10 +31529,10 @@
         <v>197</v>
       </c>
       <c r="F10" s="56" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="G10" s="56" t="s">
-        <v>1257</v>
+        <v>1256</v>
       </c>
       <c r="H10" s="56" t="s">
         <v>10</v>
@@ -31544,7 +31544,7 @@
         <v>14</v>
       </c>
       <c r="K10" s="34" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="L10" s="56" t="s">
         <v>197</v>
@@ -31579,7 +31579,7 @@
         <v>14</v>
       </c>
       <c r="K11" s="35" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="L11" s="35" t="s">
         <v>557</v>
@@ -31614,7 +31614,7 @@
         <v>14</v>
       </c>
       <c r="K12" s="35" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="L12" s="35" t="s">
         <v>246</v>
@@ -31626,53 +31626,53 @@
     <row r="13" spans="1:22" s="23" customFormat="1" ht="24" x14ac:dyDescent="0.45">
       <c r="A13" s="103"/>
       <c r="B13" s="56" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="C13" s="56"/>
       <c r="D13" s="52">
         <v>10</v>
       </c>
       <c r="E13" s="56" t="s">
+        <v>1141</v>
+      </c>
+      <c r="F13" s="56" t="s">
+        <v>1140</v>
+      </c>
+      <c r="G13" s="56" t="s">
+        <v>1249</v>
+      </c>
+      <c r="H13" s="56" t="s">
         <v>1142</v>
-      </c>
-      <c r="F13" s="56" t="s">
-        <v>1141</v>
-      </c>
-      <c r="G13" s="56" t="s">
-        <v>1250</v>
-      </c>
-      <c r="H13" s="56" t="s">
-        <v>1143</v>
       </c>
       <c r="I13" s="56" t="s">
         <v>11</v>
       </c>
       <c r="J13" s="56" t="s">
-        <v>1143</v>
+        <v>1142</v>
       </c>
       <c r="K13" s="35"/>
       <c r="L13" s="35" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="M13" s="35"/>
     </row>
     <row r="14" spans="1:22" s="23" customFormat="1" ht="24" x14ac:dyDescent="0.45">
       <c r="A14" s="103"/>
       <c r="B14" s="56" t="s">
-        <v>1256</v>
+        <v>1255</v>
       </c>
       <c r="C14" s="56"/>
       <c r="D14" s="52">
         <v>11</v>
       </c>
       <c r="E14" s="56" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="F14" s="34" t="s">
-        <v>1144</v>
+        <v>1143</v>
       </c>
       <c r="G14" s="34" t="s">
-        <v>1251</v>
+        <v>1250</v>
       </c>
       <c r="H14" s="56" t="s">
         <v>10</v>
@@ -31684,10 +31684,10 @@
         <v>14</v>
       </c>
       <c r="K14" s="35" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="L14" s="35" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="M14" s="35"/>
     </row>
@@ -31751,7 +31751,7 @@
       <c r="J16" s="56"/>
       <c r="K16" s="35"/>
       <c r="L16" s="35" t="s">
-        <v>1133</v>
+        <v>1132</v>
       </c>
       <c r="M16" s="35"/>
     </row>
@@ -31781,10 +31781,10 @@
         <v>14</v>
       </c>
       <c r="K17" s="35" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="L17" s="104" t="s">
-        <v>1132</v>
+        <v>1131</v>
       </c>
       <c r="M17" s="35"/>
     </row>
@@ -31799,7 +31799,7 @@
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -32009,10 +32009,10 @@
         <v>2</v>
       </c>
       <c r="E6" s="56" t="s">
-        <v>1124</v>
+        <v>1123</v>
       </c>
       <c r="F6" s="56" t="s">
-        <v>1122</v>
+        <v>1121</v>
       </c>
       <c r="G6" s="56" t="s">
         <v>899</v>
@@ -32026,7 +32026,7 @@
       <c r="J6" s="56"/>
       <c r="K6" s="34"/>
       <c r="L6" s="35" t="s">
-        <v>1123</v>
+        <v>1122</v>
       </c>
       <c r="M6" s="35" t="s">
         <v>189</v>
@@ -32035,20 +32035,20 @@
     <row r="7" spans="1:13" s="51" customFormat="1" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A7" s="35"/>
       <c r="B7" s="56" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="C7" s="56"/>
       <c r="D7" s="52">
         <v>3</v>
       </c>
       <c r="E7" s="56" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
       <c r="F7" s="56" t="s">
+        <v>1300</v>
+      </c>
+      <c r="G7" s="56" t="s">
         <v>1301</v>
-      </c>
-      <c r="G7" s="56" t="s">
-        <v>1302</v>
       </c>
       <c r="H7" s="56" t="s">
         <v>10</v>
@@ -32060,19 +32060,19 @@
         <v>14</v>
       </c>
       <c r="K7" s="56" t="s">
-        <v>1292</v>
+        <v>1291</v>
       </c>
       <c r="L7" s="35" t="s">
-        <v>1151</v>
+        <v>1150</v>
       </c>
       <c r="M7" s="35" t="s">
-        <v>1127</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="51" customFormat="1" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A8" s="35"/>
       <c r="B8" s="56" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="C8" s="56"/>
       <c r="D8" s="52">
@@ -32082,10 +32082,10 @@
         <v>22</v>
       </c>
       <c r="F8" s="56" t="s">
+        <v>1148</v>
+      </c>
+      <c r="G8" s="56" t="s">
         <v>1149</v>
-      </c>
-      <c r="G8" s="56" t="s">
-        <v>1150</v>
       </c>
       <c r="H8" s="56" t="s">
         <v>10</v>
@@ -32097,13 +32097,13 @@
         <v>14</v>
       </c>
       <c r="K8" s="56" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="L8" s="35" t="s">
-        <v>1130</v>
+        <v>1129</v>
       </c>
       <c r="M8" s="35" t="s">
-        <v>1128</v>
+        <v>1127</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="51" customFormat="1" ht="24" x14ac:dyDescent="0.45">
@@ -32149,7 +32149,7 @@
         <v>6</v>
       </c>
       <c r="E10" s="56" t="s">
-        <v>1225</v>
+        <v>1224</v>
       </c>
       <c r="F10" s="35" t="s">
         <v>760</v>
@@ -32182,13 +32182,13 @@
         <v>7</v>
       </c>
       <c r="E11" s="56" t="s">
-        <v>1246</v>
+        <v>1245</v>
       </c>
       <c r="F11" s="56" t="s">
+        <v>1151</v>
+      </c>
+      <c r="G11" s="56" t="s">
         <v>1152</v>
-      </c>
-      <c r="G11" s="56" t="s">
-        <v>1153</v>
       </c>
       <c r="H11" s="56" t="s">
         <v>10</v>
@@ -32200,7 +32200,7 @@
         <v>14</v>
       </c>
       <c r="K11" s="34" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="L11" s="35" t="s">
         <v>886</v>
@@ -32217,13 +32217,13 @@
         <v>8</v>
       </c>
       <c r="E12" s="56" t="s">
-        <v>1247</v>
+        <v>1246</v>
       </c>
       <c r="F12" s="56" t="s">
+        <v>1153</v>
+      </c>
+      <c r="G12" s="56" t="s">
         <v>1154</v>
-      </c>
-      <c r="G12" s="56" t="s">
-        <v>1155</v>
       </c>
       <c r="H12" s="56" t="s">
         <v>10</v>
@@ -32248,13 +32248,13 @@
         <v>9</v>
       </c>
       <c r="E13" s="56" t="s">
-        <v>1222</v>
+        <v>1221</v>
       </c>
       <c r="F13" s="56" t="s">
+        <v>1079</v>
+      </c>
+      <c r="G13" s="56" t="s">
         <v>1080</v>
-      </c>
-      <c r="G13" s="56" t="s">
-        <v>1081</v>
       </c>
       <c r="H13" s="56" t="s">
         <v>10</v>
@@ -32266,13 +32266,13 @@
         <v>14</v>
       </c>
       <c r="K13" s="34" t="s">
+        <v>1081</v>
+      </c>
+      <c r="L13" s="35" t="s">
         <v>1082</v>
       </c>
-      <c r="L13" s="35" t="s">
+      <c r="M13" s="56" t="s">
         <v>1083</v>
-      </c>
-      <c r="M13" s="56" t="s">
-        <v>1084</v>
       </c>
     </row>
     <row r="14" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.45">
@@ -32301,7 +32301,7 @@
         <v>14</v>
       </c>
       <c r="K14" s="34" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="L14" s="56" t="s">
         <v>192</v>
@@ -32336,7 +32336,7 @@
         <v>14</v>
       </c>
       <c r="K15" s="34" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="L15" s="56" t="s">
         <v>557</v>
@@ -32348,20 +32348,20 @@
     <row r="16" spans="1:13" s="51" customFormat="1" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A16" s="56"/>
       <c r="B16" s="56" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="C16" s="56"/>
       <c r="D16" s="52">
         <v>12</v>
       </c>
       <c r="E16" s="56" t="s">
+        <v>1084</v>
+      </c>
+      <c r="F16" s="56" t="s">
         <v>1085</v>
       </c>
-      <c r="F16" s="56" t="s">
-        <v>1086</v>
-      </c>
       <c r="G16" s="56" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="H16" s="56" t="s">
         <v>10</v>
@@ -32373,30 +32373,30 @@
         <v>14</v>
       </c>
       <c r="K16" s="34" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="L16" s="35" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="M16" s="56"/>
     </row>
     <row r="17" spans="1:13" s="51" customFormat="1" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A17" s="56"/>
       <c r="B17" s="56" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="C17" s="56"/>
       <c r="D17" s="52">
         <v>13</v>
       </c>
       <c r="E17" s="56" t="s">
+        <v>1087</v>
+      </c>
+      <c r="F17" s="56" t="s">
         <v>1088</v>
       </c>
-      <c r="F17" s="56" t="s">
+      <c r="G17" s="56" t="s">
         <v>1089</v>
-      </c>
-      <c r="G17" s="56" t="s">
-        <v>1090</v>
       </c>
       <c r="H17" s="56" t="s">
         <v>10</v>
@@ -32408,30 +32408,30 @@
         <v>14</v>
       </c>
       <c r="K17" s="34" t="s">
+        <v>1090</v>
+      </c>
+      <c r="L17" s="35" t="s">
         <v>1091</v>
-      </c>
-      <c r="L17" s="35" t="s">
-        <v>1092</v>
       </c>
       <c r="M17" s="56"/>
     </row>
     <row r="18" spans="1:13" s="51" customFormat="1" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="56"/>
       <c r="B18" s="56" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="C18" s="56"/>
       <c r="D18" s="52">
         <v>14</v>
       </c>
       <c r="E18" s="56" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="F18" s="56" t="s">
+        <v>1253</v>
+      </c>
+      <c r="G18" s="56" t="s">
         <v>1254</v>
-      </c>
-      <c r="G18" s="56" t="s">
-        <v>1255</v>
       </c>
       <c r="H18" s="56" t="s">
         <v>148</v>
@@ -32442,30 +32442,30 @@
       <c r="J18" s="56"/>
       <c r="K18" s="34"/>
       <c r="L18" s="35" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="M18" s="56"/>
     </row>
     <row r="19" spans="1:13" s="51" customFormat="1" ht="24" x14ac:dyDescent="0.45">
       <c r="A19" s="56"/>
       <c r="B19" s="56" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="C19" s="56"/>
       <c r="D19" s="52">
         <v>15</v>
       </c>
       <c r="E19" s="56" t="s">
-        <v>1142</v>
+        <v>1141</v>
       </c>
       <c r="F19" s="56" t="s">
-        <v>1156</v>
+        <v>1155</v>
       </c>
       <c r="G19" s="56" t="s">
-        <v>1249</v>
+        <v>1248</v>
       </c>
       <c r="H19" s="56" t="s">
-        <v>1253</v>
+        <v>1252</v>
       </c>
       <c r="I19" s="56" t="s">
         <v>11</v>
@@ -32473,27 +32473,27 @@
       <c r="J19" s="56"/>
       <c r="K19" s="35"/>
       <c r="L19" s="35" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="M19" s="35"/>
     </row>
     <row r="20" spans="1:13" s="51" customFormat="1" ht="24" x14ac:dyDescent="0.45">
       <c r="A20" s="56"/>
       <c r="B20" s="56" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="C20" s="56"/>
       <c r="D20" s="52">
         <v>16</v>
       </c>
       <c r="E20" s="56" t="s">
-        <v>1145</v>
+        <v>1144</v>
       </c>
       <c r="F20" s="34" t="s">
-        <v>1157</v>
+        <v>1156</v>
       </c>
       <c r="G20" s="34" t="s">
-        <v>1248</v>
+        <v>1247</v>
       </c>
       <c r="H20" s="56" t="s">
         <v>10</v>
@@ -32505,10 +32505,10 @@
         <v>14</v>
       </c>
       <c r="K20" s="34" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="L20" s="35" t="s">
-        <v>1148</v>
+        <v>1147</v>
       </c>
       <c r="M20" s="35"/>
     </row>
@@ -32520,7 +32520,7 @@
         <v>17</v>
       </c>
       <c r="E21" s="56" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="F21" s="35" t="s">
         <v>828</v>
@@ -32551,7 +32551,7 @@
         <v>18</v>
       </c>
       <c r="E22" s="56" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="F22" s="34" t="s">
         <v>782</v>
@@ -32662,7 +32662,7 @@
         <v>14</v>
       </c>
       <c r="K25" s="15" t="s">
-        <v>1020</v>
+        <v>1303</v>
       </c>
       <c r="L25" s="35" t="s">
         <v>196</v>
@@ -32905,7 +32905,7 @@
         <v>834</v>
       </c>
       <c r="L4" s="35" t="s">
-        <v>1258</v>
+        <v>1257</v>
       </c>
       <c r="M4" s="35" t="s">
         <v>108</v>
@@ -32943,7 +32943,7 @@
         <v>1012</v>
       </c>
       <c r="M5" s="50" t="s">
-        <v>1259</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="10" customFormat="1" ht="11.65" x14ac:dyDescent="0.35">
@@ -32993,7 +32993,7 @@
         <v>5</v>
       </c>
       <c r="E7" s="35" t="s">
-        <v>1260</v>
+        <v>1259</v>
       </c>
       <c r="F7" s="35" t="s">
         <v>750</v>
@@ -33024,7 +33024,7 @@
         <v>6</v>
       </c>
       <c r="E8" s="35" t="s">
-        <v>1164</v>
+        <v>1163</v>
       </c>
       <c r="F8" s="35" t="s">
         <v>302</v>
@@ -33099,10 +33099,10 @@
         <v>689</v>
       </c>
       <c r="F10" s="34" t="s">
-        <v>1158</v>
+        <v>1157</v>
       </c>
       <c r="G10" s="34" t="s">
-        <v>1160</v>
+        <v>1159</v>
       </c>
       <c r="H10" s="35" t="s">
         <v>10</v>
@@ -33117,7 +33117,7 @@
         <v>1015</v>
       </c>
       <c r="L10" s="35" t="s">
-        <v>1162</v>
+        <v>1161</v>
       </c>
       <c r="M10" s="34"/>
     </row>
@@ -33132,10 +33132,10 @@
         <v>255</v>
       </c>
       <c r="F11" s="35" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="G11" s="34" t="s">
-        <v>1161</v>
+        <v>1160</v>
       </c>
       <c r="H11" s="35" t="s">
         <v>10</v>
@@ -33147,7 +33147,7 @@
         <v>14</v>
       </c>
       <c r="K11" s="34" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="L11" s="35" t="s">
         <v>255</v>
@@ -33724,8 +33724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -34065,7 +34065,7 @@
         <v>5</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>1165</v>
+        <v>1164</v>
       </c>
       <c r="F10" s="35" t="s">
         <v>751</v>
@@ -34082,7 +34082,7 @@
       <c r="J10" s="35"/>
       <c r="K10" s="35"/>
       <c r="L10" s="35" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="M10" s="35" t="s">
         <v>120</v>
@@ -34096,7 +34096,7 @@
         <v>6</v>
       </c>
       <c r="E11" s="34" t="s">
-        <v>1166</v>
+        <v>1165</v>
       </c>
       <c r="F11" s="34" t="s">
         <v>315</v>
@@ -34131,7 +34131,7 @@
         <v>7</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>1167</v>
+        <v>1166</v>
       </c>
       <c r="F12" s="34" t="s">
         <v>316</v>
@@ -34197,7 +34197,7 @@
         <v>9</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="F14" s="35" t="s">
         <v>813</v>
@@ -34228,7 +34228,7 @@
         <v>10</v>
       </c>
       <c r="E15" s="35" t="s">
-        <v>1169</v>
+        <v>1168</v>
       </c>
       <c r="F15" s="34" t="s">
         <v>761</v>
@@ -34339,7 +34339,7 @@
         <v>14</v>
       </c>
       <c r="K18" s="35" t="s">
-        <v>1020</v>
+        <v>1303</v>
       </c>
       <c r="L18" s="54" t="s">
         <v>201</v>
@@ -34387,7 +34387,7 @@
         <v>15</v>
       </c>
       <c r="E20" s="58" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="F20" s="58" t="s">
         <v>320</v>
@@ -34405,7 +34405,7 @@
         <v>14</v>
       </c>
       <c r="K20" s="35" t="s">
-        <v>1020</v>
+        <v>1303</v>
       </c>
       <c r="L20" s="57" t="s">
         <v>524</v>
@@ -34422,7 +34422,7 @@
         <v>16</v>
       </c>
       <c r="E21" s="34" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="F21" s="34" t="s">
         <v>812</v>
@@ -34453,7 +34453,7 @@
         <v>17</v>
       </c>
       <c r="E22" s="34" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="F22" s="34" t="s">
         <v>762</v>
@@ -34595,7 +34595,7 @@
         <v>14</v>
       </c>
       <c r="K26" s="15" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="L26" s="35" t="s">
         <v>255</v>
@@ -34859,10 +34859,10 @@
         <v>1015</v>
       </c>
       <c r="L6" s="35" t="s">
+        <v>1094</v>
+      </c>
+      <c r="M6" s="35" t="s">
         <v>1095</v>
-      </c>
-      <c r="M6" s="35" t="s">
-        <v>1096</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="35.65" x14ac:dyDescent="0.45">
@@ -34873,7 +34873,7 @@
         <v>4</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="F7" s="34" t="s">
         <v>944</v>
@@ -34891,7 +34891,7 @@
         <v>91</v>
       </c>
       <c r="K7" s="35" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="L7" s="59" t="s">
         <v>631</v>
@@ -34908,13 +34908,13 @@
         <v>5</v>
       </c>
       <c r="E8" s="35" t="s">
+        <v>1234</v>
+      </c>
+      <c r="F8" s="35" t="s">
         <v>1235</v>
       </c>
-      <c r="F8" s="35" t="s">
-        <v>1236</v>
-      </c>
       <c r="G8" s="35" t="s">
-        <v>1238</v>
+        <v>1237</v>
       </c>
       <c r="H8" s="35" t="s">
         <v>10</v>
@@ -34940,13 +34940,13 @@
         <v>6</v>
       </c>
       <c r="E9" s="34" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="F9" s="34" t="s">
-        <v>1231</v>
+        <v>1230</v>
       </c>
       <c r="G9" s="34" t="s">
-        <v>1237</v>
+        <v>1236</v>
       </c>
       <c r="H9" s="34" t="s">
         <v>10</v>
@@ -34958,7 +34958,7 @@
         <v>14</v>
       </c>
       <c r="K9" s="102" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="L9" s="59"/>
       <c r="M9" s="59"/>
@@ -34988,10 +34988,10 @@
       <c r="J10" s="35"/>
       <c r="K10" s="35"/>
       <c r="L10" s="35" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="M10" s="35" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="35.65" x14ac:dyDescent="0.45">
@@ -35037,7 +35037,7 @@
         <v>9</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="F12" s="34" t="s">
         <v>350</v>
@@ -35103,7 +35103,7 @@
         <v>11</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>1173</v>
+        <v>1172</v>
       </c>
       <c r="F14" s="35" t="s">
         <v>814</v>
@@ -35134,7 +35134,7 @@
         <v>12</v>
       </c>
       <c r="E15" s="35" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="F15" s="34" t="s">
         <v>763</v>
@@ -35245,7 +35245,7 @@
         <v>14</v>
       </c>
       <c r="K18" s="35" t="s">
-        <v>1020</v>
+        <v>1303</v>
       </c>
       <c r="L18" s="35" t="s">
         <v>201</v>
@@ -35293,7 +35293,7 @@
         <v>17</v>
       </c>
       <c r="E20" s="34" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="F20" s="34" t="s">
         <v>324</v>
@@ -35311,7 +35311,7 @@
         <v>14</v>
       </c>
       <c r="K20" s="35" t="s">
-        <v>1020</v>
+        <v>1303</v>
       </c>
       <c r="L20" s="35" t="s">
         <v>524</v>
@@ -35328,7 +35328,7 @@
         <v>18</v>
       </c>
       <c r="E21" s="34" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="F21" s="34" t="s">
         <v>815</v>
@@ -35359,7 +35359,7 @@
         <v>19</v>
       </c>
       <c r="E22" s="34" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="F22" s="34" t="s">
         <v>764</v>
@@ -35501,7 +35501,7 @@
         <v>14</v>
       </c>
       <c r="K26" s="35" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="L26" s="35" t="s">
         <v>255</v>
@@ -35764,7 +35764,7 @@
         <v>1003</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="M5" s="6" t="s">
         <v>115</v>
@@ -35798,7 +35798,7 @@
         <v>14</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="L6" s="12" t="s">
         <v>54</v>
@@ -36096,7 +36096,7 @@
         <v>3</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>580</v>
@@ -36111,11 +36111,11 @@
         <v>11</v>
       </c>
       <c r="J8" s="35" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="K8" s="34"/>
       <c r="L8" s="35" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="M8" s="35" t="s">
         <v>577</v>
@@ -36150,10 +36150,10 @@
         <v>1015</v>
       </c>
       <c r="L9" s="35" t="s">
+        <v>1094</v>
+      </c>
+      <c r="M9" s="35" t="s">
         <v>1095</v>
-      </c>
-      <c r="M9" s="35" t="s">
-        <v>1096</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.45">
@@ -36164,7 +36164,7 @@
         <v>5</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>1177</v>
+        <v>1176</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>753</v>
@@ -36181,10 +36181,10 @@
       <c r="J10" s="35"/>
       <c r="K10" s="34"/>
       <c r="L10" s="35" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="M10" s="35" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="11" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.45">
@@ -36230,7 +36230,7 @@
         <v>7</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="F12" s="15" t="s">
         <v>353</v>
@@ -36296,7 +36296,7 @@
         <v>9</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>1168</v>
+        <v>1167</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>691</v>
@@ -36327,7 +36327,7 @@
         <v>10</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="F15" s="15" t="s">
         <v>694</v>
@@ -36438,7 +36438,7 @@
         <v>14</v>
       </c>
       <c r="K18" s="15" t="s">
-        <v>1020</v>
+        <v>1303</v>
       </c>
       <c r="L18" s="12" t="s">
         <v>122</v>
@@ -36486,7 +36486,7 @@
         <v>15</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="F20" s="15" t="s">
         <v>328</v>
@@ -36504,7 +36504,7 @@
         <v>14</v>
       </c>
       <c r="K20" s="15" t="s">
-        <v>1020</v>
+        <v>1303</v>
       </c>
       <c r="L20" s="12" t="s">
         <v>524</v>
@@ -36521,7 +36521,7 @@
         <v>16</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="F21" s="15" t="s">
         <v>816</v>
@@ -36552,7 +36552,7 @@
         <v>17</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="F22" s="15" t="s">
         <v>765</v>
@@ -36694,7 +36694,7 @@
         <v>14</v>
       </c>
       <c r="K26" s="15" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="L26" s="12" t="s">
         <v>255</v>
@@ -37074,7 +37074,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>1176</v>
+        <v>1175</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>855</v>
@@ -37089,11 +37089,11 @@
         <v>11</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="K10" s="12"/>
       <c r="L10" s="12" t="s">
-        <v>1065</v>
+        <v>1064</v>
       </c>
       <c r="M10" s="12"/>
     </row>
@@ -37159,10 +37159,10 @@
         <v>1015</v>
       </c>
       <c r="L12" s="35" t="s">
+        <v>1094</v>
+      </c>
+      <c r="M12" s="35" t="s">
         <v>1095</v>
-      </c>
-      <c r="M12" s="35" t="s">
-        <v>1096</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.45">
@@ -37173,7 +37173,7 @@
         <v>5</v>
       </c>
       <c r="E13" s="35" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="F13" s="35" t="s">
         <v>754</v>
@@ -37190,7 +37190,7 @@
       <c r="J13" s="35"/>
       <c r="K13" s="35"/>
       <c r="L13" s="35" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="M13" s="35" t="s">
         <v>120</v>
@@ -37204,7 +37204,7 @@
         <v>6</v>
       </c>
       <c r="E14" s="34" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="F14" s="34" t="s">
         <v>279</v>
@@ -37239,7 +37239,7 @@
         <v>7</v>
       </c>
       <c r="E15" s="34" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="F15" s="34" t="s">
         <v>280</v>
@@ -37323,13 +37323,13 @@
         <v>14</v>
       </c>
       <c r="K17" s="35" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="L17" s="52" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
       <c r="M17" s="52" t="s">
-        <v>1262</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="18" spans="1:14" s="2" customFormat="1" ht="35.65" x14ac:dyDescent="0.45">
@@ -37340,10 +37340,10 @@
         <v>10</v>
       </c>
       <c r="E18" s="35" t="s">
+        <v>1262</v>
+      </c>
+      <c r="F18" s="35" t="s">
         <v>1263</v>
-      </c>
-      <c r="F18" s="35" t="s">
-        <v>1264</v>
       </c>
       <c r="G18" s="35" t="s">
         <v>290</v>
@@ -37359,10 +37359,10 @@
       </c>
       <c r="K18" s="35"/>
       <c r="L18" s="35" t="s">
+        <v>1264</v>
+      </c>
+      <c r="M18" s="35" t="s">
         <v>1265</v>
-      </c>
-      <c r="M18" s="35" t="s">
-        <v>1266</v>
       </c>
       <c r="N18" s="101"/>
     </row>
@@ -37392,13 +37392,13 @@
         <v>14</v>
       </c>
       <c r="K19" s="35" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="L19" s="35" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
       <c r="M19" s="35" t="s">
-        <v>1267</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="20" spans="1:14" s="2" customFormat="1" ht="24" x14ac:dyDescent="0.45">
@@ -37457,10 +37457,10 @@
       <c r="J21" s="35"/>
       <c r="K21" s="35"/>
       <c r="L21" s="35" t="s">
+        <v>1267</v>
+      </c>
+      <c r="M21" s="35" t="s">
         <v>1268</v>
-      </c>
-      <c r="M21" s="35" t="s">
-        <v>1269</v>
       </c>
     </row>
     <row r="22" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.45">
@@ -37491,7 +37491,7 @@
         <v>14</v>
       </c>
       <c r="K22" s="35" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="L22" s="35" t="s">
         <v>127</v>
@@ -37510,7 +37510,7 @@
         <v>15</v>
       </c>
       <c r="E23" s="35" t="s">
-        <v>1270</v>
+        <v>1269</v>
       </c>
       <c r="F23" s="35" t="s">
         <v>250</v>
@@ -37558,10 +37558,10 @@
       <c r="J24" s="35"/>
       <c r="K24" s="35"/>
       <c r="L24" s="35" t="s">
+        <v>1270</v>
+      </c>
+      <c r="M24" s="35" t="s">
         <v>1271</v>
-      </c>
-      <c r="M24" s="35" t="s">
-        <v>1272</v>
       </c>
     </row>
     <row r="25" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.45">
@@ -37572,7 +37572,7 @@
         <v>17</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>1182</v>
+        <v>1181</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>817</v>
@@ -37603,7 +37603,7 @@
         <v>18</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>1183</v>
+        <v>1182</v>
       </c>
       <c r="F26" s="15" t="s">
         <v>771</v>
@@ -37714,7 +37714,7 @@
         <v>14</v>
       </c>
       <c r="K29" s="12" t="s">
-        <v>1020</v>
+        <v>1303</v>
       </c>
       <c r="L29" s="35" t="s">
         <v>562</v>
@@ -37762,7 +37762,7 @@
         <v>23</v>
       </c>
       <c r="E31" s="34" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="F31" s="34" t="s">
         <v>287</v>
@@ -37778,7 +37778,7 @@
         <v>14</v>
       </c>
       <c r="K31" s="12" t="s">
-        <v>1020</v>
+        <v>1303</v>
       </c>
       <c r="L31" s="35" t="s">
         <v>524</v>
@@ -37795,7 +37795,7 @@
         <v>24</v>
       </c>
       <c r="E32" s="34" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="F32" s="34" t="s">
         <v>818</v>
@@ -37826,7 +37826,7 @@
         <v>25</v>
       </c>
       <c r="E33" s="34" t="s">
-        <v>1185</v>
+        <v>1184</v>
       </c>
       <c r="F33" s="34" t="s">
         <v>772</v>
@@ -37968,7 +37968,7 @@
         <v>14</v>
       </c>
       <c r="K37" s="12" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="L37" s="35" t="s">
         <v>255</v>
@@ -38285,10 +38285,10 @@
         <v>1015</v>
       </c>
       <c r="L6" s="35" t="s">
+        <v>1094</v>
+      </c>
+      <c r="M6" s="35" t="s">
         <v>1095</v>
-      </c>
-      <c r="M6" s="35" t="s">
-        <v>1096</v>
       </c>
       <c r="N6" s="90"/>
     </row>
@@ -38332,7 +38332,7 @@
         <v>4</v>
       </c>
       <c r="E8" s="34" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="F8" s="35" t="s">
         <v>755</v>
@@ -38349,7 +38349,7 @@
       <c r="J8" s="34"/>
       <c r="K8" s="34"/>
       <c r="L8" s="35" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="M8" s="35" t="s">
         <v>120</v>
@@ -38400,7 +38400,7 @@
         <v>6</v>
       </c>
       <c r="E10" s="34" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="F10" s="34" t="s">
         <v>356</v>
@@ -38486,7 +38486,7 @@
         <v>14</v>
       </c>
       <c r="K12" s="34" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="L12" s="35" t="s">
         <v>71</v>
@@ -38522,7 +38522,7 @@
         <v>14</v>
       </c>
       <c r="K13" s="34" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="L13" s="35" t="s">
         <v>134</v>
@@ -38558,7 +38558,7 @@
         <v>14</v>
       </c>
       <c r="K14" s="34" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="L14" s="35" t="s">
         <v>684</v>
@@ -38576,7 +38576,7 @@
         <v>11</v>
       </c>
       <c r="E15" s="34" t="s">
-        <v>1186</v>
+        <v>1185</v>
       </c>
       <c r="F15" s="34" t="s">
         <v>449</v>
@@ -38593,10 +38593,10 @@
       <c r="J15" s="34"/>
       <c r="K15" s="34"/>
       <c r="L15" s="35" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="M15" s="35" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="N15" s="90"/>
     </row>
@@ -38608,7 +38608,7 @@
         <v>12</v>
       </c>
       <c r="E16" s="34" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="F16" s="34" t="s">
         <v>450</v>
@@ -38625,10 +38625,10 @@
       <c r="J16" s="34"/>
       <c r="K16" s="34"/>
       <c r="L16" s="35" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="M16" s="35" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="N16" s="90"/>
     </row>
@@ -38640,7 +38640,7 @@
         <v>13</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>1188</v>
+        <v>1187</v>
       </c>
       <c r="F17" s="34" t="s">
         <v>451</v>
@@ -38657,10 +38657,10 @@
       <c r="J17" s="34"/>
       <c r="K17" s="34"/>
       <c r="L17" s="35" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="M17" s="35" t="s">
-        <v>1273</v>
+        <v>1272</v>
       </c>
       <c r="N17" s="90"/>
     </row>
@@ -38672,7 +38672,7 @@
         <v>14</v>
       </c>
       <c r="E18" s="34" t="s">
-        <v>1189</v>
+        <v>1188</v>
       </c>
       <c r="F18" s="34" t="s">
         <v>452</v>
@@ -38689,10 +38689,10 @@
       <c r="J18" s="34"/>
       <c r="K18" s="34"/>
       <c r="L18" s="35" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="M18" s="35" t="s">
-        <v>1274</v>
+        <v>1273</v>
       </c>
       <c r="N18" s="90"/>
     </row>
@@ -38721,10 +38721,10 @@
       <c r="J19" s="34"/>
       <c r="K19" s="34"/>
       <c r="L19" s="35" t="s">
+        <v>1274</v>
+      </c>
+      <c r="M19" s="35" t="s">
         <v>1275</v>
-      </c>
-      <c r="M19" s="35" t="s">
-        <v>1276</v>
       </c>
       <c r="N19" s="90"/>
     </row>
@@ -38733,16 +38733,16 @@
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="D20" s="56" t="s">
+        <v>1096</v>
+      </c>
+      <c r="E20" s="34" t="s">
         <v>1097</v>
       </c>
-      <c r="E20" s="34" t="s">
+      <c r="F20" s="34" t="s">
         <v>1098</v>
       </c>
-      <c r="F20" s="34" t="s">
+      <c r="G20" s="34" t="s">
         <v>1099</v>
-      </c>
-      <c r="G20" s="34" t="s">
-        <v>1100</v>
       </c>
       <c r="H20" s="34" t="s">
         <v>10</v>
@@ -38754,13 +38754,13 @@
         <v>14</v>
       </c>
       <c r="K20" s="34" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="L20" s="35" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="M20" s="35" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="N20" s="90"/>
     </row>
@@ -38769,16 +38769,16 @@
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="56" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="E21" s="34" t="s">
+        <v>1101</v>
+      </c>
+      <c r="F21" s="34" t="s">
         <v>1102</v>
       </c>
-      <c r="F21" s="34" t="s">
+      <c r="G21" s="34" t="s">
         <v>1103</v>
-      </c>
-      <c r="G21" s="34" t="s">
-        <v>1104</v>
       </c>
       <c r="H21" s="34" t="s">
         <v>13</v>
@@ -38789,10 +38789,10 @@
       <c r="J21" s="34"/>
       <c r="K21" s="34"/>
       <c r="L21" s="35" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="M21" s="35" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="N21" s="90"/>
     </row>
@@ -38932,7 +38932,7 @@
         <v>20</v>
       </c>
       <c r="E26" s="34" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="F26" s="34" t="s">
         <v>863</v>
@@ -38950,7 +38950,7 @@
         <v>14</v>
       </c>
       <c r="K26" s="34" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="L26" s="35" t="s">
         <v>865</v>
@@ -38986,7 +38986,7 @@
         <v>14</v>
       </c>
       <c r="K27" s="34" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="L27" s="35" t="s">
         <v>869</v>
@@ -39022,10 +39022,10 @@
         <v>14</v>
       </c>
       <c r="K28" s="34" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="L28" s="35" t="s">
-        <v>1066</v>
+        <v>1065</v>
       </c>
       <c r="M28" s="35" t="s">
         <v>139</v>
@@ -39058,13 +39058,13 @@
         <v>14</v>
       </c>
       <c r="K29" s="34" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="L29" s="35" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="M29" s="35" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="N29" s="90"/>
     </row>
@@ -39094,13 +39094,13 @@
         <v>14</v>
       </c>
       <c r="K30" s="34" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="L30" s="35" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="M30" s="35" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="N30" s="90"/>
     </row>
@@ -39112,7 +39112,7 @@
         <v>25</v>
       </c>
       <c r="E31" s="34" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="F31" s="34" t="s">
         <v>466</v>
@@ -39129,7 +39129,7 @@
       <c r="J31" s="34"/>
       <c r="K31" s="34"/>
       <c r="L31" s="35" t="s">
-        <v>1163</v>
+        <v>1162</v>
       </c>
       <c r="M31" s="35" t="s">
         <v>140</v>
@@ -39144,7 +39144,7 @@
         <v>26</v>
       </c>
       <c r="E32" s="34" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="F32" s="34" t="s">
         <v>468</v>
@@ -39194,10 +39194,10 @@
         <v>14</v>
       </c>
       <c r="K33" s="34" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="L33" s="35" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="M33" s="35" t="s">
         <v>619</v>
@@ -39230,7 +39230,7 @@
         <v>14</v>
       </c>
       <c r="K34" s="34" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="L34" s="35" t="s">
         <v>613</v>
@@ -39266,7 +39266,7 @@
         <v>14</v>
       </c>
       <c r="K35" s="34" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="L35" s="35" t="s">
         <v>614</v>
@@ -39302,7 +39302,7 @@
         <v>14</v>
       </c>
       <c r="K36" s="34" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="L36" s="35" t="s">
         <v>77</v>
@@ -39370,13 +39370,13 @@
         <v>14</v>
       </c>
       <c r="K38" s="34" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="L38" s="35" t="s">
+        <v>1278</v>
+      </c>
+      <c r="M38" s="35" t="s">
         <v>1279</v>
-      </c>
-      <c r="M38" s="35" t="s">
-        <v>1280</v>
       </c>
       <c r="N38" s="90"/>
     </row>
@@ -39438,7 +39438,7 @@
         <v>14</v>
       </c>
       <c r="K40" s="34" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="L40" s="35" t="s">
         <v>95</v>
@@ -39455,13 +39455,13 @@
         <v>35</v>
       </c>
       <c r="E41" s="34" t="s">
+        <v>1280</v>
+      </c>
+      <c r="F41" s="34" t="s">
         <v>1281</v>
       </c>
-      <c r="F41" s="34" t="s">
+      <c r="G41" s="34" t="s">
         <v>1282</v>
-      </c>
-      <c r="G41" s="34" t="s">
-        <v>1283</v>
       </c>
       <c r="H41" s="34" t="s">
         <v>10</v>
@@ -39473,13 +39473,13 @@
         <v>14</v>
       </c>
       <c r="K41" s="34" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="L41" s="35" t="s">
-        <v>1227</v>
+        <v>1226</v>
       </c>
       <c r="M41" s="35" t="s">
-        <v>1119</v>
+        <v>1118</v>
       </c>
       <c r="N41" s="98"/>
     </row>
@@ -39488,16 +39488,16 @@
       <c r="B42" s="15"/>
       <c r="C42" s="15"/>
       <c r="D42" s="56" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="E42" s="34" t="s">
-        <v>1113</v>
+        <v>1112</v>
       </c>
       <c r="F42" s="34" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="G42" s="34" t="s">
-        <v>1116</v>
+        <v>1115</v>
       </c>
       <c r="H42" s="34" t="s">
         <v>10</v>
@@ -39509,13 +39509,13 @@
         <v>14</v>
       </c>
       <c r="K42" s="34" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="L42" s="35" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="M42" s="35" t="s">
-        <v>1110</v>
+        <v>1109</v>
       </c>
       <c r="N42" s="97"/>
     </row>
@@ -39524,16 +39524,16 @@
       <c r="B43" s="15"/>
       <c r="C43" s="15"/>
       <c r="D43" s="56" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="E43" s="34" t="s">
-        <v>1114</v>
+        <v>1113</v>
       </c>
       <c r="F43" s="34" t="s">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="G43" s="34" t="s">
-        <v>1117</v>
+        <v>1116</v>
       </c>
       <c r="H43" s="34" t="s">
         <v>10</v>
@@ -39545,13 +39545,13 @@
         <v>14</v>
       </c>
       <c r="K43" s="34" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="L43" s="35" t="s">
-        <v>1226</v>
+        <v>1225</v>
       </c>
       <c r="M43" s="35" t="s">
-        <v>1120</v>
+        <v>1119</v>
       </c>
       <c r="N43" s="98"/>
     </row>
@@ -39560,16 +39560,16 @@
       <c r="B44" s="15"/>
       <c r="C44" s="15"/>
       <c r="D44" s="56" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="E44" s="34" t="s">
-        <v>1115</v>
+        <v>1114</v>
       </c>
       <c r="F44" s="34" t="s">
-        <v>1112</v>
+        <v>1111</v>
       </c>
       <c r="G44" s="34" t="s">
-        <v>1118</v>
+        <v>1117</v>
       </c>
       <c r="H44" s="34" t="s">
         <v>10</v>
@@ -39581,13 +39581,13 @@
         <v>14</v>
       </c>
       <c r="K44" s="34" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="L44" s="35" t="s">
+        <v>1228</v>
+      </c>
+      <c r="M44" s="35" t="s">
         <v>1229</v>
-      </c>
-      <c r="M44" s="35" t="s">
-        <v>1230</v>
       </c>
       <c r="N44" s="97"/>
     </row>
@@ -39628,7 +39628,7 @@
         <v>37</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="F46" s="12" t="s">
         <v>567</v>
@@ -39646,7 +39646,7 @@
         <v>14</v>
       </c>
       <c r="K46" s="15" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="L46" s="12" t="s">
         <v>840</v>
@@ -39663,7 +39663,7 @@
         <v>38</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>1192</v>
+        <v>1191</v>
       </c>
       <c r="F47" s="12" t="s">
         <v>819</v>
@@ -39694,7 +39694,7 @@
         <v>39</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>1193</v>
+        <v>1192</v>
       </c>
       <c r="F48" s="15" t="s">
         <v>773</v>
@@ -39711,7 +39711,7 @@
       <c r="J48" s="15"/>
       <c r="K48" s="15"/>
       <c r="L48" s="12" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="M48" s="12" t="s">
         <v>1002</v>
@@ -39805,7 +39805,7 @@
         <v>14</v>
       </c>
       <c r="K51" s="15" t="s">
-        <v>1020</v>
+        <v>1303</v>
       </c>
       <c r="L51" s="12" t="s">
         <v>138</v>
@@ -39853,7 +39853,7 @@
         <v>44</v>
       </c>
       <c r="E53" s="15" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="F53" s="15" t="s">
         <v>332</v>
@@ -39869,7 +39869,7 @@
         <v>14</v>
       </c>
       <c r="K53" s="15" t="s">
-        <v>1020</v>
+        <v>1303</v>
       </c>
       <c r="L53" s="12" t="s">
         <v>524</v>
@@ -39886,7 +39886,7 @@
         <v>45</v>
       </c>
       <c r="E54" s="15" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="F54" s="15" t="s">
         <v>820</v>
@@ -39917,7 +39917,7 @@
         <v>46</v>
       </c>
       <c r="E55" s="15" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="F55" s="15" t="s">
         <v>774</v>
@@ -40060,7 +40060,7 @@
         <v>14</v>
       </c>
       <c r="K59" s="15" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="L59" s="12" t="s">
         <v>255</v>
@@ -40189,7 +40189,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
@@ -40406,10 +40406,10 @@
         <v>1015</v>
       </c>
       <c r="L6" s="35" t="s">
+        <v>1094</v>
+      </c>
+      <c r="M6" s="35" t="s">
         <v>1095</v>
-      </c>
-      <c r="M6" s="35" t="s">
-        <v>1096</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="24" x14ac:dyDescent="0.45">
@@ -40422,7 +40422,7 @@
         <v>4</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>1244</v>
+        <v>1243</v>
       </c>
       <c r="F7" s="34" t="s">
         <v>628</v>
@@ -40440,7 +40440,7 @@
         <v>632</v>
       </c>
       <c r="K7" s="34" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="L7" s="59" t="s">
         <v>631</v>
@@ -40461,13 +40461,13 @@
         <v>5</v>
       </c>
       <c r="E8" s="35" t="s">
-        <v>1242</v>
+        <v>1241</v>
       </c>
       <c r="F8" s="34" t="s">
+        <v>1239</v>
+      </c>
+      <c r="G8" s="34" t="s">
         <v>1240</v>
-      </c>
-      <c r="G8" s="34" t="s">
-        <v>1241</v>
       </c>
       <c r="H8" s="34" t="s">
         <v>10</v>
@@ -40493,7 +40493,7 @@
         <v>6</v>
       </c>
       <c r="E9" s="34" t="s">
-        <v>1243</v>
+        <v>1242</v>
       </c>
       <c r="F9" s="34" t="s">
         <v>432</v>
@@ -40511,7 +40511,7 @@
         <v>14</v>
       </c>
       <c r="K9" s="102" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="L9" s="35" t="s">
         <v>151</v>
@@ -40594,7 +40594,7 @@
         <v>9</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="F12" s="35" t="s">
         <v>756</v>
@@ -40611,7 +40611,7 @@
       <c r="J12" s="34"/>
       <c r="K12" s="34"/>
       <c r="L12" s="35" t="s">
-        <v>1261</v>
+        <v>1260</v>
       </c>
       <c r="M12" s="35" t="s">
         <v>120</v>
@@ -40660,7 +40660,7 @@
         <v>11</v>
       </c>
       <c r="E14" s="34" t="s">
-        <v>1174</v>
+        <v>1173</v>
       </c>
       <c r="F14" s="34" t="s">
         <v>359</v>
@@ -40761,7 +40761,7 @@
         <v>14</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
       <c r="F17" s="34" t="s">
         <v>430</v>
@@ -40792,7 +40792,7 @@
         <v>15</v>
       </c>
       <c r="E18" s="34" t="s">
-        <v>1197</v>
+        <v>1196</v>
       </c>
       <c r="F18" s="35" t="s">
         <v>821</v>
@@ -40823,7 +40823,7 @@
         <v>16</v>
       </c>
       <c r="E19" s="34" t="s">
-        <v>1198</v>
+        <v>1197</v>
       </c>
       <c r="F19" s="34" t="s">
         <v>775</v>
@@ -40934,7 +40934,7 @@
         <v>14</v>
       </c>
       <c r="K22" s="34" t="s">
-        <v>1020</v>
+        <v>1303</v>
       </c>
       <c r="L22" s="35" t="s">
         <v>150</v>
@@ -40982,7 +40982,7 @@
         <v>21</v>
       </c>
       <c r="E24" s="34" t="s">
-        <v>1170</v>
+        <v>1169</v>
       </c>
       <c r="F24" s="34" t="s">
         <v>336</v>
@@ -41000,7 +41000,7 @@
         <v>14</v>
       </c>
       <c r="K24" s="34" t="s">
-        <v>1020</v>
+        <v>1303</v>
       </c>
       <c r="L24" s="35" t="s">
         <v>524</v>
@@ -41017,7 +41017,7 @@
         <v>22</v>
       </c>
       <c r="E25" s="34" t="s">
-        <v>1171</v>
+        <v>1170</v>
       </c>
       <c r="F25" s="34" t="s">
         <v>822</v>
@@ -41048,7 +41048,7 @@
         <v>23</v>
       </c>
       <c r="E26" s="34" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="F26" s="34" t="s">
         <v>776</v>
@@ -41160,7 +41160,7 @@
         <v>1015</v>
       </c>
       <c r="L29" s="35" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="M29" s="34"/>
     </row>
@@ -41190,7 +41190,7 @@
         <v>14</v>
       </c>
       <c r="K30" s="34" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="L30" s="35" t="s">
         <v>255</v>
@@ -41210,27 +41210,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
-    <TaxCatchAllLabel xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
-    <TaxKeywordTaxHTField xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100584B29A9F606E64BBE0B94B46ABEDBD5" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ad12f995843361ff338b3798f1f5f41c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4d5313c0-c1e6-4122-afa9-da1ccdba405d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8fda66a02b6b5d1f39f2000ab0f58af4" ns2:_="">
     <xsd:import namespace="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
@@ -41402,31 +41381,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60949D59-0B5B-44ED-ACEF-9231A5F5D889}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
+    <TaxCatchAllLabel xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
+    <TaxKeywordTaxHTField xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04CD8B6C-25F0-471A-A724-387AC1B5060F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F67F35D-1CDD-4110-B6CE-1A6865489AEE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -41442,4 +41418,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60949D59-0B5B-44ED-ACEF-9231A5F5D889}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04CD8B6C-25F0-471A-A724-387AC1B5060F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Changed fields are marked yellow
Changed fields are marked yellow.
</commit_message>
<xml_diff>
--- a/Documents/RDBES Data Model.xlsx
+++ b/Documents/RDBES Data Model.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profile\Henrik K\Documents\GitHub\RDBES_Core_Group\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profile\Henrik K\Documents\GitHub\RDBESpublic\RDBES\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72F1B5C4-C717-4170-8BE8-3CA106829E24}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A36D17-8D4E-435F-8BD0-AFBFD4634A05}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="435" windowWidth="17430" windowHeight="5595" tabRatio="781" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4398,7 +4398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -4596,6 +4596,14 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -9135,7 +9143,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:XFC62"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
+    <sheetView topLeftCell="A29" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K48" activeCellId="1" sqref="K46 K48"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -10063,7 +10073,7 @@
       </c>
       <c r="N26" s="51"/>
     </row>
-    <row r="27" spans="1:14" ht="24" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:14" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A27" s="12"/>
       <c r="B27" s="12"/>
       <c r="C27" s="35"/>
@@ -10740,7 +10750,7 @@
       <c r="J46" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="K46" s="34" t="s">
+      <c r="K46" s="106" t="s">
         <v>1303</v>
       </c>
       <c r="L46" s="35" t="s">
@@ -10808,7 +10818,7 @@
       <c r="J48" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="K48" s="34" t="s">
+      <c r="K48" s="106" t="s">
         <v>1303</v>
       </c>
       <c r="L48" s="35" t="s">
@@ -10819,7 +10829,7 @@
       </c>
       <c r="N48" s="51"/>
     </row>
-    <row r="49" spans="1:16383" ht="24" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:16383" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A49" s="12"/>
       <c r="B49" s="12"/>
       <c r="C49" s="35"/>
@@ -27540,8 +27550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K27" activeCellId="1" sqref="K25 K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -28435,7 +28445,7 @@
       <c r="J25" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="K25" s="15" t="s">
+      <c r="K25" s="108" t="s">
         <v>1303</v>
       </c>
       <c r="L25" s="35" t="s">
@@ -28505,7 +28515,7 @@
       <c r="J27" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="K27" s="15" t="s">
+      <c r="K27" s="108" t="s">
         <v>1303</v>
       </c>
       <c r="L27" s="35" t="s">
@@ -28848,8 +28858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:V61"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -29842,7 +29852,7 @@
       <c r="U23" s="51"/>
       <c r="V23" s="51"/>
     </row>
-    <row r="24" spans="1:22" s="23" customFormat="1" ht="82.15" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:22" s="23" customFormat="1" ht="93.75" x14ac:dyDescent="0.45">
       <c r="A24" s="12"/>
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
@@ -30142,7 +30152,7 @@
       <c r="U30" s="51"/>
       <c r="V30" s="51"/>
     </row>
-    <row r="31" spans="1:22" ht="35.65" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:22" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A31" s="12"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
@@ -30451,7 +30461,7 @@
       <c r="J38" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="K38" s="11" t="s">
+      <c r="K38" s="110" t="s">
         <v>1303</v>
       </c>
       <c r="L38" s="12" t="s">
@@ -30799,7 +30809,7 @@
       <c r="U46" s="51"/>
       <c r="V46" s="51"/>
     </row>
-    <row r="47" spans="1:22" ht="24" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:22" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A47" s="12"/>
       <c r="B47" s="11"/>
       <c r="C47" s="11"/>
@@ -31691,7 +31701,7 @@
       </c>
       <c r="M14" s="35"/>
     </row>
-    <row r="15" spans="1:22" ht="24" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:22" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A15" s="52"/>
       <c r="B15" s="52"/>
       <c r="C15" s="52"/>
@@ -31799,7 +31809,7 @@
   <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -32661,7 +32671,7 @@
       <c r="J25" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="K25" s="15" t="s">
+      <c r="K25" s="108" t="s">
         <v>1303</v>
       </c>
       <c r="L25" s="35" t="s">
@@ -33725,7 +33735,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -34338,7 +34348,7 @@
       <c r="J18" s="54" t="s">
         <v>14</v>
       </c>
-      <c r="K18" s="35" t="s">
+      <c r="K18" s="107" t="s">
         <v>1303</v>
       </c>
       <c r="L18" s="54" t="s">
@@ -34404,7 +34414,7 @@
       <c r="J20" s="57" t="s">
         <v>14</v>
       </c>
-      <c r="K20" s="35" t="s">
+      <c r="K20" s="107" t="s">
         <v>1303</v>
       </c>
       <c r="L20" s="57" t="s">
@@ -34635,7 +34645,7 @@
   <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="K20" activeCellId="1" sqref="K18 K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -35244,7 +35254,7 @@
       <c r="J18" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="K18" s="35" t="s">
+      <c r="K18" s="107" t="s">
         <v>1303</v>
       </c>
       <c r="L18" s="35" t="s">
@@ -35310,7 +35320,7 @@
       <c r="J20" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="K20" s="35" t="s">
+      <c r="K20" s="107" t="s">
         <v>1303</v>
       </c>
       <c r="L20" s="35" t="s">
@@ -35818,7 +35828,7 @@
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+      <selection activeCell="K20" activeCellId="1" sqref="K18 K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -36437,7 +36447,7 @@
       <c r="J18" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="K18" s="15" t="s">
+      <c r="K18" s="108" t="s">
         <v>1303</v>
       </c>
       <c r="L18" s="12" t="s">
@@ -36503,7 +36513,7 @@
       <c r="J20" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="K20" s="15" t="s">
+      <c r="K20" s="108" t="s">
         <v>1303</v>
       </c>
       <c r="L20" s="12" t="s">
@@ -36735,8 +36745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView topLeftCell="C7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K31" activeCellId="1" sqref="K29 K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -37713,7 +37723,7 @@
       <c r="J29" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="K29" s="12" t="s">
+      <c r="K29" s="109" t="s">
         <v>1303</v>
       </c>
       <c r="L29" s="35" t="s">
@@ -37777,7 +37787,7 @@
       <c r="J31" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="K31" s="12" t="s">
+      <c r="K31" s="109" t="s">
         <v>1303</v>
       </c>
       <c r="L31" s="35" t="s">
@@ -38055,8 +38065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F46" sqref="F46"/>
+    <sheetView topLeftCell="A35" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K51" activeCellId="1" sqref="K53 K51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -39804,7 +39814,7 @@
       <c r="J51" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="K51" s="15" t="s">
+      <c r="K51" s="108" t="s">
         <v>1303</v>
       </c>
       <c r="L51" s="12" t="s">
@@ -39868,7 +39878,7 @@
       <c r="J53" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="K53" s="15" t="s">
+      <c r="K53" s="108" t="s">
         <v>1303</v>
       </c>
       <c r="L53" s="12" t="s">
@@ -40189,8 +40199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K24" activeCellId="1" sqref="K22 K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -40933,7 +40943,7 @@
       <c r="J22" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="K22" s="34" t="s">
+      <c r="K22" s="106" t="s">
         <v>1303</v>
       </c>
       <c r="L22" s="35" t="s">
@@ -40999,7 +41009,7 @@
       <c r="J24" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="K24" s="34" t="s">
+      <c r="K24" s="106" t="s">
         <v>1303</v>
       </c>
       <c r="L24" s="35" t="s">
@@ -41210,6 +41220,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
+    <TaxCatchAllLabel xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
+    <TaxKeywordTaxHTField xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100584B29A9F606E64BBE0B94B46ABEDBD5" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ad12f995843361ff338b3798f1f5f41c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4d5313c0-c1e6-4122-afa9-da1ccdba405d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8fda66a02b6b5d1f39f2000ab0f58af4" ns2:_="">
     <xsd:import namespace="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
@@ -41381,41 +41412,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
-    <TaxCatchAllLabel xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
-    <TaxKeywordTaxHTField xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F67F35D-1CDD-4110-B6CE-1A6865489AEE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04CD8B6C-25F0-471A-A724-387AC1B5060F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -41437,9 +41437,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04CD8B6C-25F0-471A-A724-387AC1B5060F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F67F35D-1CDD-4110-B6CE-1A6865489AEE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Changes and updates of specially code types, see the yellow marks. Ver 1.19.3
Changes and updates of specially code types, see the yellow marks. Ver 1.19.3
</commit_message>
<xml_diff>
--- a/Documents/RDBES Data Model.xlsx
+++ b/Documents/RDBES Data Model.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20375"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20376"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profile\Henrik K\Documents\GitHub\RDBESpublic\RDBES\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profile\Henrik K\Documents\GitHub\RDBES_Core_Group\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20A36D17-8D4E-435F-8BD0-AFBFD4634A05}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{621ADA0C-6EAA-4B1A-94B6-119EA333811E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="17430" windowHeight="5595" tabRatio="781" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="17430" windowHeight="5595" tabRatio="781" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Model v1.19.2" sheetId="1" r:id="rId1"/>
+    <sheet name="Model v1.19.3" sheetId="1" r:id="rId1"/>
     <sheet name="Design" sheetId="5" r:id="rId2"/>
     <sheet name="Temporal Event" sheetId="21" r:id="rId3"/>
     <sheet name="Location" sheetId="20" r:id="rId4"/>
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3403" uniqueCount="1304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3403" uniqueCount="1303">
   <si>
     <t>Design Table (DE)</t>
   </si>
@@ -3258,9 +3258,6 @@
     <t>UK1, Uk2</t>
   </si>
   <si>
-    <t>RS_SamplingSchemeType</t>
-  </si>
-  <si>
     <t>YesNoFields</t>
   </si>
   <si>
@@ -3273,12 +3270,6 @@
     <t>RS_Clustering</t>
   </si>
   <si>
-    <t>RS_Sampler</t>
-  </si>
-  <si>
-    <t>RS_ReasonForNotSampling</t>
-  </si>
-  <si>
     <t>Harbour_LOCODE</t>
   </si>
   <si>
@@ -3324,63 +3315,39 @@
     <t>GearType</t>
   </si>
   <si>
-    <t>RS_SelectionDevice</t>
-  </si>
-  <si>
     <t>TargetSpecies</t>
   </si>
   <si>
     <t>RS_incidentialByCatchMitigateD</t>
   </si>
   <si>
-    <t>RS_ObservationCode</t>
-  </si>
-  <si>
     <t>RS_LocationType</t>
   </si>
   <si>
     <t>Indicating if the unit was sampled: Y/N. If No no child records are expected.</t>
   </si>
   <si>
-    <t>RS_ObservationActivityType</t>
-  </si>
-  <si>
     <t>RS_CatchFraction</t>
   </si>
   <si>
-    <t>RS_ObservationType</t>
-  </si>
-  <si>
     <t>SpecWoRMS</t>
   </si>
   <si>
     <t>SpecASFIS</t>
   </si>
   <si>
-    <t>RS_Presentation</t>
-  </si>
-  <si>
-    <t>RS_SpecimensState</t>
-  </si>
-  <si>
     <t>RS_CatchCategory</t>
   </si>
   <si>
     <t>RS_LandingCategory</t>
   </si>
   <si>
-    <t>RS_CommercialSizeCategoryScale</t>
-  </si>
-  <si>
     <t>RS_CommercialSizeCategory</t>
   </si>
   <si>
     <t>RS_Sex</t>
   </si>
   <si>
-    <t>RS_UnitType</t>
-  </si>
-  <si>
     <t>RS_LowerHierarchy</t>
   </si>
   <si>
@@ -3390,9 +3357,6 @@
     <t>RS_AddGrpMeasurementType</t>
   </si>
   <si>
-    <t>RS_BiologicalMeasurementType</t>
-  </si>
-  <si>
     <t>RS_LEfullTripAvailable</t>
   </si>
   <si>
@@ -3459,9 +3423,6 @@
     <t>BVvalUnitScale</t>
   </si>
   <si>
-    <t>RS_ValueUnitOrScale</t>
-  </si>
-  <si>
     <t xml:space="preserve">The unit or scale of the measured value in the biovarValue, e.g. Year/mm/g/maturity scale/winter rings. </t>
   </si>
   <si>
@@ -3486,9 +3447,6 @@
     <t>BVcertaintyQuali</t>
   </si>
   <si>
-    <t>RS_CertaintyQualitative</t>
-  </si>
-  <si>
     <t>Qualitative measures of certainty e.g. WGBIOP's quality scale for age readability. Use 'Unknown' if not recorded and 'NotApplicable' if this is not reported for this measuremnet e.g. length</t>
   </si>
   <si>
@@ -3574,9 +3532,6 @@
   </si>
   <si>
     <t>Second mitigation device specific for reducing incidental by-catch</t>
-  </si>
-  <si>
-    <t>RS_IncidentalByCatchMitigationDevTarget</t>
   </si>
   <si>
     <t>BVnationalUniqueFishId</t>
@@ -4064,9 +4019,6 @@
   </si>
   <si>
     <t>FOincBycMitigDevFirst</t>
-  </si>
-  <si>
-    <t>RS_IncidentalByCatchMitigationDev</t>
   </si>
   <si>
     <t>The haul number (if there is one) for this LandingEvent record.</t>
@@ -4123,9 +4075,6 @@
     <t>METOA</t>
   </si>
   <si>
-    <t>RS_DurationSource</t>
-  </si>
-  <si>
     <t>SAstateOfProcessing</t>
   </si>
   <si>
@@ -4148,6 +4097,54 @@
   </si>
   <si>
     <t>SelectionMethod</t>
+  </si>
+  <si>
+    <t>BycatchMitigationDevice</t>
+  </si>
+  <si>
+    <t>BycatchMitigationDeviceTarget</t>
+  </si>
+  <si>
+    <t>ObservationCode</t>
+  </si>
+  <si>
+    <t>MeasurementCertainty</t>
+  </si>
+  <si>
+    <t>ObservationMethod</t>
+  </si>
+  <si>
+    <t>SamplingUnit</t>
+  </si>
+  <si>
+    <t>ObservationActivityType</t>
+  </si>
+  <si>
+    <t>StateOfProcessing</t>
+  </si>
+  <si>
+    <t>SelectionDevice</t>
+  </si>
+  <si>
+    <t>DurationSource</t>
+  </si>
+  <si>
+    <t>CommercialSizeCategoryScale</t>
+  </si>
+  <si>
+    <t>ValueUnitOrScale</t>
+  </si>
+  <si>
+    <t>SamplingSchemeType</t>
+  </si>
+  <si>
+    <t>SpecimensState</t>
+  </si>
+  <si>
+    <t>ReasonForNotSampling</t>
+  </si>
+  <si>
+    <t>BiologicalMeasurementType</t>
   </si>
 </sst>
 </file>
@@ -4398,7 +4395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="112">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
@@ -4604,6 +4601,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4958,8 +4956,8 @@
   </sheetPr>
   <dimension ref="A1:AI112"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView showZeros="0" topLeftCell="A7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -5010,7 +5008,7 @@
     </row>
     <row r="2" spans="1:35" ht="21" x14ac:dyDescent="0.65">
       <c r="B2" s="105" t="s">
-        <v>1302</v>
+        <v>1285</v>
       </c>
       <c r="D2" s="19"/>
       <c r="L2" s="17"/>
@@ -9143,8 +9141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:XFC62"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K48" activeCellId="1" sqref="K46 K48"/>
+    <sheetView topLeftCell="A39" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K54" sqref="K54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -9198,7 +9196,7 @@
         <v>7</v>
       </c>
       <c r="K1" s="25" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="L1" s="25" t="s">
         <v>8</v>
@@ -9537,7 +9535,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>1175</v>
+        <v>1160</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>929</v>
@@ -9552,11 +9550,11 @@
         <v>11</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>1061</v>
+        <v>1049</v>
       </c>
       <c r="K11" s="12"/>
       <c r="L11" s="12" t="s">
-        <v>1064</v>
+        <v>1052</v>
       </c>
       <c r="M11" s="12" t="s">
         <v>577</v>
@@ -9589,13 +9587,13 @@
         <v>14</v>
       </c>
       <c r="K12" s="35" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="L12" s="35" t="s">
-        <v>1094</v>
+        <v>1080</v>
       </c>
       <c r="M12" s="35" t="s">
-        <v>1095</v>
+        <v>1081</v>
       </c>
       <c r="N12" s="51"/>
     </row>
@@ -9658,10 +9656,10 @@
       <c r="J14" s="35"/>
       <c r="K14" s="34"/>
       <c r="L14" s="35" t="s">
-        <v>1284</v>
+        <v>1268</v>
       </c>
       <c r="M14" s="35" t="s">
-        <v>1284</v>
+        <v>1268</v>
       </c>
       <c r="N14" s="101"/>
     </row>
@@ -9673,7 +9671,7 @@
         <v>6</v>
       </c>
       <c r="E15" s="35" t="s">
-        <v>1198</v>
+        <v>1183</v>
       </c>
       <c r="F15" s="35" t="s">
         <v>757</v>
@@ -9690,10 +9688,10 @@
       <c r="J15" s="35"/>
       <c r="K15" s="34"/>
       <c r="L15" s="35" t="s">
-        <v>1285</v>
+        <v>1269</v>
       </c>
       <c r="M15" s="35" t="s">
-        <v>1286</v>
+        <v>1270</v>
       </c>
       <c r="N15" s="51"/>
     </row>
@@ -9723,7 +9721,7 @@
         <v>14</v>
       </c>
       <c r="K16" s="34" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="L16" s="35" t="s">
         <v>262</v>
@@ -9741,7 +9739,7 @@
         <v>8</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>1173</v>
+        <v>1158</v>
       </c>
       <c r="F17" s="34" t="s">
         <v>362</v>
@@ -9790,8 +9788,8 @@
       <c r="J18" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="K18" s="34" t="s">
-        <v>1019</v>
+      <c r="K18" s="106" t="s">
+        <v>256</v>
       </c>
       <c r="L18" s="35" t="s">
         <v>829</v>
@@ -9827,7 +9825,7 @@
         <v>14</v>
       </c>
       <c r="K19" s="34" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="L19" s="35" t="s">
         <v>154</v>
@@ -9863,7 +9861,7 @@
         <v>14</v>
       </c>
       <c r="K20" s="34" t="s">
-        <v>1026</v>
+        <v>1023</v>
       </c>
       <c r="L20" s="35" t="s">
         <v>240</v>
@@ -9881,13 +9879,13 @@
         <v>12</v>
       </c>
       <c r="E21" s="35" t="s">
-        <v>1287</v>
+        <v>1271</v>
       </c>
       <c r="F21" s="35" t="s">
-        <v>1231</v>
+        <v>1216</v>
       </c>
       <c r="G21" s="35" t="s">
-        <v>1231</v>
+        <v>1216</v>
       </c>
       <c r="H21" s="35" t="s">
         <v>10</v>
@@ -9897,7 +9895,7 @@
       </c>
       <c r="J21" s="35"/>
       <c r="K21" s="34" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
       <c r="L21" s="35" t="s">
         <v>92</v>
@@ -9911,19 +9909,19 @@
       <c r="A22" s="12"/>
       <c r="B22" s="12"/>
       <c r="C22" s="35" t="s">
-        <v>1096</v>
+        <v>1082</v>
       </c>
       <c r="D22" s="35">
         <v>13</v>
       </c>
       <c r="E22" s="35" t="s">
-        <v>1232</v>
+        <v>1217</v>
       </c>
       <c r="F22" s="35" t="s">
-        <v>1233</v>
+        <v>1218</v>
       </c>
       <c r="G22" s="35" t="s">
-        <v>1238</v>
+        <v>1223</v>
       </c>
       <c r="H22" s="35" t="s">
         <v>10</v>
@@ -9963,7 +9961,7 @@
         <v>14</v>
       </c>
       <c r="K23" s="34" t="s">
-        <v>1040</v>
+        <v>1035</v>
       </c>
       <c r="L23" s="35" t="s">
         <v>78</v>
@@ -10002,7 +10000,7 @@
         <v>1003</v>
       </c>
       <c r="L24" s="35" t="s">
-        <v>1070</v>
+        <v>1058</v>
       </c>
       <c r="M24" s="35" t="s">
         <v>158</v>
@@ -10073,7 +10071,7 @@
       </c>
       <c r="N26" s="51"/>
     </row>
-    <row r="27" spans="1:14" ht="35.65" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:14" ht="24" x14ac:dyDescent="0.45">
       <c r="A27" s="12"/>
       <c r="B27" s="12"/>
       <c r="C27" s="35"/>
@@ -10081,7 +10079,7 @@
         <v>18</v>
       </c>
       <c r="E27" s="35" t="s">
-        <v>1189</v>
+        <v>1174</v>
       </c>
       <c r="F27" s="34" t="s">
         <v>932</v>
@@ -10099,7 +10097,7 @@
         <v>14</v>
       </c>
       <c r="K27" s="34" t="s">
-        <v>1027</v>
+        <v>1024</v>
       </c>
       <c r="L27" s="35" t="s">
         <v>866</v>
@@ -10135,7 +10133,7 @@
         <v>14</v>
       </c>
       <c r="K28" s="34" t="s">
-        <v>1028</v>
+        <v>1025</v>
       </c>
       <c r="L28" s="35" t="s">
         <v>872</v>
@@ -10171,10 +10169,10 @@
         <v>14</v>
       </c>
       <c r="K29" s="34" t="s">
-        <v>1029</v>
+        <v>1026</v>
       </c>
       <c r="L29" s="35" t="s">
-        <v>1071</v>
+        <v>1059</v>
       </c>
       <c r="M29" s="35" t="s">
         <v>162</v>
@@ -10207,13 +10205,13 @@
         <v>14</v>
       </c>
       <c r="K30" s="34" t="s">
-        <v>1030</v>
+        <v>1027</v>
       </c>
       <c r="L30" s="35" t="s">
-        <v>1066</v>
+        <v>1054</v>
       </c>
       <c r="M30" s="35" t="s">
-        <v>1066</v>
+        <v>1054</v>
       </c>
       <c r="N30" s="66"/>
     </row>
@@ -10243,10 +10241,10 @@
         <v>14</v>
       </c>
       <c r="K31" s="34" t="s">
-        <v>1031</v>
+        <v>1028</v>
       </c>
       <c r="L31" s="34" t="s">
-        <v>1072</v>
+        <v>1060</v>
       </c>
       <c r="M31" s="34" t="s">
         <v>846</v>
@@ -10279,10 +10277,10 @@
         <v>14</v>
       </c>
       <c r="K32" s="34" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="L32" s="35" t="s">
-        <v>1073</v>
+        <v>1061</v>
       </c>
       <c r="M32" s="35" t="s">
         <v>612</v>
@@ -10315,7 +10313,7 @@
         <v>14</v>
       </c>
       <c r="K33" s="34" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="L33" s="35" t="s">
         <v>873</v>
@@ -10351,7 +10349,7 @@
         <v>14</v>
       </c>
       <c r="K34" s="34" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
       <c r="L34" s="35" t="s">
         <v>874</v>
@@ -10387,7 +10385,7 @@
         <v>14</v>
       </c>
       <c r="K35" s="34" t="s">
-        <v>1035</v>
+        <v>1032</v>
       </c>
       <c r="L35" s="35" t="s">
         <v>875</v>
@@ -10454,8 +10452,8 @@
       <c r="J37" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="K37" s="34" t="s">
-        <v>1036</v>
+      <c r="K37" s="106" t="s">
+        <v>1295</v>
       </c>
       <c r="L37" s="35" t="s">
         <v>877</v>
@@ -10523,7 +10521,7 @@
         <v>14</v>
       </c>
       <c r="K39" s="34" t="s">
-        <v>1037</v>
+        <v>1033</v>
       </c>
       <c r="L39" s="35" t="s">
         <v>94</v>
@@ -10559,7 +10557,7 @@
         <v>14</v>
       </c>
       <c r="K40" s="34" t="s">
-        <v>1038</v>
+        <v>1034</v>
       </c>
       <c r="L40" s="35" t="s">
         <v>879</v>
@@ -10605,7 +10603,7 @@
         <v>33</v>
       </c>
       <c r="E42" s="35" t="s">
-        <v>1199</v>
+        <v>1184</v>
       </c>
       <c r="F42" s="35" t="s">
         <v>823</v>
@@ -10637,7 +10635,7 @@
         <v>34</v>
       </c>
       <c r="E43" s="35" t="s">
-        <v>1200</v>
+        <v>1185</v>
       </c>
       <c r="F43" s="34" t="s">
         <v>777</v>
@@ -10751,7 +10749,7 @@
         <v>14</v>
       </c>
       <c r="K46" s="106" t="s">
-        <v>1303</v>
+        <v>1286</v>
       </c>
       <c r="L46" s="35" t="s">
         <v>163</v>
@@ -10801,7 +10799,7 @@
         <v>39</v>
       </c>
       <c r="E48" s="34" t="s">
-        <v>1169</v>
+        <v>1154</v>
       </c>
       <c r="F48" s="34" t="s">
         <v>341</v>
@@ -10819,7 +10817,7 @@
         <v>14</v>
       </c>
       <c r="K48" s="106" t="s">
-        <v>1303</v>
+        <v>1286</v>
       </c>
       <c r="L48" s="35" t="s">
         <v>524</v>
@@ -10829,7 +10827,7 @@
       </c>
       <c r="N48" s="51"/>
     </row>
-    <row r="49" spans="1:16383" ht="35.65" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:16383" ht="24" x14ac:dyDescent="0.45">
       <c r="A49" s="12"/>
       <c r="B49" s="12"/>
       <c r="C49" s="35"/>
@@ -10837,7 +10835,7 @@
         <v>40</v>
       </c>
       <c r="E49" s="34" t="s">
-        <v>1170</v>
+        <v>1155</v>
       </c>
       <c r="F49" s="34" t="s">
         <v>824</v>
@@ -10869,7 +10867,7 @@
         <v>41</v>
       </c>
       <c r="E50" s="34" t="s">
-        <v>1171</v>
+        <v>1156</v>
       </c>
       <c r="F50" s="34" t="s">
         <v>778</v>
@@ -10981,7 +10979,7 @@
         <v>14</v>
       </c>
       <c r="K53" s="34" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="L53" s="35" t="s">
         <v>695</v>
@@ -11013,8 +11011,8 @@
       <c r="J54" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="K54" s="34" t="s">
-        <v>1020</v>
+      <c r="K54" s="106" t="s">
+        <v>1301</v>
       </c>
       <c r="L54" s="35" t="s">
         <v>255</v>
@@ -11050,7 +11048,7 @@
         <v>14</v>
       </c>
       <c r="K55" s="34" t="s">
-        <v>1059</v>
+        <v>1047</v>
       </c>
       <c r="L55" s="35" t="s">
         <v>544</v>
@@ -27550,8 +27548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:O40"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K27" activeCellId="1" sqref="K25 K27"/>
+    <sheetView topLeftCell="A19" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -27603,7 +27601,7 @@
         <v>7</v>
       </c>
       <c r="K1" s="25" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="L1" s="25" t="s">
         <v>8</v>
@@ -27952,13 +27950,13 @@
         <v>14</v>
       </c>
       <c r="K11" s="35" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="L11" s="35" t="s">
-        <v>1094</v>
+        <v>1080</v>
       </c>
       <c r="M11" s="35" t="s">
-        <v>1095</v>
+        <v>1081</v>
       </c>
       <c r="N11" s="63"/>
       <c r="O11" s="63"/>
@@ -27973,7 +27971,7 @@
         <v>4</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>1201</v>
+        <v>1186</v>
       </c>
       <c r="F12" s="34" t="s">
         <v>967</v>
@@ -27991,7 +27989,7 @@
         <v>14</v>
       </c>
       <c r="K12" s="34" t="s">
-        <v>1042</v>
+        <v>1293</v>
       </c>
       <c r="L12" s="35" t="s">
         <v>839</v>
@@ -28012,7 +28010,7 @@
         <v>5</v>
       </c>
       <c r="E13" s="56" t="s">
-        <v>1202</v>
+        <v>1187</v>
       </c>
       <c r="F13" s="56" t="s">
         <v>685</v>
@@ -28028,7 +28026,7 @@
       </c>
       <c r="J13" s="49"/>
       <c r="K13" s="34" t="s">
-        <v>1043</v>
+        <v>1037</v>
       </c>
       <c r="L13" s="70" t="s">
         <v>882</v>
@@ -28049,7 +28047,7 @@
         <v>6</v>
       </c>
       <c r="E14" s="56" t="s">
-        <v>1203</v>
+        <v>1188</v>
       </c>
       <c r="F14" s="56" t="s">
         <v>966</v>
@@ -28066,8 +28064,8 @@
       <c r="J14" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="K14" s="34" t="s">
-        <v>1044</v>
+      <c r="K14" s="106" t="s">
+        <v>1291</v>
       </c>
       <c r="L14" s="70" t="s">
         <v>565</v>
@@ -28086,7 +28084,7 @@
         <v>7</v>
       </c>
       <c r="E15" s="49" t="s">
-        <v>1204</v>
+        <v>1189</v>
       </c>
       <c r="F15" s="35" t="s">
         <v>758</v>
@@ -28103,7 +28101,7 @@
       <c r="J15" s="49"/>
       <c r="K15" s="34"/>
       <c r="L15" s="49" t="s">
-        <v>1288</v>
+        <v>1272</v>
       </c>
       <c r="M15" s="35" t="s">
         <v>120</v>
@@ -28137,7 +28135,7 @@
         <v>14</v>
       </c>
       <c r="K16" s="34" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="L16" s="35" t="s">
         <v>262</v>
@@ -28156,7 +28154,7 @@
         <v>9</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>1173</v>
+        <v>1158</v>
       </c>
       <c r="F17" s="34" t="s">
         <v>365</v>
@@ -28206,8 +28204,8 @@
       <c r="J18" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="K18" s="34" t="s">
-        <v>1019</v>
+      <c r="K18" s="106" t="s">
+        <v>256</v>
       </c>
       <c r="L18" s="35" t="s">
         <v>829</v>
@@ -28226,7 +28224,7 @@
         <v>11</v>
       </c>
       <c r="E19" s="49" t="s">
-        <v>1205</v>
+        <v>1190</v>
       </c>
       <c r="F19" s="49" t="s">
         <v>968</v>
@@ -28261,7 +28259,7 @@
         <v>12</v>
       </c>
       <c r="E20" s="49" t="s">
-        <v>1206</v>
+        <v>1191</v>
       </c>
       <c r="F20" s="49" t="s">
         <v>592</v>
@@ -28279,7 +28277,7 @@
         <v>14</v>
       </c>
       <c r="K20" s="15" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="L20" s="49" t="s">
         <v>590</v>
@@ -28296,7 +28294,7 @@
         <v>13</v>
       </c>
       <c r="E21" s="49" t="s">
-        <v>1207</v>
+        <v>1192</v>
       </c>
       <c r="F21" s="35" t="s">
         <v>825</v>
@@ -28329,7 +28327,7 @@
         <v>14</v>
       </c>
       <c r="E22" s="49" t="s">
-        <v>1208</v>
+        <v>1193</v>
       </c>
       <c r="F22" s="34" t="s">
         <v>779</v>
@@ -28428,7 +28426,7 @@
         <v>17</v>
       </c>
       <c r="E25" s="49" t="s">
-        <v>1209</v>
+        <v>1194</v>
       </c>
       <c r="F25" s="56" t="s">
         <v>413</v>
@@ -28446,7 +28444,7 @@
         <v>14</v>
       </c>
       <c r="K25" s="108" t="s">
-        <v>1303</v>
+        <v>1286</v>
       </c>
       <c r="L25" s="35" t="s">
         <v>211</v>
@@ -28498,7 +28496,7 @@
         <v>19</v>
       </c>
       <c r="E27" s="34" t="s">
-        <v>1169</v>
+        <v>1154</v>
       </c>
       <c r="F27" s="34" t="s">
         <v>345</v>
@@ -28516,7 +28514,7 @@
         <v>14</v>
       </c>
       <c r="K27" s="108" t="s">
-        <v>1303</v>
+        <v>1286</v>
       </c>
       <c r="L27" s="35" t="s">
         <v>524</v>
@@ -28535,7 +28533,7 @@
         <v>20</v>
       </c>
       <c r="E28" s="34" t="s">
-        <v>1170</v>
+        <v>1155</v>
       </c>
       <c r="F28" s="34" t="s">
         <v>826</v>
@@ -28568,7 +28566,7 @@
         <v>21</v>
       </c>
       <c r="E29" s="34" t="s">
-        <v>1171</v>
+        <v>1156</v>
       </c>
       <c r="F29" s="34" t="s">
         <v>780</v>
@@ -28683,7 +28681,7 @@
         <v>14</v>
       </c>
       <c r="K32" s="15" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="L32" s="35" t="s">
         <v>695</v>
@@ -28715,8 +28713,8 @@
       <c r="J33" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="K33" s="15" t="s">
-        <v>1020</v>
+      <c r="K33" s="108" t="s">
+        <v>1301</v>
       </c>
       <c r="L33" s="35" t="s">
         <v>255</v>
@@ -28858,8 +28856,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:V61"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K44" sqref="K44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -28873,7 +28871,7 @@
     <col min="8" max="8" width="7.3984375" style="2" customWidth="1"/>
     <col min="9" max="9" width="11.3984375" style="2" customWidth="1"/>
     <col min="10" max="10" width="9.1328125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19" style="41" customWidth="1"/>
+    <col min="11" max="11" width="25.796875" style="41" customWidth="1"/>
     <col min="12" max="12" width="55.265625" style="2" customWidth="1"/>
     <col min="13" max="13" width="40.73046875" style="2" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="9.1328125" style="2"/>
@@ -28911,7 +28909,7 @@
         <v>7</v>
       </c>
       <c r="K1" s="40" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="L1" s="40" t="s">
         <v>8</v>
@@ -29080,7 +29078,7 @@
         <v>3</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>1210</v>
+        <v>1195</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>673</v>
@@ -29138,13 +29136,13 @@
         <v>14</v>
       </c>
       <c r="K7" s="35" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="L7" s="35" t="s">
-        <v>1094</v>
+        <v>1080</v>
       </c>
       <c r="M7" s="35" t="s">
-        <v>1095</v>
+        <v>1081</v>
       </c>
       <c r="N7" s="51"/>
       <c r="O7" s="60"/>
@@ -29181,7 +29179,7 @@
       <c r="J8" s="56"/>
       <c r="K8" s="56"/>
       <c r="L8" s="35" t="s">
-        <v>1292</v>
+        <v>1276</v>
       </c>
       <c r="M8" s="35" t="s">
         <v>98</v>
@@ -29224,7 +29222,7 @@
         <v>14</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>1045</v>
+        <v>1038</v>
       </c>
       <c r="L9" s="12" t="s">
         <v>584</v>
@@ -29270,7 +29268,7 @@
         <v>14</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>1046</v>
+        <v>1039</v>
       </c>
       <c r="L10" s="12" t="s">
         <v>997</v>
@@ -29291,18 +29289,18 @@
     <row r="11" spans="1:22" s="51" customFormat="1" ht="24" x14ac:dyDescent="0.45">
       <c r="A11" s="35"/>
       <c r="B11" s="56" t="s">
-        <v>1096</v>
+        <v>1082</v>
       </c>
       <c r="C11" s="56"/>
       <c r="D11" s="52"/>
       <c r="E11" s="56" t="s">
-        <v>1126</v>
+        <v>1111</v>
       </c>
       <c r="F11" s="56" t="s">
-        <v>1296</v>
+        <v>1279</v>
       </c>
       <c r="G11" s="56" t="s">
-        <v>1297</v>
+        <v>1280</v>
       </c>
       <c r="H11" s="56" t="s">
         <v>10</v>
@@ -29313,11 +29311,11 @@
       <c r="J11" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="K11" s="56" t="s">
-        <v>1291</v>
+      <c r="K11" s="111" t="s">
+        <v>1294</v>
       </c>
       <c r="L11" s="35" t="s">
-        <v>1128</v>
+        <v>1113</v>
       </c>
       <c r="M11" s="35"/>
     </row>
@@ -29348,11 +29346,11 @@
       <c r="J12" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="K12" s="56" t="s">
-        <v>1047</v>
+      <c r="K12" s="111" t="s">
+        <v>22</v>
       </c>
       <c r="L12" s="35" t="s">
-        <v>1130</v>
+        <v>1115</v>
       </c>
       <c r="M12" s="35" t="s">
         <v>171</v>
@@ -29366,7 +29364,7 @@
         <v>9</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>1211</v>
+        <v>1196</v>
       </c>
       <c r="F13" s="11" t="s">
         <v>560</v>
@@ -29383,8 +29381,8 @@
       <c r="J13" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="K13" s="11" t="s">
-        <v>1048</v>
+      <c r="K13" s="110" t="s">
+        <v>1300</v>
       </c>
       <c r="L13" s="87" t="s">
         <v>884</v>
@@ -29412,7 +29410,7 @@
         <v>10</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>1212</v>
+        <v>1197</v>
       </c>
       <c r="F14" s="11" t="s">
         <v>548</v>
@@ -29430,7 +29428,7 @@
         <v>14</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>1049</v>
+        <v>1040</v>
       </c>
       <c r="L14" s="87" t="s">
         <v>697</v>
@@ -29476,7 +29474,7 @@
         <v>14</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>1050</v>
+        <v>1041</v>
       </c>
       <c r="L15" s="12" t="s">
         <v>835</v>
@@ -29521,8 +29519,8 @@
       <c r="J16" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="K16" s="11" t="s">
-        <v>1051</v>
+      <c r="K16" s="110" t="s">
+        <v>1297</v>
       </c>
       <c r="L16" s="12" t="s">
         <v>173</v>
@@ -29568,7 +29566,7 @@
         <v>14</v>
       </c>
       <c r="K17" s="11" t="s">
-        <v>1052</v>
+        <v>1042</v>
       </c>
       <c r="L17" s="12" t="s">
         <v>19</v>
@@ -29614,10 +29612,10 @@
         <v>14</v>
       </c>
       <c r="K18" s="11" t="s">
-        <v>1053</v>
+        <v>1043</v>
       </c>
       <c r="L18" s="12" t="s">
-        <v>1074</v>
+        <v>1062</v>
       </c>
       <c r="M18" s="12" t="s">
         <v>20</v>
@@ -29640,7 +29638,7 @@
         <v>15</v>
       </c>
       <c r="E19" s="95" t="s">
-        <v>1189</v>
+        <v>1174</v>
       </c>
       <c r="F19" s="95" t="s">
         <v>861</v>
@@ -29658,7 +29656,7 @@
         <v>14</v>
       </c>
       <c r="K19" s="11" t="s">
-        <v>1027</v>
+        <v>1024</v>
       </c>
       <c r="L19" s="96" t="s">
         <v>836</v>
@@ -29702,7 +29700,7 @@
         <v>14</v>
       </c>
       <c r="K20" s="11" t="s">
-        <v>1028</v>
+        <v>1025</v>
       </c>
       <c r="L20" s="12" t="s">
         <v>713</v>
@@ -29746,10 +29744,10 @@
         <v>14</v>
       </c>
       <c r="K21" s="11" t="s">
-        <v>1029</v>
+        <v>1026</v>
       </c>
       <c r="L21" s="12" t="s">
-        <v>1075</v>
+        <v>1063</v>
       </c>
       <c r="M21" s="12" t="s">
         <v>162</v>
@@ -29790,13 +29788,13 @@
         <v>14</v>
       </c>
       <c r="K22" s="11" t="s">
-        <v>1030</v>
+        <v>1027</v>
       </c>
       <c r="L22" s="12" t="s">
-        <v>1066</v>
+        <v>1054</v>
       </c>
       <c r="M22" s="12" t="s">
-        <v>1066</v>
+        <v>1054</v>
       </c>
       <c r="N22" s="51"/>
       <c r="O22" s="51"/>
@@ -29834,10 +29832,10 @@
         <v>14</v>
       </c>
       <c r="K23" s="11" t="s">
-        <v>1031</v>
+        <v>1028</v>
       </c>
       <c r="L23" s="12" t="s">
-        <v>1067</v>
+        <v>1055</v>
       </c>
       <c r="M23" s="12" t="s">
         <v>846</v>
@@ -29852,7 +29850,7 @@
       <c r="U23" s="51"/>
       <c r="V23" s="51"/>
     </row>
-    <row r="24" spans="1:22" s="23" customFormat="1" ht="93.75" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:22" s="23" customFormat="1" ht="82.15" x14ac:dyDescent="0.45">
       <c r="A24" s="12"/>
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
@@ -29878,10 +29876,10 @@
         <v>14</v>
       </c>
       <c r="K24" s="11" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="L24" s="12" t="s">
-        <v>1076</v>
+        <v>1064</v>
       </c>
       <c r="M24" s="12" t="s">
         <v>612</v>
@@ -29922,7 +29920,7 @@
         <v>14</v>
       </c>
       <c r="K25" s="11" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="L25" s="12" t="s">
         <v>714</v>
@@ -29966,7 +29964,7 @@
         <v>14</v>
       </c>
       <c r="K26" s="11" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
       <c r="L26" s="12" t="s">
         <v>715</v>
@@ -30010,7 +30008,7 @@
         <v>14</v>
       </c>
       <c r="K27" s="11" t="s">
-        <v>1035</v>
+        <v>1032</v>
       </c>
       <c r="L27" s="12" t="s">
         <v>716</v>
@@ -30093,8 +30091,8 @@
       <c r="J29" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="K29" s="11" t="s">
-        <v>1036</v>
+      <c r="K29" s="110" t="s">
+        <v>1295</v>
       </c>
       <c r="L29" s="12" t="s">
         <v>718</v>
@@ -30152,7 +30150,7 @@
       <c r="U30" s="51"/>
       <c r="V30" s="51"/>
     </row>
-    <row r="31" spans="1:22" ht="47.25" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:22" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A31" s="12"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
@@ -30177,8 +30175,8 @@
       <c r="J31" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="K31" s="11" t="s">
-        <v>1054</v>
+      <c r="K31" s="110" t="s">
+        <v>1292</v>
       </c>
       <c r="L31" s="12" t="s">
         <v>683</v>
@@ -30204,7 +30202,7 @@
         <v>28</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>1213</v>
+        <v>1198</v>
       </c>
       <c r="F32" s="11" t="s">
         <v>538</v>
@@ -30221,7 +30219,7 @@
       <c r="J32" s="11"/>
       <c r="K32" s="11"/>
       <c r="L32" s="12" t="s">
-        <v>1077</v>
+        <v>1065</v>
       </c>
       <c r="M32" s="12" t="s">
         <v>176</v>
@@ -30244,7 +30242,7 @@
         <v>29</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>1216</v>
+        <v>1201</v>
       </c>
       <c r="F33" s="11" t="s">
         <v>537</v>
@@ -30261,7 +30259,7 @@
       <c r="J33" s="11"/>
       <c r="K33" s="11"/>
       <c r="L33" s="12" t="s">
-        <v>1078</v>
+        <v>1066</v>
       </c>
       <c r="M33" s="12" t="s">
         <v>177</v>
@@ -30284,7 +30282,7 @@
         <v>30</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>1214</v>
+        <v>1199</v>
       </c>
       <c r="F34" s="12" t="s">
         <v>827</v>
@@ -30324,7 +30322,7 @@
         <v>31</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>1215</v>
+        <v>1200</v>
       </c>
       <c r="F35" s="15" t="s">
         <v>781</v>
@@ -30462,7 +30460,7 @@
         <v>14</v>
       </c>
       <c r="K38" s="110" t="s">
-        <v>1303</v>
+        <v>1286</v>
       </c>
       <c r="L38" s="12" t="s">
         <v>180</v>
@@ -30528,7 +30526,7 @@
         <v>36</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>1217</v>
+        <v>1202</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>515</v>
@@ -30546,7 +30544,7 @@
         <v>14</v>
       </c>
       <c r="K40" s="11" t="s">
-        <v>1055</v>
+        <v>1044</v>
       </c>
       <c r="L40" s="12" t="s">
         <v>181</v>
@@ -30589,8 +30587,8 @@
       <c r="J41" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="K41" s="11" t="s">
-        <v>1019</v>
+      <c r="K41" s="110" t="s">
+        <v>256</v>
       </c>
       <c r="L41" s="12" t="s">
         <v>829</v>
@@ -30634,7 +30632,7 @@
         <v>14</v>
       </c>
       <c r="K42" s="11" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="L42" s="12" t="s">
         <v>695</v>
@@ -30666,8 +30664,8 @@
       <c r="J43" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="K43" s="11" t="s">
-        <v>1020</v>
+      <c r="K43" s="110" t="s">
+        <v>1301</v>
       </c>
       <c r="L43" s="12" t="s">
         <v>687</v>
@@ -30710,8 +30708,8 @@
       <c r="J44" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="K44" s="11" t="s">
-        <v>1020</v>
+      <c r="K44" s="110" t="s">
+        <v>1301</v>
       </c>
       <c r="L44" s="11" t="s">
         <v>688</v>
@@ -30737,7 +30735,7 @@
         <v>41</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>1218</v>
+        <v>1203</v>
       </c>
       <c r="F45" s="11" t="s">
         <v>532</v>
@@ -30777,7 +30775,7 @@
         <v>42</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>1219</v>
+        <v>1204</v>
       </c>
       <c r="F46" s="11" t="s">
         <v>533</v>
@@ -30809,7 +30807,7 @@
       <c r="U46" s="51"/>
       <c r="V46" s="51"/>
     </row>
-    <row r="47" spans="1:22" ht="35.65" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:22" ht="24" x14ac:dyDescent="0.45">
       <c r="A47" s="12"/>
       <c r="B47" s="11"/>
       <c r="C47" s="11"/>
@@ -30817,13 +30815,13 @@
         <v>43</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>1220</v>
+        <v>1205</v>
       </c>
       <c r="F47" s="56" t="s">
-        <v>1289</v>
+        <v>1273</v>
       </c>
       <c r="G47" s="56" t="s">
-        <v>1290</v>
+        <v>1274</v>
       </c>
       <c r="H47" s="11" t="s">
         <v>148</v>
@@ -31184,7 +31182,7 @@
   <dimension ref="A1:V17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -31236,7 +31234,7 @@
         <v>7</v>
       </c>
       <c r="K1" s="25" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="L1" s="25" t="s">
         <v>8</v>
@@ -31347,20 +31345,20 @@
     <row r="5" spans="1:22" s="23" customFormat="1" ht="58.9" x14ac:dyDescent="0.45">
       <c r="A5" s="45"/>
       <c r="B5" s="56" t="s">
-        <v>1255</v>
+        <v>1240</v>
       </c>
       <c r="C5" s="56"/>
       <c r="D5" s="52">
         <v>2</v>
       </c>
       <c r="E5" s="56" t="s">
-        <v>1126</v>
+        <v>1111</v>
       </c>
       <c r="F5" s="56" t="s">
-        <v>1298</v>
+        <v>1281</v>
       </c>
       <c r="G5" s="56" t="s">
-        <v>1299</v>
+        <v>1282</v>
       </c>
       <c r="H5" s="56" t="s">
         <v>10</v>
@@ -31372,19 +31370,19 @@
         <v>14</v>
       </c>
       <c r="K5" s="56" t="s">
-        <v>1291</v>
+        <v>1275</v>
       </c>
       <c r="L5" s="35" t="s">
-        <v>1244</v>
+        <v>1229</v>
       </c>
       <c r="M5" s="35" t="s">
-        <v>1126</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="6" spans="1:22" s="2" customFormat="1" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A6" s="12"/>
       <c r="B6" s="56" t="s">
-        <v>1255</v>
+        <v>1240</v>
       </c>
       <c r="C6" s="56"/>
       <c r="D6" s="52">
@@ -31394,10 +31392,10 @@
         <v>22</v>
       </c>
       <c r="F6" s="56" t="s">
-        <v>1124</v>
+        <v>1109</v>
       </c>
       <c r="G6" s="56" t="s">
-        <v>1125</v>
+        <v>1110</v>
       </c>
       <c r="H6" s="56" t="s">
         <v>10</v>
@@ -31408,14 +31406,14 @@
       <c r="J6" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="56" t="s">
-        <v>1047</v>
+      <c r="K6" s="111" t="s">
+        <v>22</v>
       </c>
       <c r="L6" s="35" t="s">
-        <v>1129</v>
+        <v>1114</v>
       </c>
       <c r="M6" s="35" t="s">
-        <v>1127</v>
+        <v>1112</v>
       </c>
       <c r="N6" s="51"/>
       <c r="O6" s="51"/>
@@ -31437,13 +31435,13 @@
         <v>4</v>
       </c>
       <c r="E7" s="56" t="s">
-        <v>1135</v>
+        <v>1120</v>
       </c>
       <c r="F7" s="56" t="s">
-        <v>1133</v>
+        <v>1118</v>
       </c>
       <c r="G7" s="56" t="s">
-        <v>1134</v>
+        <v>1119</v>
       </c>
       <c r="H7" s="56" t="s">
         <v>13</v>
@@ -31454,7 +31452,7 @@
       <c r="J7" s="56"/>
       <c r="K7" s="35"/>
       <c r="L7" s="35" t="s">
-        <v>1136</v>
+        <v>1121</v>
       </c>
       <c r="M7" s="35" t="s">
         <v>552</v>
@@ -31499,13 +31497,13 @@
         <v>6</v>
       </c>
       <c r="E9" s="56" t="s">
-        <v>1137</v>
+        <v>1122</v>
       </c>
       <c r="F9" s="56" t="s">
-        <v>1138</v>
+        <v>1123</v>
       </c>
       <c r="G9" s="56" t="s">
-        <v>1139</v>
+        <v>1124</v>
       </c>
       <c r="H9" s="56" t="s">
         <v>10</v>
@@ -31516,11 +31514,11 @@
       <c r="J9" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="35" t="s">
-        <v>1058</v>
+      <c r="K9" s="107" t="s">
+        <v>1302</v>
       </c>
       <c r="L9" s="35" t="s">
-        <v>1146</v>
+        <v>1131</v>
       </c>
       <c r="M9" s="35" t="s">
         <v>441</v>
@@ -31529,7 +31527,7 @@
     <row r="10" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A10" s="56"/>
       <c r="B10" s="56" t="s">
-        <v>1255</v>
+        <v>1240</v>
       </c>
       <c r="C10" s="56"/>
       <c r="D10" s="52">
@@ -31539,10 +31537,10 @@
         <v>197</v>
       </c>
       <c r="F10" s="56" t="s">
-        <v>1256</v>
+        <v>1241</v>
       </c>
       <c r="G10" s="56" t="s">
-        <v>1256</v>
+        <v>1241</v>
       </c>
       <c r="H10" s="56" t="s">
         <v>10</v>
@@ -31553,8 +31551,8 @@
       <c r="J10" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="K10" s="34" t="s">
-        <v>1293</v>
+      <c r="K10" s="106" t="s">
+        <v>1277</v>
       </c>
       <c r="L10" s="56" t="s">
         <v>197</v>
@@ -31588,8 +31586,8 @@
       <c r="J11" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="K11" s="35" t="s">
-        <v>1294</v>
+      <c r="K11" s="107" t="s">
+        <v>1278</v>
       </c>
       <c r="L11" s="35" t="s">
         <v>557</v>
@@ -31624,7 +31622,7 @@
         <v>14</v>
       </c>
       <c r="K12" s="35" t="s">
-        <v>1056</v>
+        <v>1045</v>
       </c>
       <c r="L12" s="35" t="s">
         <v>246</v>
@@ -31636,53 +31634,53 @@
     <row r="13" spans="1:22" s="23" customFormat="1" ht="24" x14ac:dyDescent="0.45">
       <c r="A13" s="103"/>
       <c r="B13" s="56" t="s">
-        <v>1255</v>
+        <v>1240</v>
       </c>
       <c r="C13" s="56"/>
       <c r="D13" s="52">
         <v>10</v>
       </c>
       <c r="E13" s="56" t="s">
-        <v>1141</v>
+        <v>1126</v>
       </c>
       <c r="F13" s="56" t="s">
-        <v>1140</v>
+        <v>1125</v>
       </c>
       <c r="G13" s="56" t="s">
-        <v>1249</v>
+        <v>1234</v>
       </c>
       <c r="H13" s="56" t="s">
-        <v>1142</v>
+        <v>1127</v>
       </c>
       <c r="I13" s="56" t="s">
         <v>11</v>
       </c>
       <c r="J13" s="56" t="s">
-        <v>1142</v>
+        <v>1127</v>
       </c>
       <c r="K13" s="35"/>
       <c r="L13" s="35" t="s">
-        <v>1145</v>
+        <v>1130</v>
       </c>
       <c r="M13" s="35"/>
     </row>
     <row r="14" spans="1:22" s="23" customFormat="1" ht="24" x14ac:dyDescent="0.45">
       <c r="A14" s="103"/>
       <c r="B14" s="56" t="s">
-        <v>1255</v>
+        <v>1240</v>
       </c>
       <c r="C14" s="56"/>
       <c r="D14" s="52">
         <v>11</v>
       </c>
       <c r="E14" s="56" t="s">
-        <v>1144</v>
+        <v>1129</v>
       </c>
       <c r="F14" s="34" t="s">
-        <v>1143</v>
+        <v>1128</v>
       </c>
       <c r="G14" s="34" t="s">
-        <v>1250</v>
+        <v>1235</v>
       </c>
       <c r="H14" s="56" t="s">
         <v>10</v>
@@ -31693,15 +31691,15 @@
       <c r="J14" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="K14" s="35" t="s">
-        <v>1058</v>
+      <c r="K14" s="107" t="s">
+        <v>1302</v>
       </c>
       <c r="L14" s="35" t="s">
-        <v>1147</v>
+        <v>1132</v>
       </c>
       <c r="M14" s="35"/>
     </row>
-    <row r="15" spans="1:22" ht="35.65" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:22" ht="24" x14ac:dyDescent="0.45">
       <c r="A15" s="52"/>
       <c r="B15" s="52"/>
       <c r="C15" s="52"/>
@@ -31726,8 +31724,8 @@
       <c r="J15" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="K15" s="35" t="s">
-        <v>1019</v>
+      <c r="K15" s="107" t="s">
+        <v>256</v>
       </c>
       <c r="L15" s="35" t="s">
         <v>829</v>
@@ -31761,7 +31759,7 @@
       <c r="J16" s="56"/>
       <c r="K16" s="35"/>
       <c r="L16" s="35" t="s">
-        <v>1132</v>
+        <v>1117</v>
       </c>
       <c r="M16" s="35"/>
     </row>
@@ -31791,10 +31789,10 @@
         <v>14</v>
       </c>
       <c r="K17" s="35" t="s">
-        <v>1057</v>
+        <v>1046</v>
       </c>
       <c r="L17" s="104" t="s">
-        <v>1131</v>
+        <v>1116</v>
       </c>
       <c r="M17" s="35"/>
     </row>
@@ -31808,8 +31806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -31860,7 +31858,7 @@
         <v>7</v>
       </c>
       <c r="K1" s="25" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="L1" s="25" t="s">
         <v>8</v>
@@ -32019,10 +32017,10 @@
         <v>2</v>
       </c>
       <c r="E6" s="56" t="s">
-        <v>1123</v>
+        <v>1108</v>
       </c>
       <c r="F6" s="56" t="s">
-        <v>1121</v>
+        <v>1106</v>
       </c>
       <c r="G6" s="56" t="s">
         <v>899</v>
@@ -32036,7 +32034,7 @@
       <c r="J6" s="56"/>
       <c r="K6" s="34"/>
       <c r="L6" s="35" t="s">
-        <v>1122</v>
+        <v>1107</v>
       </c>
       <c r="M6" s="35" t="s">
         <v>189</v>
@@ -32045,20 +32043,20 @@
     <row r="7" spans="1:13" s="51" customFormat="1" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A7" s="35"/>
       <c r="B7" s="56" t="s">
-        <v>1096</v>
+        <v>1082</v>
       </c>
       <c r="C7" s="56"/>
       <c r="D7" s="52">
         <v>3</v>
       </c>
       <c r="E7" s="56" t="s">
-        <v>1126</v>
+        <v>1111</v>
       </c>
       <c r="F7" s="56" t="s">
-        <v>1300</v>
+        <v>1283</v>
       </c>
       <c r="G7" s="56" t="s">
-        <v>1301</v>
+        <v>1284</v>
       </c>
       <c r="H7" s="56" t="s">
         <v>10</v>
@@ -32069,20 +32067,20 @@
       <c r="J7" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="56" t="s">
-        <v>1291</v>
+      <c r="K7" s="111" t="s">
+        <v>1294</v>
       </c>
       <c r="L7" s="35" t="s">
-        <v>1150</v>
+        <v>1135</v>
       </c>
       <c r="M7" s="35" t="s">
-        <v>1126</v>
+        <v>1111</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="51" customFormat="1" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A8" s="35"/>
       <c r="B8" s="56" t="s">
-        <v>1096</v>
+        <v>1082</v>
       </c>
       <c r="C8" s="56"/>
       <c r="D8" s="52">
@@ -32092,10 +32090,10 @@
         <v>22</v>
       </c>
       <c r="F8" s="56" t="s">
-        <v>1148</v>
+        <v>1133</v>
       </c>
       <c r="G8" s="56" t="s">
-        <v>1149</v>
+        <v>1134</v>
       </c>
       <c r="H8" s="56" t="s">
         <v>10</v>
@@ -32106,14 +32104,14 @@
       <c r="J8" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="56" t="s">
-        <v>1047</v>
+      <c r="K8" s="111" t="s">
+        <v>22</v>
       </c>
       <c r="L8" s="35" t="s">
-        <v>1129</v>
+        <v>1114</v>
       </c>
       <c r="M8" s="35" t="s">
-        <v>1127</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="51" customFormat="1" ht="24" x14ac:dyDescent="0.45">
@@ -32142,7 +32140,7 @@
         <v>14</v>
       </c>
       <c r="K9" s="34" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="L9" s="35" t="s">
         <v>259</v>
@@ -32159,7 +32157,7 @@
         <v>6</v>
       </c>
       <c r="E10" s="56" t="s">
-        <v>1224</v>
+        <v>1209</v>
       </c>
       <c r="F10" s="35" t="s">
         <v>760</v>
@@ -32192,13 +32190,13 @@
         <v>7</v>
       </c>
       <c r="E11" s="56" t="s">
-        <v>1245</v>
+        <v>1230</v>
       </c>
       <c r="F11" s="56" t="s">
-        <v>1151</v>
+        <v>1136</v>
       </c>
       <c r="G11" s="56" t="s">
-        <v>1152</v>
+        <v>1137</v>
       </c>
       <c r="H11" s="56" t="s">
         <v>10</v>
@@ -32209,8 +32207,8 @@
       <c r="J11" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="K11" s="34" t="s">
-        <v>1058</v>
+      <c r="K11" s="106" t="s">
+        <v>1302</v>
       </c>
       <c r="L11" s="35" t="s">
         <v>886</v>
@@ -32227,13 +32225,13 @@
         <v>8</v>
       </c>
       <c r="E12" s="56" t="s">
-        <v>1246</v>
+        <v>1231</v>
       </c>
       <c r="F12" s="56" t="s">
-        <v>1153</v>
+        <v>1138</v>
       </c>
       <c r="G12" s="56" t="s">
-        <v>1154</v>
+        <v>1139</v>
       </c>
       <c r="H12" s="56" t="s">
         <v>10</v>
@@ -32258,13 +32256,13 @@
         <v>9</v>
       </c>
       <c r="E13" s="56" t="s">
-        <v>1221</v>
+        <v>1206</v>
       </c>
       <c r="F13" s="56" t="s">
-        <v>1079</v>
+        <v>1067</v>
       </c>
       <c r="G13" s="56" t="s">
-        <v>1080</v>
+        <v>1068</v>
       </c>
       <c r="H13" s="56" t="s">
         <v>10</v>
@@ -32276,13 +32274,13 @@
         <v>14</v>
       </c>
       <c r="K13" s="34" t="s">
-        <v>1081</v>
+        <v>1298</v>
       </c>
       <c r="L13" s="35" t="s">
-        <v>1082</v>
+        <v>1069</v>
       </c>
       <c r="M13" s="56" t="s">
-        <v>1083</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="14" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.45">
@@ -32310,8 +32308,8 @@
       <c r="J14" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="K14" s="34" t="s">
-        <v>1293</v>
+      <c r="K14" s="106" t="s">
+        <v>1277</v>
       </c>
       <c r="L14" s="56" t="s">
         <v>192</v>
@@ -32345,8 +32343,8 @@
       <c r="J15" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="K15" s="34" t="s">
-        <v>1294</v>
+      <c r="K15" s="106" t="s">
+        <v>1278</v>
       </c>
       <c r="L15" s="56" t="s">
         <v>557</v>
@@ -32358,20 +32356,20 @@
     <row r="16" spans="1:13" s="51" customFormat="1" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A16" s="56"/>
       <c r="B16" s="56" t="s">
-        <v>1096</v>
+        <v>1082</v>
       </c>
       <c r="C16" s="56"/>
       <c r="D16" s="52">
         <v>12</v>
       </c>
       <c r="E16" s="56" t="s">
-        <v>1084</v>
+        <v>1071</v>
       </c>
       <c r="F16" s="56" t="s">
-        <v>1085</v>
+        <v>1072</v>
       </c>
       <c r="G16" s="56" t="s">
-        <v>1085</v>
+        <v>1072</v>
       </c>
       <c r="H16" s="56" t="s">
         <v>10</v>
@@ -32383,30 +32381,30 @@
         <v>14</v>
       </c>
       <c r="K16" s="34" t="s">
-        <v>1056</v>
+        <v>1045</v>
       </c>
       <c r="L16" s="35" t="s">
-        <v>1086</v>
+        <v>1073</v>
       </c>
       <c r="M16" s="56"/>
     </row>
     <row r="17" spans="1:13" s="51" customFormat="1" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A17" s="56"/>
       <c r="B17" s="56" t="s">
-        <v>1096</v>
+        <v>1082</v>
       </c>
       <c r="C17" s="56"/>
       <c r="D17" s="52">
         <v>13</v>
       </c>
       <c r="E17" s="56" t="s">
-        <v>1087</v>
+        <v>1074</v>
       </c>
       <c r="F17" s="56" t="s">
-        <v>1088</v>
+        <v>1075</v>
       </c>
       <c r="G17" s="56" t="s">
-        <v>1089</v>
+        <v>1076</v>
       </c>
       <c r="H17" s="56" t="s">
         <v>10</v>
@@ -32417,31 +32415,31 @@
       <c r="J17" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="K17" s="34" t="s">
-        <v>1090</v>
+      <c r="K17" s="106" t="s">
+        <v>1290</v>
       </c>
       <c r="L17" s="35" t="s">
-        <v>1091</v>
+        <v>1077</v>
       </c>
       <c r="M17" s="56"/>
     </row>
     <row r="18" spans="1:13" s="51" customFormat="1" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="56"/>
       <c r="B18" s="56" t="s">
-        <v>1096</v>
+        <v>1082</v>
       </c>
       <c r="C18" s="56"/>
       <c r="D18" s="52">
         <v>14</v>
       </c>
       <c r="E18" s="56" t="s">
-        <v>1092</v>
+        <v>1078</v>
       </c>
       <c r="F18" s="56" t="s">
-        <v>1253</v>
+        <v>1238</v>
       </c>
       <c r="G18" s="56" t="s">
-        <v>1254</v>
+        <v>1239</v>
       </c>
       <c r="H18" s="56" t="s">
         <v>148</v>
@@ -32452,30 +32450,30 @@
       <c r="J18" s="56"/>
       <c r="K18" s="34"/>
       <c r="L18" s="35" t="s">
-        <v>1093</v>
+        <v>1079</v>
       </c>
       <c r="M18" s="56"/>
     </row>
     <row r="19" spans="1:13" s="51" customFormat="1" ht="24" x14ac:dyDescent="0.45">
       <c r="A19" s="56"/>
       <c r="B19" s="56" t="s">
-        <v>1096</v>
+        <v>1082</v>
       </c>
       <c r="C19" s="56"/>
       <c r="D19" s="52">
         <v>15</v>
       </c>
       <c r="E19" s="56" t="s">
-        <v>1141</v>
+        <v>1126</v>
       </c>
       <c r="F19" s="56" t="s">
-        <v>1155</v>
+        <v>1140</v>
       </c>
       <c r="G19" s="56" t="s">
-        <v>1248</v>
+        <v>1233</v>
       </c>
       <c r="H19" s="56" t="s">
-        <v>1252</v>
+        <v>1237</v>
       </c>
       <c r="I19" s="56" t="s">
         <v>11</v>
@@ -32483,27 +32481,27 @@
       <c r="J19" s="56"/>
       <c r="K19" s="35"/>
       <c r="L19" s="35" t="s">
-        <v>1251</v>
+        <v>1236</v>
       </c>
       <c r="M19" s="35"/>
     </row>
     <row r="20" spans="1:13" s="51" customFormat="1" ht="24" x14ac:dyDescent="0.45">
       <c r="A20" s="56"/>
       <c r="B20" s="56" t="s">
-        <v>1096</v>
+        <v>1082</v>
       </c>
       <c r="C20" s="56"/>
       <c r="D20" s="52">
         <v>16</v>
       </c>
       <c r="E20" s="56" t="s">
-        <v>1144</v>
+        <v>1129</v>
       </c>
       <c r="F20" s="34" t="s">
-        <v>1156</v>
+        <v>1141</v>
       </c>
       <c r="G20" s="34" t="s">
-        <v>1247</v>
+        <v>1232</v>
       </c>
       <c r="H20" s="56" t="s">
         <v>10</v>
@@ -32514,11 +32512,11 @@
       <c r="J20" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="K20" s="34" t="s">
-        <v>1058</v>
+      <c r="K20" s="106" t="s">
+        <v>1302</v>
       </c>
       <c r="L20" s="35" t="s">
-        <v>1147</v>
+        <v>1132</v>
       </c>
       <c r="M20" s="35"/>
     </row>
@@ -32530,7 +32528,7 @@
         <v>17</v>
       </c>
       <c r="E21" s="56" t="s">
-        <v>1222</v>
+        <v>1207</v>
       </c>
       <c r="F21" s="35" t="s">
         <v>828</v>
@@ -32561,7 +32559,7 @@
         <v>18</v>
       </c>
       <c r="E22" s="56" t="s">
-        <v>1223</v>
+        <v>1208</v>
       </c>
       <c r="F22" s="34" t="s">
         <v>782</v>
@@ -32672,7 +32670,7 @@
         <v>14</v>
       </c>
       <c r="K25" s="108" t="s">
-        <v>1303</v>
+        <v>1286</v>
       </c>
       <c r="L25" s="35" t="s">
         <v>196</v>
@@ -32737,8 +32735,8 @@
       <c r="J27" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="K27" s="15" t="s">
-        <v>1019</v>
+      <c r="K27" s="108" t="s">
+        <v>256</v>
       </c>
       <c r="L27" s="35" t="s">
         <v>829</v>
@@ -32757,7 +32755,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -32771,7 +32771,7 @@
     <col min="8" max="8" width="11.86328125" style="10" customWidth="1"/>
     <col min="9" max="9" width="9.3984375" style="10" customWidth="1"/>
     <col min="10" max="10" width="9.1328125" style="10" customWidth="1"/>
-    <col min="11" max="11" width="15.59765625" style="77" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" style="77" customWidth="1"/>
     <col min="12" max="12" width="35" style="10" customWidth="1"/>
     <col min="13" max="13" width="50.3984375" style="10" customWidth="1"/>
     <col min="14" max="16384" width="8.86328125" style="2"/>
@@ -32809,7 +32809,7 @@
         <v>7</v>
       </c>
       <c r="K1" s="25" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="L1" s="25" t="s">
         <v>8</v>
@@ -32915,7 +32915,7 @@
         <v>834</v>
       </c>
       <c r="L4" s="35" t="s">
-        <v>1257</v>
+        <v>1242</v>
       </c>
       <c r="M4" s="35" t="s">
         <v>108</v>
@@ -32946,14 +32946,14 @@
       <c r="J5" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="35" t="s">
-        <v>1014</v>
+      <c r="K5" s="107" t="s">
+        <v>1299</v>
       </c>
       <c r="L5" s="50" t="s">
         <v>1012</v>
       </c>
       <c r="M5" s="50" t="s">
-        <v>1258</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="10" customFormat="1" ht="11.65" x14ac:dyDescent="0.35">
@@ -33003,7 +33003,7 @@
         <v>5</v>
       </c>
       <c r="E7" s="35" t="s">
-        <v>1259</v>
+        <v>1244</v>
       </c>
       <c r="F7" s="35" t="s">
         <v>750</v>
@@ -33034,7 +33034,7 @@
         <v>6</v>
       </c>
       <c r="E8" s="35" t="s">
-        <v>1163</v>
+        <v>1148</v>
       </c>
       <c r="F8" s="35" t="s">
         <v>302</v>
@@ -33052,7 +33052,7 @@
         <v>14</v>
       </c>
       <c r="K8" s="35" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="L8" s="35" t="s">
         <v>248</v>
@@ -33089,7 +33089,7 @@
         <v>14</v>
       </c>
       <c r="K9" s="35" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="L9" s="35" t="s">
         <v>112</v>
@@ -33109,10 +33109,10 @@
         <v>689</v>
       </c>
       <c r="F10" s="34" t="s">
-        <v>1157</v>
+        <v>1142</v>
       </c>
       <c r="G10" s="34" t="s">
-        <v>1159</v>
+        <v>1144</v>
       </c>
       <c r="H10" s="35" t="s">
         <v>10</v>
@@ -33124,10 +33124,10 @@
         <v>14</v>
       </c>
       <c r="K10" s="34" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="L10" s="35" t="s">
-        <v>1161</v>
+        <v>1146</v>
       </c>
       <c r="M10" s="34"/>
     </row>
@@ -33142,10 +33142,10 @@
         <v>255</v>
       </c>
       <c r="F11" s="35" t="s">
-        <v>1158</v>
+        <v>1143</v>
       </c>
       <c r="G11" s="34" t="s">
-        <v>1160</v>
+        <v>1145</v>
       </c>
       <c r="H11" s="35" t="s">
         <v>10</v>
@@ -33156,8 +33156,8 @@
       <c r="J11" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="K11" s="34" t="s">
-        <v>1020</v>
+      <c r="K11" s="106" t="s">
+        <v>1301</v>
       </c>
       <c r="L11" s="35" t="s">
         <v>255</v>
@@ -33735,7 +33735,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -33784,7 +33784,7 @@
         <v>7</v>
       </c>
       <c r="K1" s="25" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="L1" s="25" t="s">
         <v>8</v>
@@ -34021,7 +34021,7 @@
         <v>14</v>
       </c>
       <c r="K8" s="35" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="L8" s="35" t="s">
         <v>259</v>
@@ -34075,7 +34075,7 @@
         <v>5</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>1164</v>
+        <v>1149</v>
       </c>
       <c r="F10" s="35" t="s">
         <v>751</v>
@@ -34092,7 +34092,7 @@
       <c r="J10" s="35"/>
       <c r="K10" s="35"/>
       <c r="L10" s="35" t="s">
-        <v>1260</v>
+        <v>1245</v>
       </c>
       <c r="M10" s="35" t="s">
         <v>120</v>
@@ -34106,7 +34106,7 @@
         <v>6</v>
       </c>
       <c r="E11" s="34" t="s">
-        <v>1165</v>
+        <v>1150</v>
       </c>
       <c r="F11" s="34" t="s">
         <v>315</v>
@@ -34124,7 +34124,7 @@
         <v>14</v>
       </c>
       <c r="K11" s="35" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="L11" s="35" t="s">
         <v>262</v>
@@ -34141,7 +34141,7 @@
         <v>7</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>1166</v>
+        <v>1151</v>
       </c>
       <c r="F12" s="34" t="s">
         <v>316</v>
@@ -34189,8 +34189,8 @@
       <c r="J13" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="K13" s="35" t="s">
-        <v>1019</v>
+      <c r="K13" s="107" t="s">
+        <v>256</v>
       </c>
       <c r="L13" s="35" t="s">
         <v>829</v>
@@ -34207,7 +34207,7 @@
         <v>9</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>1167</v>
+        <v>1152</v>
       </c>
       <c r="F14" s="35" t="s">
         <v>813</v>
@@ -34238,7 +34238,7 @@
         <v>10</v>
       </c>
       <c r="E15" s="35" t="s">
-        <v>1168</v>
+        <v>1153</v>
       </c>
       <c r="F15" s="34" t="s">
         <v>761</v>
@@ -34349,7 +34349,7 @@
         <v>14</v>
       </c>
       <c r="K18" s="107" t="s">
-        <v>1303</v>
+        <v>1286</v>
       </c>
       <c r="L18" s="54" t="s">
         <v>201</v>
@@ -34397,7 +34397,7 @@
         <v>15</v>
       </c>
       <c r="E20" s="58" t="s">
-        <v>1169</v>
+        <v>1154</v>
       </c>
       <c r="F20" s="58" t="s">
         <v>320</v>
@@ -34415,7 +34415,7 @@
         <v>14</v>
       </c>
       <c r="K20" s="107" t="s">
-        <v>1303</v>
+        <v>1286</v>
       </c>
       <c r="L20" s="57" t="s">
         <v>524</v>
@@ -34432,7 +34432,7 @@
         <v>16</v>
       </c>
       <c r="E21" s="34" t="s">
-        <v>1170</v>
+        <v>1155</v>
       </c>
       <c r="F21" s="34" t="s">
         <v>812</v>
@@ -34463,7 +34463,7 @@
         <v>17</v>
       </c>
       <c r="E22" s="34" t="s">
-        <v>1171</v>
+        <v>1156</v>
       </c>
       <c r="F22" s="34" t="s">
         <v>762</v>
@@ -34572,7 +34572,7 @@
         <v>14</v>
       </c>
       <c r="K25" s="35" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="L25" s="35" t="s">
         <v>695</v>
@@ -34604,8 +34604,8 @@
       <c r="J26" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="K26" s="15" t="s">
-        <v>1020</v>
+      <c r="K26" s="108" t="s">
+        <v>1301</v>
       </c>
       <c r="L26" s="35" t="s">
         <v>255</v>
@@ -34644,8 +34644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K20" activeCellId="1" sqref="K18 K20"/>
+    <sheetView topLeftCell="A15" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -34695,7 +34695,7 @@
         <v>7</v>
       </c>
       <c r="K1" s="25" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="L1" s="25" t="s">
         <v>8</v>
@@ -34866,13 +34866,13 @@
         <v>14</v>
       </c>
       <c r="K6" s="35" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="L6" s="35" t="s">
-        <v>1094</v>
+        <v>1080</v>
       </c>
       <c r="M6" s="35" t="s">
-        <v>1095</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="35.65" x14ac:dyDescent="0.45">
@@ -34883,7 +34883,7 @@
         <v>4</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>1243</v>
+        <v>1228</v>
       </c>
       <c r="F7" s="34" t="s">
         <v>944</v>
@@ -34901,7 +34901,7 @@
         <v>91</v>
       </c>
       <c r="K7" s="35" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
       <c r="L7" s="59" t="s">
         <v>631</v>
@@ -34918,13 +34918,13 @@
         <v>5</v>
       </c>
       <c r="E8" s="35" t="s">
-        <v>1234</v>
+        <v>1219</v>
       </c>
       <c r="F8" s="35" t="s">
-        <v>1235</v>
+        <v>1220</v>
       </c>
       <c r="G8" s="35" t="s">
-        <v>1237</v>
+        <v>1222</v>
       </c>
       <c r="H8" s="35" t="s">
         <v>10</v>
@@ -34950,13 +34950,13 @@
         <v>6</v>
       </c>
       <c r="E9" s="34" t="s">
-        <v>1242</v>
+        <v>1227</v>
       </c>
       <c r="F9" s="34" t="s">
-        <v>1230</v>
+        <v>1215</v>
       </c>
       <c r="G9" s="34" t="s">
-        <v>1236</v>
+        <v>1221</v>
       </c>
       <c r="H9" s="34" t="s">
         <v>10</v>
@@ -34968,7 +34968,7 @@
         <v>14</v>
       </c>
       <c r="K9" s="102" t="s">
-        <v>1040</v>
+        <v>1035</v>
       </c>
       <c r="L9" s="59"/>
       <c r="M9" s="59"/>
@@ -34998,10 +34998,10 @@
       <c r="J10" s="35"/>
       <c r="K10" s="35"/>
       <c r="L10" s="35" t="s">
-        <v>1260</v>
+        <v>1245</v>
       </c>
       <c r="M10" s="35" t="s">
-        <v>1107</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="35.65" x14ac:dyDescent="0.45">
@@ -35030,7 +35030,7 @@
         <v>14</v>
       </c>
       <c r="K11" s="35" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="L11" s="35" t="s">
         <v>262</v>
@@ -35047,7 +35047,7 @@
         <v>9</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>1173</v>
+        <v>1158</v>
       </c>
       <c r="F12" s="34" t="s">
         <v>350</v>
@@ -35095,8 +35095,8 @@
       <c r="J13" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="K13" s="35" t="s">
-        <v>1019</v>
+      <c r="K13" s="107" t="s">
+        <v>256</v>
       </c>
       <c r="L13" s="35" t="s">
         <v>829</v>
@@ -35113,7 +35113,7 @@
         <v>11</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>1172</v>
+        <v>1157</v>
       </c>
       <c r="F14" s="35" t="s">
         <v>814</v>
@@ -35144,7 +35144,7 @@
         <v>12</v>
       </c>
       <c r="E15" s="35" t="s">
-        <v>1174</v>
+        <v>1159</v>
       </c>
       <c r="F15" s="34" t="s">
         <v>763</v>
@@ -35255,7 +35255,7 @@
         <v>14</v>
       </c>
       <c r="K18" s="107" t="s">
-        <v>1303</v>
+        <v>1286</v>
       </c>
       <c r="L18" s="35" t="s">
         <v>201</v>
@@ -35303,7 +35303,7 @@
         <v>17</v>
       </c>
       <c r="E20" s="34" t="s">
-        <v>1169</v>
+        <v>1154</v>
       </c>
       <c r="F20" s="34" t="s">
         <v>324</v>
@@ -35321,7 +35321,7 @@
         <v>14</v>
       </c>
       <c r="K20" s="107" t="s">
-        <v>1303</v>
+        <v>1286</v>
       </c>
       <c r="L20" s="35" t="s">
         <v>524</v>
@@ -35338,7 +35338,7 @@
         <v>18</v>
       </c>
       <c r="E21" s="34" t="s">
-        <v>1170</v>
+        <v>1155</v>
       </c>
       <c r="F21" s="34" t="s">
         <v>815</v>
@@ -35369,7 +35369,7 @@
         <v>19</v>
       </c>
       <c r="E22" s="34" t="s">
-        <v>1171</v>
+        <v>1156</v>
       </c>
       <c r="F22" s="34" t="s">
         <v>764</v>
@@ -35478,7 +35478,7 @@
         <v>14</v>
       </c>
       <c r="K25" s="35" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="L25" s="35" t="s">
         <v>695</v>
@@ -35510,8 +35510,8 @@
       <c r="J26" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="K26" s="35" t="s">
-        <v>1020</v>
+      <c r="K26" s="107" t="s">
+        <v>1301</v>
       </c>
       <c r="L26" s="35" t="s">
         <v>255</v>
@@ -35580,7 +35580,7 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.73046875" defaultRowHeight="11.65" x14ac:dyDescent="0.45"/>
@@ -35631,7 +35631,7 @@
         <v>7</v>
       </c>
       <c r="K1" s="25" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="L1" s="25" t="s">
         <v>8</v>
@@ -35774,7 +35774,7 @@
         <v>1003</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>1060</v>
+        <v>1048</v>
       </c>
       <c r="M5" s="6" t="s">
         <v>115</v>
@@ -35808,7 +35808,7 @@
         <v>14</v>
       </c>
       <c r="K6" s="12" t="s">
-        <v>1022</v>
+        <v>1019</v>
       </c>
       <c r="L6" s="12" t="s">
         <v>54</v>
@@ -35828,7 +35828,7 @@
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K20" activeCellId="1" sqref="K18 K20"/>
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -35879,7 +35879,7 @@
         <v>7</v>
       </c>
       <c r="K1" s="25" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="L1" s="25" t="s">
         <v>8</v>
@@ -36106,7 +36106,7 @@
         <v>3</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>1175</v>
+        <v>1160</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>580</v>
@@ -36121,11 +36121,11 @@
         <v>11</v>
       </c>
       <c r="J8" s="35" t="s">
-        <v>1061</v>
+        <v>1049</v>
       </c>
       <c r="K8" s="34"/>
       <c r="L8" s="35" t="s">
-        <v>1062</v>
+        <v>1050</v>
       </c>
       <c r="M8" s="35" t="s">
         <v>577</v>
@@ -36157,13 +36157,13 @@
         <v>14</v>
       </c>
       <c r="K9" s="35" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="L9" s="35" t="s">
-        <v>1094</v>
+        <v>1080</v>
       </c>
       <c r="M9" s="35" t="s">
-        <v>1095</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.45">
@@ -36174,7 +36174,7 @@
         <v>5</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>1176</v>
+        <v>1161</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>753</v>
@@ -36191,10 +36191,10 @@
       <c r="J10" s="35"/>
       <c r="K10" s="34"/>
       <c r="L10" s="35" t="s">
-        <v>1260</v>
+        <v>1245</v>
       </c>
       <c r="M10" s="35" t="s">
-        <v>1107</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="11" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.45">
@@ -36223,7 +36223,7 @@
         <v>14</v>
       </c>
       <c r="K11" s="34" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="L11" s="35" t="s">
         <v>262</v>
@@ -36240,7 +36240,7 @@
         <v>7</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>1173</v>
+        <v>1158</v>
       </c>
       <c r="F12" s="15" t="s">
         <v>353</v>
@@ -36288,8 +36288,8 @@
       <c r="J13" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="K13" s="15" t="s">
-        <v>1019</v>
+      <c r="K13" s="108" t="s">
+        <v>256</v>
       </c>
       <c r="L13" s="12" t="s">
         <v>829</v>
@@ -36306,7 +36306,7 @@
         <v>9</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>1167</v>
+        <v>1152</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>691</v>
@@ -36337,7 +36337,7 @@
         <v>10</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>1177</v>
+        <v>1162</v>
       </c>
       <c r="F15" s="15" t="s">
         <v>694</v>
@@ -36448,7 +36448,7 @@
         <v>14</v>
       </c>
       <c r="K18" s="108" t="s">
-        <v>1303</v>
+        <v>1286</v>
       </c>
       <c r="L18" s="12" t="s">
         <v>122</v>
@@ -36496,7 +36496,7 @@
         <v>15</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>1169</v>
+        <v>1154</v>
       </c>
       <c r="F20" s="15" t="s">
         <v>328</v>
@@ -36514,7 +36514,7 @@
         <v>14</v>
       </c>
       <c r="K20" s="108" t="s">
-        <v>1303</v>
+        <v>1286</v>
       </c>
       <c r="L20" s="12" t="s">
         <v>524</v>
@@ -36531,7 +36531,7 @@
         <v>16</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>1170</v>
+        <v>1155</v>
       </c>
       <c r="F21" s="15" t="s">
         <v>816</v>
@@ -36562,7 +36562,7 @@
         <v>17</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>1171</v>
+        <v>1156</v>
       </c>
       <c r="F22" s="15" t="s">
         <v>765</v>
@@ -36671,7 +36671,7 @@
         <v>14</v>
       </c>
       <c r="K25" s="15" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="L25" s="12" t="s">
         <v>695</v>
@@ -36703,8 +36703,8 @@
       <c r="J26" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="K26" s="15" t="s">
-        <v>1020</v>
+      <c r="K26" s="108" t="s">
+        <v>1301</v>
       </c>
       <c r="L26" s="12" t="s">
         <v>255</v>
@@ -36745,8 +36745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView topLeftCell="C7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K31" activeCellId="1" sqref="K29 K31"/>
+    <sheetView topLeftCell="C10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -36797,7 +36797,7 @@
         <v>7</v>
       </c>
       <c r="K1" s="25" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="L1" s="25" t="s">
         <v>8</v>
@@ -37084,7 +37084,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>1175</v>
+        <v>1160</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>855</v>
@@ -37099,11 +37099,11 @@
         <v>11</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>1063</v>
+        <v>1051</v>
       </c>
       <c r="K10" s="12"/>
       <c r="L10" s="12" t="s">
-        <v>1064</v>
+        <v>1052</v>
       </c>
       <c r="M10" s="12"/>
     </row>
@@ -37166,13 +37166,13 @@
         <v>14</v>
       </c>
       <c r="K12" s="35" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="L12" s="35" t="s">
-        <v>1094</v>
+        <v>1080</v>
       </c>
       <c r="M12" s="35" t="s">
-        <v>1095</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.45">
@@ -37183,7 +37183,7 @@
         <v>5</v>
       </c>
       <c r="E13" s="35" t="s">
-        <v>1178</v>
+        <v>1163</v>
       </c>
       <c r="F13" s="35" t="s">
         <v>754</v>
@@ -37200,7 +37200,7 @@
       <c r="J13" s="35"/>
       <c r="K13" s="35"/>
       <c r="L13" s="35" t="s">
-        <v>1260</v>
+        <v>1245</v>
       </c>
       <c r="M13" s="35" t="s">
         <v>120</v>
@@ -37214,7 +37214,7 @@
         <v>6</v>
       </c>
       <c r="E14" s="34" t="s">
-        <v>1179</v>
+        <v>1164</v>
       </c>
       <c r="F14" s="34" t="s">
         <v>279</v>
@@ -37232,7 +37232,7 @@
         <v>14</v>
       </c>
       <c r="K14" s="35" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="L14" s="35" t="s">
         <v>262</v>
@@ -37249,7 +37249,7 @@
         <v>7</v>
       </c>
       <c r="E15" s="34" t="s">
-        <v>1180</v>
+        <v>1165</v>
       </c>
       <c r="F15" s="34" t="s">
         <v>280</v>
@@ -37297,8 +37297,8 @@
       <c r="J16" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="K16" s="35" t="s">
-        <v>1019</v>
+      <c r="K16" s="107" t="s">
+        <v>256</v>
       </c>
       <c r="L16" s="35" t="s">
         <v>829</v>
@@ -37333,13 +37333,13 @@
         <v>14</v>
       </c>
       <c r="K17" s="35" t="s">
-        <v>1023</v>
+        <v>1020</v>
       </c>
       <c r="L17" s="52" t="s">
-        <v>1261</v>
+        <v>1246</v>
       </c>
       <c r="M17" s="52" t="s">
-        <v>1261</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="18" spans="1:14" s="2" customFormat="1" ht="35.65" x14ac:dyDescent="0.45">
@@ -37350,10 +37350,10 @@
         <v>10</v>
       </c>
       <c r="E18" s="35" t="s">
-        <v>1262</v>
+        <v>1247</v>
       </c>
       <c r="F18" s="35" t="s">
-        <v>1263</v>
+        <v>1248</v>
       </c>
       <c r="G18" s="35" t="s">
         <v>290</v>
@@ -37369,10 +37369,10 @@
       </c>
       <c r="K18" s="35"/>
       <c r="L18" s="35" t="s">
-        <v>1264</v>
+        <v>1249</v>
       </c>
       <c r="M18" s="35" t="s">
-        <v>1265</v>
+        <v>1250</v>
       </c>
       <c r="N18" s="101"/>
     </row>
@@ -37402,13 +37402,13 @@
         <v>14</v>
       </c>
       <c r="K19" s="35" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
       <c r="L19" s="35" t="s">
-        <v>1266</v>
+        <v>1251</v>
       </c>
       <c r="M19" s="35" t="s">
-        <v>1266</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="20" spans="1:14" s="2" customFormat="1" ht="24" x14ac:dyDescent="0.45">
@@ -37467,10 +37467,10 @@
       <c r="J21" s="35"/>
       <c r="K21" s="35"/>
       <c r="L21" s="35" t="s">
-        <v>1267</v>
+        <v>1252</v>
       </c>
       <c r="M21" s="35" t="s">
-        <v>1268</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="22" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.45">
@@ -37501,7 +37501,7 @@
         <v>14</v>
       </c>
       <c r="K22" s="35" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
       <c r="L22" s="35" t="s">
         <v>127</v>
@@ -37520,7 +37520,7 @@
         <v>15</v>
       </c>
       <c r="E23" s="35" t="s">
-        <v>1269</v>
+        <v>1254</v>
       </c>
       <c r="F23" s="35" t="s">
         <v>250</v>
@@ -37568,10 +37568,10 @@
       <c r="J24" s="35"/>
       <c r="K24" s="35"/>
       <c r="L24" s="35" t="s">
-        <v>1270</v>
+        <v>1255</v>
       </c>
       <c r="M24" s="35" t="s">
-        <v>1271</v>
+        <v>1256</v>
       </c>
     </row>
     <row r="25" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.45">
@@ -37582,7 +37582,7 @@
         <v>17</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>1181</v>
+        <v>1166</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>817</v>
@@ -37613,7 +37613,7 @@
         <v>18</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>1182</v>
+        <v>1167</v>
       </c>
       <c r="F26" s="15" t="s">
         <v>771</v>
@@ -37724,7 +37724,7 @@
         <v>14</v>
       </c>
       <c r="K29" s="109" t="s">
-        <v>1303</v>
+        <v>1286</v>
       </c>
       <c r="L29" s="35" t="s">
         <v>562</v>
@@ -37772,7 +37772,7 @@
         <v>23</v>
       </c>
       <c r="E31" s="34" t="s">
-        <v>1169</v>
+        <v>1154</v>
       </c>
       <c r="F31" s="34" t="s">
         <v>287</v>
@@ -37788,7 +37788,7 @@
         <v>14</v>
       </c>
       <c r="K31" s="109" t="s">
-        <v>1303</v>
+        <v>1286</v>
       </c>
       <c r="L31" s="35" t="s">
         <v>524</v>
@@ -37805,7 +37805,7 @@
         <v>24</v>
       </c>
       <c r="E32" s="34" t="s">
-        <v>1183</v>
+        <v>1168</v>
       </c>
       <c r="F32" s="34" t="s">
         <v>818</v>
@@ -37836,7 +37836,7 @@
         <v>25</v>
       </c>
       <c r="E33" s="34" t="s">
-        <v>1184</v>
+        <v>1169</v>
       </c>
       <c r="F33" s="34" t="s">
         <v>772</v>
@@ -37945,7 +37945,7 @@
         <v>14</v>
       </c>
       <c r="K36" s="12" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="L36" s="35" t="s">
         <v>695</v>
@@ -37977,8 +37977,8 @@
       <c r="J37" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="K37" s="12" t="s">
-        <v>1020</v>
+      <c r="K37" s="109" t="s">
+        <v>1301</v>
       </c>
       <c r="L37" s="35" t="s">
         <v>255</v>
@@ -38065,8 +38065,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:N66"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="K51" activeCellId="1" sqref="K53 K51"/>
+    <sheetView topLeftCell="A44" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K59" sqref="K59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -38080,7 +38080,8 @@
     <col min="7" max="7" width="16.73046875" style="89" customWidth="1"/>
     <col min="8" max="8" width="11" style="89" customWidth="1"/>
     <col min="9" max="9" width="9.3984375" style="89" customWidth="1"/>
-    <col min="10" max="11" width="20.73046875" style="89" customWidth="1"/>
+    <col min="10" max="10" width="20.73046875" style="89" customWidth="1"/>
+    <col min="11" max="11" width="29.265625" style="89" customWidth="1"/>
     <col min="12" max="12" width="59.265625" style="94" customWidth="1"/>
     <col min="13" max="13" width="57.1328125" style="94" customWidth="1"/>
     <col min="14" max="16384" width="20.1328125" style="89"/>
@@ -38118,7 +38119,7 @@
         <v>7</v>
       </c>
       <c r="K1" s="25" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="L1" s="25" t="s">
         <v>8</v>
@@ -38292,13 +38293,13 @@
         <v>14</v>
       </c>
       <c r="K6" s="35" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="L6" s="35" t="s">
-        <v>1094</v>
+        <v>1080</v>
       </c>
       <c r="M6" s="35" t="s">
-        <v>1095</v>
+        <v>1081</v>
       </c>
       <c r="N6" s="90"/>
     </row>
@@ -38342,7 +38343,7 @@
         <v>4</v>
       </c>
       <c r="E8" s="34" t="s">
-        <v>1193</v>
+        <v>1178</v>
       </c>
       <c r="F8" s="35" t="s">
         <v>755</v>
@@ -38359,7 +38360,7 @@
       <c r="J8" s="34"/>
       <c r="K8" s="34"/>
       <c r="L8" s="35" t="s">
-        <v>1260</v>
+        <v>1245</v>
       </c>
       <c r="M8" s="35" t="s">
         <v>120</v>
@@ -38392,7 +38393,7 @@
         <v>14</v>
       </c>
       <c r="K9" s="34" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="L9" s="35" t="s">
         <v>262</v>
@@ -38410,7 +38411,7 @@
         <v>6</v>
       </c>
       <c r="E10" s="34" t="s">
-        <v>1173</v>
+        <v>1158</v>
       </c>
       <c r="F10" s="34" t="s">
         <v>356</v>
@@ -38459,8 +38460,8 @@
       <c r="J11" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="K11" s="34" t="s">
-        <v>1019</v>
+      <c r="K11" s="106" t="s">
+        <v>256</v>
       </c>
       <c r="L11" s="35" t="s">
         <v>829</v>
@@ -38496,7 +38497,7 @@
         <v>14</v>
       </c>
       <c r="K12" s="34" t="s">
-        <v>1024</v>
+        <v>1021</v>
       </c>
       <c r="L12" s="35" t="s">
         <v>71</v>
@@ -38532,7 +38533,7 @@
         <v>14</v>
       </c>
       <c r="K13" s="34" t="s">
-        <v>1025</v>
+        <v>1022</v>
       </c>
       <c r="L13" s="35" t="s">
         <v>134</v>
@@ -38568,7 +38569,7 @@
         <v>14</v>
       </c>
       <c r="K14" s="34" t="s">
-        <v>1026</v>
+        <v>1023</v>
       </c>
       <c r="L14" s="35" t="s">
         <v>684</v>
@@ -38586,7 +38587,7 @@
         <v>11</v>
       </c>
       <c r="E15" s="34" t="s">
-        <v>1185</v>
+        <v>1170</v>
       </c>
       <c r="F15" s="34" t="s">
         <v>449</v>
@@ -38603,10 +38604,10 @@
       <c r="J15" s="34"/>
       <c r="K15" s="34"/>
       <c r="L15" s="35" t="s">
-        <v>1105</v>
+        <v>1091</v>
       </c>
       <c r="M15" s="35" t="s">
-        <v>1105</v>
+        <v>1091</v>
       </c>
       <c r="N15" s="90"/>
     </row>
@@ -38618,7 +38619,7 @@
         <v>12</v>
       </c>
       <c r="E16" s="34" t="s">
-        <v>1186</v>
+        <v>1171</v>
       </c>
       <c r="F16" s="34" t="s">
         <v>450</v>
@@ -38635,10 +38636,10 @@
       <c r="J16" s="34"/>
       <c r="K16" s="34"/>
       <c r="L16" s="35" t="s">
-        <v>1106</v>
+        <v>1092</v>
       </c>
       <c r="M16" s="35" t="s">
-        <v>1106</v>
+        <v>1092</v>
       </c>
       <c r="N16" s="90"/>
     </row>
@@ -38650,7 +38651,7 @@
         <v>13</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>1187</v>
+        <v>1172</v>
       </c>
       <c r="F17" s="34" t="s">
         <v>451</v>
@@ -38667,10 +38668,10 @@
       <c r="J17" s="34"/>
       <c r="K17" s="34"/>
       <c r="L17" s="35" t="s">
-        <v>1272</v>
+        <v>1257</v>
       </c>
       <c r="M17" s="35" t="s">
-        <v>1272</v>
+        <v>1257</v>
       </c>
       <c r="N17" s="90"/>
     </row>
@@ -38682,7 +38683,7 @@
         <v>14</v>
       </c>
       <c r="E18" s="34" t="s">
-        <v>1188</v>
+        <v>1173</v>
       </c>
       <c r="F18" s="34" t="s">
         <v>452</v>
@@ -38699,10 +38700,10 @@
       <c r="J18" s="34"/>
       <c r="K18" s="34"/>
       <c r="L18" s="35" t="s">
-        <v>1273</v>
+        <v>1258</v>
       </c>
       <c r="M18" s="35" t="s">
-        <v>1273</v>
+        <v>1258</v>
       </c>
       <c r="N18" s="90"/>
     </row>
@@ -38731,10 +38732,10 @@
       <c r="J19" s="34"/>
       <c r="K19" s="34"/>
       <c r="L19" s="35" t="s">
-        <v>1274</v>
+        <v>1259</v>
       </c>
       <c r="M19" s="35" t="s">
-        <v>1275</v>
+        <v>1260</v>
       </c>
       <c r="N19" s="90"/>
     </row>
@@ -38743,16 +38744,16 @@
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="D20" s="56" t="s">
-        <v>1096</v>
+        <v>1082</v>
       </c>
       <c r="E20" s="34" t="s">
-        <v>1097</v>
+        <v>1083</v>
       </c>
       <c r="F20" s="34" t="s">
-        <v>1098</v>
+        <v>1084</v>
       </c>
       <c r="G20" s="34" t="s">
-        <v>1099</v>
+        <v>1085</v>
       </c>
       <c r="H20" s="34" t="s">
         <v>10</v>
@@ -38763,14 +38764,14 @@
       <c r="J20" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="K20" s="34" t="s">
-        <v>1295</v>
+      <c r="K20" s="106" t="s">
+        <v>1296</v>
       </c>
       <c r="L20" s="35" t="s">
-        <v>1100</v>
+        <v>1086</v>
       </c>
       <c r="M20" s="35" t="s">
-        <v>1100</v>
+        <v>1086</v>
       </c>
       <c r="N20" s="90"/>
     </row>
@@ -38779,16 +38780,16 @@
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="56" t="s">
-        <v>1096</v>
+        <v>1082</v>
       </c>
       <c r="E21" s="34" t="s">
-        <v>1101</v>
+        <v>1087</v>
       </c>
       <c r="F21" s="34" t="s">
-        <v>1102</v>
+        <v>1088</v>
       </c>
       <c r="G21" s="34" t="s">
-        <v>1103</v>
+        <v>1089</v>
       </c>
       <c r="H21" s="34" t="s">
         <v>13</v>
@@ -38799,10 +38800,10 @@
       <c r="J21" s="34"/>
       <c r="K21" s="34"/>
       <c r="L21" s="35" t="s">
-        <v>1104</v>
+        <v>1090</v>
       </c>
       <c r="M21" s="35" t="s">
-        <v>1104</v>
+        <v>1090</v>
       </c>
       <c r="N21" s="90"/>
     </row>
@@ -38942,7 +38943,7 @@
         <v>20</v>
       </c>
       <c r="E26" s="34" t="s">
-        <v>1189</v>
+        <v>1174</v>
       </c>
       <c r="F26" s="34" t="s">
         <v>863</v>
@@ -38960,7 +38961,7 @@
         <v>14</v>
       </c>
       <c r="K26" s="34" t="s">
-        <v>1027</v>
+        <v>1024</v>
       </c>
       <c r="L26" s="35" t="s">
         <v>865</v>
@@ -38996,7 +38997,7 @@
         <v>14</v>
       </c>
       <c r="K27" s="34" t="s">
-        <v>1028</v>
+        <v>1025</v>
       </c>
       <c r="L27" s="35" t="s">
         <v>869</v>
@@ -39032,10 +39033,10 @@
         <v>14</v>
       </c>
       <c r="K28" s="34" t="s">
-        <v>1029</v>
+        <v>1026</v>
       </c>
       <c r="L28" s="35" t="s">
-        <v>1065</v>
+        <v>1053</v>
       </c>
       <c r="M28" s="35" t="s">
         <v>139</v>
@@ -39068,13 +39069,13 @@
         <v>14</v>
       </c>
       <c r="K29" s="34" t="s">
-        <v>1030</v>
+        <v>1027</v>
       </c>
       <c r="L29" s="35" t="s">
-        <v>1066</v>
+        <v>1054</v>
       </c>
       <c r="M29" s="35" t="s">
-        <v>1066</v>
+        <v>1054</v>
       </c>
       <c r="N29" s="90"/>
     </row>
@@ -39104,13 +39105,13 @@
         <v>14</v>
       </c>
       <c r="K30" s="34" t="s">
-        <v>1031</v>
+        <v>1028</v>
       </c>
       <c r="L30" s="35" t="s">
-        <v>1067</v>
+        <v>1055</v>
       </c>
       <c r="M30" s="35" t="s">
-        <v>1067</v>
+        <v>1055</v>
       </c>
       <c r="N30" s="90"/>
     </row>
@@ -39122,7 +39123,7 @@
         <v>25</v>
       </c>
       <c r="E31" s="34" t="s">
-        <v>1276</v>
+        <v>1261</v>
       </c>
       <c r="F31" s="34" t="s">
         <v>466</v>
@@ -39139,7 +39140,7 @@
       <c r="J31" s="34"/>
       <c r="K31" s="34"/>
       <c r="L31" s="35" t="s">
-        <v>1162</v>
+        <v>1147</v>
       </c>
       <c r="M31" s="35" t="s">
         <v>140</v>
@@ -39154,7 +39155,7 @@
         <v>26</v>
       </c>
       <c r="E32" s="34" t="s">
-        <v>1277</v>
+        <v>1262</v>
       </c>
       <c r="F32" s="34" t="s">
         <v>468</v>
@@ -39204,10 +39205,10 @@
         <v>14</v>
       </c>
       <c r="K33" s="34" t="s">
-        <v>1032</v>
+        <v>1029</v>
       </c>
       <c r="L33" s="35" t="s">
-        <v>1068</v>
+        <v>1056</v>
       </c>
       <c r="M33" s="35" t="s">
         <v>619</v>
@@ -39240,7 +39241,7 @@
         <v>14</v>
       </c>
       <c r="K34" s="34" t="s">
-        <v>1033</v>
+        <v>1030</v>
       </c>
       <c r="L34" s="35" t="s">
         <v>613</v>
@@ -39276,7 +39277,7 @@
         <v>14</v>
       </c>
       <c r="K35" s="34" t="s">
-        <v>1034</v>
+        <v>1031</v>
       </c>
       <c r="L35" s="35" t="s">
         <v>614</v>
@@ -39312,7 +39313,7 @@
         <v>14</v>
       </c>
       <c r="K36" s="34" t="s">
-        <v>1035</v>
+        <v>1032</v>
       </c>
       <c r="L36" s="35" t="s">
         <v>77</v>
@@ -39379,14 +39380,14 @@
       <c r="J38" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="K38" s="34" t="s">
-        <v>1036</v>
+      <c r="K38" s="106" t="s">
+        <v>1295</v>
       </c>
       <c r="L38" s="35" t="s">
-        <v>1278</v>
+        <v>1263</v>
       </c>
       <c r="M38" s="35" t="s">
-        <v>1279</v>
+        <v>1264</v>
       </c>
       <c r="N38" s="90"/>
     </row>
@@ -39448,7 +39449,7 @@
         <v>14</v>
       </c>
       <c r="K40" s="34" t="s">
-        <v>1037</v>
+        <v>1033</v>
       </c>
       <c r="L40" s="35" t="s">
         <v>95</v>
@@ -39465,13 +39466,13 @@
         <v>35</v>
       </c>
       <c r="E41" s="34" t="s">
-        <v>1280</v>
+        <v>1265</v>
       </c>
       <c r="F41" s="34" t="s">
-        <v>1281</v>
+        <v>1266</v>
       </c>
       <c r="G41" s="34" t="s">
-        <v>1282</v>
+        <v>1267</v>
       </c>
       <c r="H41" s="34" t="s">
         <v>10</v>
@@ -39482,14 +39483,14 @@
       <c r="J41" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="K41" s="34" t="s">
-        <v>1283</v>
+      <c r="K41" s="106" t="s">
+        <v>1287</v>
       </c>
       <c r="L41" s="35" t="s">
-        <v>1226</v>
+        <v>1211</v>
       </c>
       <c r="M41" s="35" t="s">
-        <v>1118</v>
+        <v>1104</v>
       </c>
       <c r="N41" s="98"/>
     </row>
@@ -39498,16 +39499,16 @@
       <c r="B42" s="15"/>
       <c r="C42" s="15"/>
       <c r="D42" s="56" t="s">
-        <v>1096</v>
+        <v>1082</v>
       </c>
       <c r="E42" s="34" t="s">
-        <v>1112</v>
+        <v>1098</v>
       </c>
       <c r="F42" s="34" t="s">
-        <v>1108</v>
+        <v>1094</v>
       </c>
       <c r="G42" s="34" t="s">
-        <v>1115</v>
+        <v>1101</v>
       </c>
       <c r="H42" s="34" t="s">
         <v>10</v>
@@ -39518,14 +39519,14 @@
       <c r="J42" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="K42" s="34" t="s">
-        <v>1120</v>
+      <c r="K42" s="106" t="s">
+        <v>1288</v>
       </c>
       <c r="L42" s="35" t="s">
-        <v>1227</v>
+        <v>1212</v>
       </c>
       <c r="M42" s="35" t="s">
-        <v>1109</v>
+        <v>1095</v>
       </c>
       <c r="N42" s="97"/>
     </row>
@@ -39534,16 +39535,16 @@
       <c r="B43" s="15"/>
       <c r="C43" s="15"/>
       <c r="D43" s="56" t="s">
+        <v>1082</v>
+      </c>
+      <c r="E43" s="34" t="s">
+        <v>1099</v>
+      </c>
+      <c r="F43" s="34" t="s">
         <v>1096</v>
       </c>
-      <c r="E43" s="34" t="s">
-        <v>1113</v>
-      </c>
-      <c r="F43" s="34" t="s">
-        <v>1110</v>
-      </c>
       <c r="G43" s="34" t="s">
-        <v>1116</v>
+        <v>1102</v>
       </c>
       <c r="H43" s="34" t="s">
         <v>10</v>
@@ -39554,14 +39555,14 @@
       <c r="J43" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="K43" s="34" t="s">
-        <v>1283</v>
+      <c r="K43" s="106" t="s">
+        <v>1287</v>
       </c>
       <c r="L43" s="35" t="s">
-        <v>1225</v>
+        <v>1210</v>
       </c>
       <c r="M43" s="35" t="s">
-        <v>1119</v>
+        <v>1105</v>
       </c>
       <c r="N43" s="98"/>
     </row>
@@ -39570,16 +39571,16 @@
       <c r="B44" s="15"/>
       <c r="C44" s="15"/>
       <c r="D44" s="56" t="s">
-        <v>1096</v>
+        <v>1082</v>
       </c>
       <c r="E44" s="34" t="s">
-        <v>1114</v>
+        <v>1100</v>
       </c>
       <c r="F44" s="34" t="s">
-        <v>1111</v>
+        <v>1097</v>
       </c>
       <c r="G44" s="34" t="s">
-        <v>1117</v>
+        <v>1103</v>
       </c>
       <c r="H44" s="34" t="s">
         <v>10</v>
@@ -39590,14 +39591,14 @@
       <c r="J44" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="K44" s="34" t="s">
-        <v>1120</v>
+      <c r="K44" s="106" t="s">
+        <v>1288</v>
       </c>
       <c r="L44" s="35" t="s">
-        <v>1228</v>
+        <v>1213</v>
       </c>
       <c r="M44" s="35" t="s">
-        <v>1229</v>
+        <v>1214</v>
       </c>
       <c r="N44" s="97"/>
     </row>
@@ -39638,7 +39639,7 @@
         <v>37</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>1190</v>
+        <v>1175</v>
       </c>
       <c r="F46" s="12" t="s">
         <v>567</v>
@@ -39655,8 +39656,8 @@
       <c r="J46" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="K46" s="15" t="s">
-        <v>1039</v>
+      <c r="K46" s="108" t="s">
+        <v>1289</v>
       </c>
       <c r="L46" s="12" t="s">
         <v>840</v>
@@ -39673,7 +39674,7 @@
         <v>38</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>1191</v>
+        <v>1176</v>
       </c>
       <c r="F47" s="12" t="s">
         <v>819</v>
@@ -39704,7 +39705,7 @@
         <v>39</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>1192</v>
+        <v>1177</v>
       </c>
       <c r="F48" s="15" t="s">
         <v>773</v>
@@ -39721,7 +39722,7 @@
       <c r="J48" s="15"/>
       <c r="K48" s="15"/>
       <c r="L48" s="12" t="s">
-        <v>1069</v>
+        <v>1057</v>
       </c>
       <c r="M48" s="12" t="s">
         <v>1002</v>
@@ -39815,7 +39816,7 @@
         <v>14</v>
       </c>
       <c r="K51" s="108" t="s">
-        <v>1303</v>
+        <v>1286</v>
       </c>
       <c r="L51" s="12" t="s">
         <v>138</v>
@@ -39863,7 +39864,7 @@
         <v>44</v>
       </c>
       <c r="E53" s="15" t="s">
-        <v>1169</v>
+        <v>1154</v>
       </c>
       <c r="F53" s="15" t="s">
         <v>332</v>
@@ -39879,7 +39880,7 @@
         <v>14</v>
       </c>
       <c r="K53" s="108" t="s">
-        <v>1303</v>
+        <v>1286</v>
       </c>
       <c r="L53" s="12" t="s">
         <v>524</v>
@@ -39896,7 +39897,7 @@
         <v>45</v>
       </c>
       <c r="E54" s="15" t="s">
-        <v>1170</v>
+        <v>1155</v>
       </c>
       <c r="F54" s="15" t="s">
         <v>820</v>
@@ -39927,7 +39928,7 @@
         <v>46</v>
       </c>
       <c r="E55" s="15" t="s">
-        <v>1171</v>
+        <v>1156</v>
       </c>
       <c r="F55" s="15" t="s">
         <v>774</v>
@@ -40036,7 +40037,7 @@
         <v>14</v>
       </c>
       <c r="K58" s="15" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="L58" s="12" t="s">
         <v>695</v>
@@ -40069,8 +40070,8 @@
       <c r="J59" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="K59" s="15" t="s">
-        <v>1020</v>
+      <c r="K59" s="108" t="s">
+        <v>1301</v>
       </c>
       <c r="L59" s="12" t="s">
         <v>255</v>
@@ -40199,8 +40200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:O33"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K24" activeCellId="1" sqref="K22 K24"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -40247,7 +40248,7 @@
         <v>7</v>
       </c>
       <c r="K1" s="25" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="L1" s="25" t="s">
         <v>8</v>
@@ -40413,13 +40414,13 @@
         <v>14</v>
       </c>
       <c r="K6" s="35" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="L6" s="35" t="s">
-        <v>1094</v>
+        <v>1080</v>
       </c>
       <c r="M6" s="35" t="s">
-        <v>1095</v>
+        <v>1081</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="24" x14ac:dyDescent="0.45">
@@ -40432,7 +40433,7 @@
         <v>4</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>1243</v>
+        <v>1228</v>
       </c>
       <c r="F7" s="34" t="s">
         <v>628</v>
@@ -40450,7 +40451,7 @@
         <v>632</v>
       </c>
       <c r="K7" s="34" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
       <c r="L7" s="59" t="s">
         <v>631</v>
@@ -40471,13 +40472,13 @@
         <v>5</v>
       </c>
       <c r="E8" s="35" t="s">
-        <v>1241</v>
+        <v>1226</v>
       </c>
       <c r="F8" s="34" t="s">
-        <v>1239</v>
+        <v>1224</v>
       </c>
       <c r="G8" s="34" t="s">
-        <v>1240</v>
+        <v>1225</v>
       </c>
       <c r="H8" s="34" t="s">
         <v>10</v>
@@ -40503,7 +40504,7 @@
         <v>6</v>
       </c>
       <c r="E9" s="34" t="s">
-        <v>1242</v>
+        <v>1227</v>
       </c>
       <c r="F9" s="34" t="s">
         <v>432</v>
@@ -40521,7 +40522,7 @@
         <v>14</v>
       </c>
       <c r="K9" s="102" t="s">
-        <v>1040</v>
+        <v>1035</v>
       </c>
       <c r="L9" s="35" t="s">
         <v>151</v>
@@ -40604,7 +40605,7 @@
         <v>9</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>1194</v>
+        <v>1179</v>
       </c>
       <c r="F12" s="35" t="s">
         <v>756</v>
@@ -40621,7 +40622,7 @@
       <c r="J12" s="34"/>
       <c r="K12" s="34"/>
       <c r="L12" s="35" t="s">
-        <v>1260</v>
+        <v>1245</v>
       </c>
       <c r="M12" s="35" t="s">
         <v>120</v>
@@ -40653,7 +40654,7 @@
         <v>14</v>
       </c>
       <c r="K13" s="34" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="L13" s="35" t="s">
         <v>262</v>
@@ -40670,7 +40671,7 @@
         <v>11</v>
       </c>
       <c r="E14" s="34" t="s">
-        <v>1173</v>
+        <v>1158</v>
       </c>
       <c r="F14" s="34" t="s">
         <v>359</v>
@@ -40718,8 +40719,8 @@
       <c r="J15" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="K15" s="34" t="s">
-        <v>1019</v>
+      <c r="K15" s="106" t="s">
+        <v>256</v>
       </c>
       <c r="L15" s="35" t="s">
         <v>829</v>
@@ -40771,7 +40772,7 @@
         <v>14</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>1195</v>
+        <v>1180</v>
       </c>
       <c r="F17" s="34" t="s">
         <v>430</v>
@@ -40802,7 +40803,7 @@
         <v>15</v>
       </c>
       <c r="E18" s="34" t="s">
-        <v>1196</v>
+        <v>1181</v>
       </c>
       <c r="F18" s="35" t="s">
         <v>821</v>
@@ -40833,7 +40834,7 @@
         <v>16</v>
       </c>
       <c r="E19" s="34" t="s">
-        <v>1197</v>
+        <v>1182</v>
       </c>
       <c r="F19" s="34" t="s">
         <v>775</v>
@@ -40944,7 +40945,7 @@
         <v>14</v>
       </c>
       <c r="K22" s="106" t="s">
-        <v>1303</v>
+        <v>1286</v>
       </c>
       <c r="L22" s="35" t="s">
         <v>150</v>
@@ -40992,7 +40993,7 @@
         <v>21</v>
       </c>
       <c r="E24" s="34" t="s">
-        <v>1169</v>
+        <v>1154</v>
       </c>
       <c r="F24" s="34" t="s">
         <v>336</v>
@@ -41010,7 +41011,7 @@
         <v>14</v>
       </c>
       <c r="K24" s="106" t="s">
-        <v>1303</v>
+        <v>1286</v>
       </c>
       <c r="L24" s="35" t="s">
         <v>524</v>
@@ -41027,7 +41028,7 @@
         <v>22</v>
       </c>
       <c r="E25" s="34" t="s">
-        <v>1170</v>
+        <v>1155</v>
       </c>
       <c r="F25" s="34" t="s">
         <v>822</v>
@@ -41058,7 +41059,7 @@
         <v>23</v>
       </c>
       <c r="E26" s="34" t="s">
-        <v>1171</v>
+        <v>1156</v>
       </c>
       <c r="F26" s="34" t="s">
         <v>776</v>
@@ -41167,10 +41168,10 @@
         <v>14</v>
       </c>
       <c r="K29" s="34" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="L29" s="35" t="s">
-        <v>1041</v>
+        <v>1036</v>
       </c>
       <c r="M29" s="34"/>
     </row>
@@ -41199,8 +41200,8 @@
       <c r="J30" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="K30" s="34" t="s">
-        <v>1020</v>
+      <c r="K30" s="106" t="s">
+        <v>1301</v>
       </c>
       <c r="L30" s="35" t="s">
         <v>255</v>
@@ -41220,27 +41221,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
-    <TaxCatchAllLabel xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
-    <TaxKeywordTaxHTField xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </TaxKeywordTaxHTField>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100584B29A9F606E64BBE0B94B46ABEDBD5" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ad12f995843361ff338b3798f1f5f41c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4d5313c0-c1e6-4122-afa9-da1ccdba405d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8fda66a02b6b5d1f39f2000ab0f58af4" ns2:_="">
     <xsd:import namespace="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
@@ -41412,31 +41392,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04CD8B6C-25F0-471A-A724-387AC1B5060F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60949D59-0B5B-44ED-ACEF-9231A5F5D889}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
+    <TaxCatchAllLabel xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
+    <TaxKeywordTaxHTField xmlns="4d5313c0-c1e6-4122-afa9-da1ccdba405d">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </TaxKeywordTaxHTField>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F67F35D-1CDD-4110-B6CE-1A6865489AEE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -41452,4 +41429,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04CD8B6C-25F0-471A-A724-387AC1B5060F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{60949D59-0B5B-44ED-ACEF-9231A5F5D889}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Ver 1.19.5. BiologicalMeasurementType replaces RS_AddGrpMeasurementType
For the field ‘FMaddGrpMeasurementType’ in the FM table the code type BiologicalMeasurementType replaces RS_AddGrpMeasurementType.
</commit_message>
<xml_diff>
--- a/Documents/RDBES Data Model.xlsx
+++ b/Documents/RDBES Data Model.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20376"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20377"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Profile\Henrik K\Documents\GitHub\RDBES_Core_Group\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{621ADA0C-6EAA-4B1A-94B6-119EA333811E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1874A91F-65D3-403E-BA3A-4CB64EAD759F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="17430" windowHeight="5595" tabRatio="781" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="17430" windowHeight="5595" tabRatio="781" firstSheet="1" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Model v1.19.3" sheetId="1" r:id="rId1"/>
+    <sheet name="Model v1.19.5" sheetId="1" r:id="rId1"/>
     <sheet name="Design" sheetId="5" r:id="rId2"/>
     <sheet name="Temporal Event" sheetId="21" r:id="rId3"/>
     <sheet name="Location" sheetId="20" r:id="rId4"/>
@@ -181,7 +181,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3403" uniqueCount="1303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3403" uniqueCount="1300">
   <si>
     <t>Design Table (DE)</t>
   </si>
@@ -3318,9 +3318,6 @@
     <t>TargetSpecies</t>
   </si>
   <si>
-    <t>RS_incidentialByCatchMitigateD</t>
-  </si>
-  <si>
     <t>RS_LocationType</t>
   </si>
   <si>
@@ -3345,16 +3342,10 @@
     <t>RS_CommercialSizeCategory</t>
   </si>
   <si>
-    <t>RS_Sex</t>
-  </si>
-  <si>
     <t>RS_LowerHierarchy</t>
   </si>
   <si>
     <t>RS_AccuracyCode</t>
-  </si>
-  <si>
-    <t>RS_AddGrpMeasurementType</t>
   </si>
   <si>
     <t>RS_LEfullTripAvailable</t>
@@ -4063,9 +4054,6 @@
     <t>SAconFacMeasLive</t>
   </si>
   <si>
-    <t>RS_StateOfProcessing</t>
-  </si>
-  <si>
     <t>The stratum of this sample, 'U' if unstratified. Name should be as concise and meaningful as possible.</t>
   </si>
   <si>
@@ -4145,6 +4133,9 @@
   </si>
   <si>
     <t>BiologicalMeasurementType</t>
+  </si>
+  <si>
+    <t>SEXCO</t>
   </si>
 </sst>
 </file>
@@ -5008,7 +4999,7 @@
     </row>
     <row r="2" spans="1:35" ht="21" x14ac:dyDescent="0.65">
       <c r="B2" s="105" t="s">
-        <v>1285</v>
+        <v>1281</v>
       </c>
       <c r="D2" s="19"/>
       <c r="L2" s="17"/>
@@ -7214,7 +7205,7 @@
         <v>Conversion factor between measured weight and live weight.</v>
       </c>
     </row>
-    <row r="32" spans="9:35" x14ac:dyDescent="0.5">
+    <row r="32" spans="9:35" ht="31.5" x14ac:dyDescent="0.5">
       <c r="I32" s="17">
         <f>IF(ISBLANK(Location!A4)=TRUE, Location!B4, "")</f>
         <v>0</v>
@@ -7660,7 +7651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="8:27" x14ac:dyDescent="0.5">
+    <row r="41" spans="8:27" ht="31.5" x14ac:dyDescent="0.5">
       <c r="H41" s="48"/>
       <c r="I41" s="48">
         <f>IF(ISBLANK(Location!A27)=TRUE, Location!B27, "")</f>
@@ -7705,7 +7696,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="8:27" x14ac:dyDescent="0.5">
+    <row r="42" spans="8:27" ht="31.5" x14ac:dyDescent="0.5">
       <c r="H42" s="48"/>
       <c r="I42" s="48"/>
       <c r="J42" s="42" t="str">
@@ -8432,7 +8423,7 @@
       <c r="Y64" s="19"/>
       <c r="Z64" s="19"/>
     </row>
-    <row r="65" spans="10:26" x14ac:dyDescent="0.5">
+    <row r="65" spans="10:26" ht="31.5" x14ac:dyDescent="0.5">
       <c r="J65" s="43" t="str">
         <f>IF(ISBLANK(Location!A18)=TRUE, Location!F18, "")</f>
         <v>LOselectionMethod</v>
@@ -9141,8 +9132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:XFC62"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K54" sqref="K54"/>
+    <sheetView topLeftCell="A33" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -9157,7 +9148,7 @@
     <col min="8" max="8" width="13.3984375" style="16" customWidth="1"/>
     <col min="9" max="9" width="9.1328125" style="16" customWidth="1"/>
     <col min="10" max="10" width="20.73046875" style="16" customWidth="1"/>
-    <col min="11" max="11" width="20.73046875" style="81" customWidth="1"/>
+    <col min="11" max="11" width="26.86328125" style="81" customWidth="1"/>
     <col min="12" max="12" width="63.1328125" style="13" customWidth="1"/>
     <col min="13" max="13" width="57.1328125" style="13" customWidth="1"/>
     <col min="14" max="14" width="25.3984375" style="2" bestFit="1" customWidth="1"/>
@@ -9535,7 +9526,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>1160</v>
+        <v>1157</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>929</v>
@@ -9550,11 +9541,11 @@
         <v>11</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="K11" s="12"/>
       <c r="L11" s="12" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
       <c r="M11" s="12" t="s">
         <v>577</v>
@@ -9590,10 +9581,10 @@
         <v>1014</v>
       </c>
       <c r="L12" s="35" t="s">
-        <v>1080</v>
+        <v>1077</v>
       </c>
       <c r="M12" s="35" t="s">
-        <v>1081</v>
+        <v>1078</v>
       </c>
       <c r="N12" s="51"/>
     </row>
@@ -9656,10 +9647,10 @@
       <c r="J14" s="35"/>
       <c r="K14" s="34"/>
       <c r="L14" s="35" t="s">
-        <v>1268</v>
+        <v>1265</v>
       </c>
       <c r="M14" s="35" t="s">
-        <v>1268</v>
+        <v>1265</v>
       </c>
       <c r="N14" s="101"/>
     </row>
@@ -9671,7 +9662,7 @@
         <v>6</v>
       </c>
       <c r="E15" s="35" t="s">
-        <v>1183</v>
+        <v>1180</v>
       </c>
       <c r="F15" s="35" t="s">
         <v>757</v>
@@ -9688,10 +9679,10 @@
       <c r="J15" s="35"/>
       <c r="K15" s="34"/>
       <c r="L15" s="35" t="s">
-        <v>1269</v>
+        <v>1266</v>
       </c>
       <c r="M15" s="35" t="s">
-        <v>1270</v>
+        <v>1267</v>
       </c>
       <c r="N15" s="51"/>
     </row>
@@ -9739,7 +9730,7 @@
         <v>8</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>1158</v>
+        <v>1155</v>
       </c>
       <c r="F17" s="34" t="s">
         <v>362</v>
@@ -9879,13 +9870,13 @@
         <v>12</v>
       </c>
       <c r="E21" s="35" t="s">
-        <v>1271</v>
+        <v>1268</v>
       </c>
       <c r="F21" s="35" t="s">
-        <v>1216</v>
+        <v>1213</v>
       </c>
       <c r="G21" s="35" t="s">
-        <v>1216</v>
+        <v>1213</v>
       </c>
       <c r="H21" s="35" t="s">
         <v>10</v>
@@ -9909,19 +9900,19 @@
       <c r="A22" s="12"/>
       <c r="B22" s="12"/>
       <c r="C22" s="35" t="s">
-        <v>1082</v>
+        <v>1079</v>
       </c>
       <c r="D22" s="35">
         <v>13</v>
       </c>
       <c r="E22" s="35" t="s">
-        <v>1217</v>
+        <v>1214</v>
       </c>
       <c r="F22" s="35" t="s">
-        <v>1218</v>
+        <v>1215</v>
       </c>
       <c r="G22" s="35" t="s">
-        <v>1223</v>
+        <v>1220</v>
       </c>
       <c r="H22" s="35" t="s">
         <v>10</v>
@@ -9961,7 +9952,7 @@
         <v>14</v>
       </c>
       <c r="K23" s="34" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="L23" s="35" t="s">
         <v>78</v>
@@ -10000,7 +9991,7 @@
         <v>1003</v>
       </c>
       <c r="L24" s="35" t="s">
-        <v>1058</v>
+        <v>1055</v>
       </c>
       <c r="M24" s="35" t="s">
         <v>158</v>
@@ -10079,7 +10070,7 @@
         <v>18</v>
       </c>
       <c r="E27" s="35" t="s">
-        <v>1174</v>
+        <v>1171</v>
       </c>
       <c r="F27" s="34" t="s">
         <v>932</v>
@@ -10172,7 +10163,7 @@
         <v>1026</v>
       </c>
       <c r="L29" s="35" t="s">
-        <v>1059</v>
+        <v>1056</v>
       </c>
       <c r="M29" s="35" t="s">
         <v>162</v>
@@ -10208,10 +10199,10 @@
         <v>1027</v>
       </c>
       <c r="L30" s="35" t="s">
-        <v>1054</v>
+        <v>1051</v>
       </c>
       <c r="M30" s="35" t="s">
-        <v>1054</v>
+        <v>1051</v>
       </c>
       <c r="N30" s="66"/>
     </row>
@@ -10244,7 +10235,7 @@
         <v>1028</v>
       </c>
       <c r="L31" s="34" t="s">
-        <v>1060</v>
+        <v>1057</v>
       </c>
       <c r="M31" s="34" t="s">
         <v>846</v>
@@ -10280,7 +10271,7 @@
         <v>1029</v>
       </c>
       <c r="L32" s="35" t="s">
-        <v>1061</v>
+        <v>1058</v>
       </c>
       <c r="M32" s="35" t="s">
         <v>612</v>
@@ -10453,7 +10444,7 @@
         <v>14</v>
       </c>
       <c r="K37" s="106" t="s">
-        <v>1295</v>
+        <v>1291</v>
       </c>
       <c r="L37" s="35" t="s">
         <v>877</v>
@@ -10556,8 +10547,8 @@
       <c r="J40" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="K40" s="34" t="s">
-        <v>1034</v>
+      <c r="K40" s="106" t="s">
+        <v>1283</v>
       </c>
       <c r="L40" s="35" t="s">
         <v>879</v>
@@ -10603,7 +10594,7 @@
         <v>33</v>
       </c>
       <c r="E42" s="35" t="s">
-        <v>1184</v>
+        <v>1181</v>
       </c>
       <c r="F42" s="35" t="s">
         <v>823</v>
@@ -10635,7 +10626,7 @@
         <v>34</v>
       </c>
       <c r="E43" s="35" t="s">
-        <v>1185</v>
+        <v>1182</v>
       </c>
       <c r="F43" s="34" t="s">
         <v>777</v>
@@ -10749,7 +10740,7 @@
         <v>14</v>
       </c>
       <c r="K46" s="106" t="s">
-        <v>1286</v>
+        <v>1282</v>
       </c>
       <c r="L46" s="35" t="s">
         <v>163</v>
@@ -10799,7 +10790,7 @@
         <v>39</v>
       </c>
       <c r="E48" s="34" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
       <c r="F48" s="34" t="s">
         <v>341</v>
@@ -10817,7 +10808,7 @@
         <v>14</v>
       </c>
       <c r="K48" s="106" t="s">
-        <v>1286</v>
+        <v>1282</v>
       </c>
       <c r="L48" s="35" t="s">
         <v>524</v>
@@ -10827,7 +10818,7 @@
       </c>
       <c r="N48" s="51"/>
     </row>
-    <row r="49" spans="1:16383" ht="24" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:16383" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A49" s="12"/>
       <c r="B49" s="12"/>
       <c r="C49" s="35"/>
@@ -10835,7 +10826,7 @@
         <v>40</v>
       </c>
       <c r="E49" s="34" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
       <c r="F49" s="34" t="s">
         <v>824</v>
@@ -10867,7 +10858,7 @@
         <v>41</v>
       </c>
       <c r="E50" s="34" t="s">
-        <v>1156</v>
+        <v>1153</v>
       </c>
       <c r="F50" s="34" t="s">
         <v>778</v>
@@ -11012,7 +11003,7 @@
         <v>14</v>
       </c>
       <c r="K54" s="106" t="s">
-        <v>1301</v>
+        <v>1297</v>
       </c>
       <c r="L54" s="35" t="s">
         <v>255</v>
@@ -11048,7 +11039,7 @@
         <v>14</v>
       </c>
       <c r="K55" s="34" t="s">
-        <v>1047</v>
+        <v>1044</v>
       </c>
       <c r="L55" s="35" t="s">
         <v>544</v>
@@ -27953,10 +27944,10 @@
         <v>1014</v>
       </c>
       <c r="L11" s="35" t="s">
-        <v>1080</v>
+        <v>1077</v>
       </c>
       <c r="M11" s="35" t="s">
-        <v>1081</v>
+        <v>1078</v>
       </c>
       <c r="N11" s="63"/>
       <c r="O11" s="63"/>
@@ -27971,7 +27962,7 @@
         <v>4</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>1186</v>
+        <v>1183</v>
       </c>
       <c r="F12" s="34" t="s">
         <v>967</v>
@@ -27989,7 +27980,7 @@
         <v>14</v>
       </c>
       <c r="K12" s="34" t="s">
-        <v>1293</v>
+        <v>1289</v>
       </c>
       <c r="L12" s="35" t="s">
         <v>839</v>
@@ -28010,7 +28001,7 @@
         <v>5</v>
       </c>
       <c r="E13" s="56" t="s">
-        <v>1187</v>
+        <v>1184</v>
       </c>
       <c r="F13" s="56" t="s">
         <v>685</v>
@@ -28026,7 +28017,7 @@
       </c>
       <c r="J13" s="49"/>
       <c r="K13" s="34" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="L13" s="70" t="s">
         <v>882</v>
@@ -28047,7 +28038,7 @@
         <v>6</v>
       </c>
       <c r="E14" s="56" t="s">
-        <v>1188</v>
+        <v>1185</v>
       </c>
       <c r="F14" s="56" t="s">
         <v>966</v>
@@ -28065,7 +28056,7 @@
         <v>14</v>
       </c>
       <c r="K14" s="106" t="s">
-        <v>1291</v>
+        <v>1287</v>
       </c>
       <c r="L14" s="70" t="s">
         <v>565</v>
@@ -28084,7 +28075,7 @@
         <v>7</v>
       </c>
       <c r="E15" s="49" t="s">
-        <v>1189</v>
+        <v>1186</v>
       </c>
       <c r="F15" s="35" t="s">
         <v>758</v>
@@ -28101,7 +28092,7 @@
       <c r="J15" s="49"/>
       <c r="K15" s="34"/>
       <c r="L15" s="49" t="s">
-        <v>1272</v>
+        <v>1269</v>
       </c>
       <c r="M15" s="35" t="s">
         <v>120</v>
@@ -28154,7 +28145,7 @@
         <v>9</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>1158</v>
+        <v>1155</v>
       </c>
       <c r="F17" s="34" t="s">
         <v>365</v>
@@ -28224,7 +28215,7 @@
         <v>11</v>
       </c>
       <c r="E19" s="49" t="s">
-        <v>1190</v>
+        <v>1187</v>
       </c>
       <c r="F19" s="49" t="s">
         <v>968</v>
@@ -28259,7 +28250,7 @@
         <v>12</v>
       </c>
       <c r="E20" s="49" t="s">
-        <v>1191</v>
+        <v>1188</v>
       </c>
       <c r="F20" s="49" t="s">
         <v>592</v>
@@ -28294,7 +28285,7 @@
         <v>13</v>
       </c>
       <c r="E21" s="49" t="s">
-        <v>1192</v>
+        <v>1189</v>
       </c>
       <c r="F21" s="35" t="s">
         <v>825</v>
@@ -28327,7 +28318,7 @@
         <v>14</v>
       </c>
       <c r="E22" s="49" t="s">
-        <v>1193</v>
+        <v>1190</v>
       </c>
       <c r="F22" s="34" t="s">
         <v>779</v>
@@ -28426,7 +28417,7 @@
         <v>17</v>
       </c>
       <c r="E25" s="49" t="s">
-        <v>1194</v>
+        <v>1191</v>
       </c>
       <c r="F25" s="56" t="s">
         <v>413</v>
@@ -28444,7 +28435,7 @@
         <v>14</v>
       </c>
       <c r="K25" s="108" t="s">
-        <v>1286</v>
+        <v>1282</v>
       </c>
       <c r="L25" s="35" t="s">
         <v>211</v>
@@ -28496,7 +28487,7 @@
         <v>19</v>
       </c>
       <c r="E27" s="34" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
       <c r="F27" s="34" t="s">
         <v>345</v>
@@ -28514,7 +28505,7 @@
         <v>14</v>
       </c>
       <c r="K27" s="108" t="s">
-        <v>1286</v>
+        <v>1282</v>
       </c>
       <c r="L27" s="35" t="s">
         <v>524</v>
@@ -28533,7 +28524,7 @@
         <v>20</v>
       </c>
       <c r="E28" s="34" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
       <c r="F28" s="34" t="s">
         <v>826</v>
@@ -28566,7 +28557,7 @@
         <v>21</v>
       </c>
       <c r="E29" s="34" t="s">
-        <v>1156</v>
+        <v>1153</v>
       </c>
       <c r="F29" s="34" t="s">
         <v>780</v>
@@ -28714,7 +28705,7 @@
         <v>14</v>
       </c>
       <c r="K33" s="108" t="s">
-        <v>1301</v>
+        <v>1297</v>
       </c>
       <c r="L33" s="35" t="s">
         <v>255</v>
@@ -28856,8 +28847,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:V61"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K44" sqref="K44"/>
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -29078,7 +29069,7 @@
         <v>3</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>1195</v>
+        <v>1192</v>
       </c>
       <c r="F6" s="12" t="s">
         <v>673</v>
@@ -29139,10 +29130,10 @@
         <v>1014</v>
       </c>
       <c r="L7" s="35" t="s">
-        <v>1080</v>
+        <v>1077</v>
       </c>
       <c r="M7" s="35" t="s">
-        <v>1081</v>
+        <v>1078</v>
       </c>
       <c r="N7" s="51"/>
       <c r="O7" s="60"/>
@@ -29179,7 +29170,7 @@
       <c r="J8" s="56"/>
       <c r="K8" s="56"/>
       <c r="L8" s="35" t="s">
-        <v>1276</v>
+        <v>1272</v>
       </c>
       <c r="M8" s="35" t="s">
         <v>98</v>
@@ -29222,7 +29213,7 @@
         <v>14</v>
       </c>
       <c r="K9" s="11" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="L9" s="12" t="s">
         <v>584</v>
@@ -29268,7 +29259,7 @@
         <v>14</v>
       </c>
       <c r="K10" s="11" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="L10" s="12" t="s">
         <v>997</v>
@@ -29289,18 +29280,18 @@
     <row r="11" spans="1:22" s="51" customFormat="1" ht="24" x14ac:dyDescent="0.45">
       <c r="A11" s="35"/>
       <c r="B11" s="56" t="s">
-        <v>1082</v>
+        <v>1079</v>
       </c>
       <c r="C11" s="56"/>
       <c r="D11" s="52"/>
       <c r="E11" s="56" t="s">
-        <v>1111</v>
+        <v>1108</v>
       </c>
       <c r="F11" s="56" t="s">
-        <v>1279</v>
+        <v>1275</v>
       </c>
       <c r="G11" s="56" t="s">
-        <v>1280</v>
+        <v>1276</v>
       </c>
       <c r="H11" s="56" t="s">
         <v>10</v>
@@ -29312,10 +29303,10 @@
         <v>14</v>
       </c>
       <c r="K11" s="111" t="s">
-        <v>1294</v>
+        <v>1290</v>
       </c>
       <c r="L11" s="35" t="s">
-        <v>1113</v>
+        <v>1110</v>
       </c>
       <c r="M11" s="35"/>
     </row>
@@ -29350,7 +29341,7 @@
         <v>22</v>
       </c>
       <c r="L12" s="35" t="s">
-        <v>1115</v>
+        <v>1112</v>
       </c>
       <c r="M12" s="35" t="s">
         <v>171</v>
@@ -29364,7 +29355,7 @@
         <v>9</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>1196</v>
+        <v>1193</v>
       </c>
       <c r="F13" s="11" t="s">
         <v>560</v>
@@ -29382,7 +29373,7 @@
         <v>14</v>
       </c>
       <c r="K13" s="110" t="s">
-        <v>1300</v>
+        <v>1296</v>
       </c>
       <c r="L13" s="87" t="s">
         <v>884</v>
@@ -29410,7 +29401,7 @@
         <v>10</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>1197</v>
+        <v>1194</v>
       </c>
       <c r="F14" s="11" t="s">
         <v>548</v>
@@ -29428,7 +29419,7 @@
         <v>14</v>
       </c>
       <c r="K14" s="11" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="L14" s="87" t="s">
         <v>697</v>
@@ -29474,7 +29465,7 @@
         <v>14</v>
       </c>
       <c r="K15" s="11" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="L15" s="12" t="s">
         <v>835</v>
@@ -29520,7 +29511,7 @@
         <v>14</v>
       </c>
       <c r="K16" s="110" t="s">
-        <v>1297</v>
+        <v>1293</v>
       </c>
       <c r="L16" s="12" t="s">
         <v>173</v>
@@ -29566,7 +29557,7 @@
         <v>14</v>
       </c>
       <c r="K17" s="11" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="L17" s="12" t="s">
         <v>19</v>
@@ -29611,11 +29602,11 @@
       <c r="J18" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="K18" s="11" t="s">
-        <v>1043</v>
+      <c r="K18" s="110" t="s">
+        <v>1299</v>
       </c>
       <c r="L18" s="12" t="s">
-        <v>1062</v>
+        <v>1059</v>
       </c>
       <c r="M18" s="12" t="s">
         <v>20</v>
@@ -29638,7 +29629,7 @@
         <v>15</v>
       </c>
       <c r="E19" s="95" t="s">
-        <v>1174</v>
+        <v>1171</v>
       </c>
       <c r="F19" s="95" t="s">
         <v>861</v>
@@ -29747,7 +29738,7 @@
         <v>1026</v>
       </c>
       <c r="L21" s="12" t="s">
-        <v>1063</v>
+        <v>1060</v>
       </c>
       <c r="M21" s="12" t="s">
         <v>162</v>
@@ -29791,10 +29782,10 @@
         <v>1027</v>
       </c>
       <c r="L22" s="12" t="s">
-        <v>1054</v>
+        <v>1051</v>
       </c>
       <c r="M22" s="12" t="s">
-        <v>1054</v>
+        <v>1051</v>
       </c>
       <c r="N22" s="51"/>
       <c r="O22" s="51"/>
@@ -29835,7 +29826,7 @@
         <v>1028</v>
       </c>
       <c r="L23" s="12" t="s">
-        <v>1055</v>
+        <v>1052</v>
       </c>
       <c r="M23" s="12" t="s">
         <v>846</v>
@@ -29850,7 +29841,7 @@
       <c r="U23" s="51"/>
       <c r="V23" s="51"/>
     </row>
-    <row r="24" spans="1:22" s="23" customFormat="1" ht="82.15" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:22" s="23" customFormat="1" ht="93.75" x14ac:dyDescent="0.45">
       <c r="A24" s="12"/>
       <c r="B24" s="12"/>
       <c r="C24" s="12"/>
@@ -29879,7 +29870,7 @@
         <v>1029</v>
       </c>
       <c r="L24" s="12" t="s">
-        <v>1064</v>
+        <v>1061</v>
       </c>
       <c r="M24" s="12" t="s">
         <v>612</v>
@@ -30092,7 +30083,7 @@
         <v>14</v>
       </c>
       <c r="K29" s="110" t="s">
-        <v>1295</v>
+        <v>1291</v>
       </c>
       <c r="L29" s="12" t="s">
         <v>718</v>
@@ -30150,7 +30141,7 @@
       <c r="U30" s="51"/>
       <c r="V30" s="51"/>
     </row>
-    <row r="31" spans="1:22" ht="35.65" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:22" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A31" s="12"/>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
@@ -30176,7 +30167,7 @@
         <v>14</v>
       </c>
       <c r="K31" s="110" t="s">
-        <v>1292</v>
+        <v>1288</v>
       </c>
       <c r="L31" s="12" t="s">
         <v>683</v>
@@ -30202,7 +30193,7 @@
         <v>28</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>1198</v>
+        <v>1195</v>
       </c>
       <c r="F32" s="11" t="s">
         <v>538</v>
@@ -30219,7 +30210,7 @@
       <c r="J32" s="11"/>
       <c r="K32" s="11"/>
       <c r="L32" s="12" t="s">
-        <v>1065</v>
+        <v>1062</v>
       </c>
       <c r="M32" s="12" t="s">
         <v>176</v>
@@ -30242,7 +30233,7 @@
         <v>29</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>1201</v>
+        <v>1198</v>
       </c>
       <c r="F33" s="11" t="s">
         <v>537</v>
@@ -30259,7 +30250,7 @@
       <c r="J33" s="11"/>
       <c r="K33" s="11"/>
       <c r="L33" s="12" t="s">
-        <v>1066</v>
+        <v>1063</v>
       </c>
       <c r="M33" s="12" t="s">
         <v>177</v>
@@ -30282,7 +30273,7 @@
         <v>30</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>1199</v>
+        <v>1196</v>
       </c>
       <c r="F34" s="12" t="s">
         <v>827</v>
@@ -30322,7 +30313,7 @@
         <v>31</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>1200</v>
+        <v>1197</v>
       </c>
       <c r="F35" s="15" t="s">
         <v>781</v>
@@ -30460,7 +30451,7 @@
         <v>14</v>
       </c>
       <c r="K38" s="110" t="s">
-        <v>1286</v>
+        <v>1282</v>
       </c>
       <c r="L38" s="12" t="s">
         <v>180</v>
@@ -30526,7 +30517,7 @@
         <v>36</v>
       </c>
       <c r="E40" s="11" t="s">
-        <v>1202</v>
+        <v>1199</v>
       </c>
       <c r="F40" s="11" t="s">
         <v>515</v>
@@ -30544,7 +30535,7 @@
         <v>14</v>
       </c>
       <c r="K40" s="11" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="L40" s="12" t="s">
         <v>181</v>
@@ -30665,7 +30656,7 @@
         <v>14</v>
       </c>
       <c r="K43" s="110" t="s">
-        <v>1301</v>
+        <v>1297</v>
       </c>
       <c r="L43" s="12" t="s">
         <v>687</v>
@@ -30709,7 +30700,7 @@
         <v>14</v>
       </c>
       <c r="K44" s="110" t="s">
-        <v>1301</v>
+        <v>1297</v>
       </c>
       <c r="L44" s="11" t="s">
         <v>688</v>
@@ -30735,7 +30726,7 @@
         <v>41</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>1203</v>
+        <v>1200</v>
       </c>
       <c r="F45" s="11" t="s">
         <v>532</v>
@@ -30775,7 +30766,7 @@
         <v>42</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>1204</v>
+        <v>1201</v>
       </c>
       <c r="F46" s="11" t="s">
         <v>533</v>
@@ -30807,7 +30798,7 @@
       <c r="U46" s="51"/>
       <c r="V46" s="51"/>
     </row>
-    <row r="47" spans="1:22" ht="24" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:22" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A47" s="12"/>
       <c r="B47" s="11"/>
       <c r="C47" s="11"/>
@@ -30815,13 +30806,13 @@
         <v>43</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>1205</v>
+        <v>1202</v>
       </c>
       <c r="F47" s="56" t="s">
-        <v>1273</v>
+        <v>1270</v>
       </c>
       <c r="G47" s="56" t="s">
-        <v>1274</v>
+        <v>1271</v>
       </c>
       <c r="H47" s="11" t="s">
         <v>148</v>
@@ -31181,8 +31172,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:V17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -31345,20 +31336,20 @@
     <row r="5" spans="1:22" s="23" customFormat="1" ht="58.9" x14ac:dyDescent="0.45">
       <c r="A5" s="45"/>
       <c r="B5" s="56" t="s">
-        <v>1240</v>
+        <v>1237</v>
       </c>
       <c r="C5" s="56"/>
       <c r="D5" s="52">
         <v>2</v>
       </c>
       <c r="E5" s="56" t="s">
-        <v>1111</v>
+        <v>1108</v>
       </c>
       <c r="F5" s="56" t="s">
-        <v>1281</v>
+        <v>1277</v>
       </c>
       <c r="G5" s="56" t="s">
-        <v>1282</v>
+        <v>1278</v>
       </c>
       <c r="H5" s="56" t="s">
         <v>10</v>
@@ -31369,20 +31360,20 @@
       <c r="J5" s="56" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="56" t="s">
-        <v>1275</v>
+      <c r="K5" s="111" t="s">
+        <v>1290</v>
       </c>
       <c r="L5" s="35" t="s">
-        <v>1229</v>
+        <v>1226</v>
       </c>
       <c r="M5" s="35" t="s">
-        <v>1111</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="6" spans="1:22" s="2" customFormat="1" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A6" s="12"/>
       <c r="B6" s="56" t="s">
-        <v>1240</v>
+        <v>1237</v>
       </c>
       <c r="C6" s="56"/>
       <c r="D6" s="52">
@@ -31392,10 +31383,10 @@
         <v>22</v>
       </c>
       <c r="F6" s="56" t="s">
-        <v>1109</v>
+        <v>1106</v>
       </c>
       <c r="G6" s="56" t="s">
-        <v>1110</v>
+        <v>1107</v>
       </c>
       <c r="H6" s="56" t="s">
         <v>10</v>
@@ -31410,10 +31401,10 @@
         <v>22</v>
       </c>
       <c r="L6" s="35" t="s">
-        <v>1114</v>
+        <v>1111</v>
       </c>
       <c r="M6" s="35" t="s">
-        <v>1112</v>
+        <v>1109</v>
       </c>
       <c r="N6" s="51"/>
       <c r="O6" s="51"/>
@@ -31435,13 +31426,13 @@
         <v>4</v>
       </c>
       <c r="E7" s="56" t="s">
-        <v>1120</v>
+        <v>1117</v>
       </c>
       <c r="F7" s="56" t="s">
-        <v>1118</v>
+        <v>1115</v>
       </c>
       <c r="G7" s="56" t="s">
-        <v>1119</v>
+        <v>1116</v>
       </c>
       <c r="H7" s="56" t="s">
         <v>13</v>
@@ -31452,7 +31443,7 @@
       <c r="J7" s="56"/>
       <c r="K7" s="35"/>
       <c r="L7" s="35" t="s">
-        <v>1121</v>
+        <v>1118</v>
       </c>
       <c r="M7" s="35" t="s">
         <v>552</v>
@@ -31497,13 +31488,13 @@
         <v>6</v>
       </c>
       <c r="E9" s="56" t="s">
-        <v>1122</v>
+        <v>1119</v>
       </c>
       <c r="F9" s="56" t="s">
-        <v>1123</v>
+        <v>1120</v>
       </c>
       <c r="G9" s="56" t="s">
-        <v>1124</v>
+        <v>1121</v>
       </c>
       <c r="H9" s="56" t="s">
         <v>10</v>
@@ -31515,10 +31506,10 @@
         <v>14</v>
       </c>
       <c r="K9" s="107" t="s">
-        <v>1302</v>
+        <v>1298</v>
       </c>
       <c r="L9" s="35" t="s">
-        <v>1131</v>
+        <v>1128</v>
       </c>
       <c r="M9" s="35" t="s">
         <v>441</v>
@@ -31527,7 +31518,7 @@
     <row r="10" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A10" s="56"/>
       <c r="B10" s="56" t="s">
-        <v>1240</v>
+        <v>1237</v>
       </c>
       <c r="C10" s="56"/>
       <c r="D10" s="52">
@@ -31537,10 +31528,10 @@
         <v>197</v>
       </c>
       <c r="F10" s="56" t="s">
-        <v>1241</v>
+        <v>1238</v>
       </c>
       <c r="G10" s="56" t="s">
-        <v>1241</v>
+        <v>1238</v>
       </c>
       <c r="H10" s="56" t="s">
         <v>10</v>
@@ -31552,7 +31543,7 @@
         <v>14</v>
       </c>
       <c r="K10" s="106" t="s">
-        <v>1277</v>
+        <v>1273</v>
       </c>
       <c r="L10" s="56" t="s">
         <v>197</v>
@@ -31587,7 +31578,7 @@
         <v>14</v>
       </c>
       <c r="K11" s="107" t="s">
-        <v>1278</v>
+        <v>1274</v>
       </c>
       <c r="L11" s="35" t="s">
         <v>557</v>
@@ -31622,7 +31613,7 @@
         <v>14</v>
       </c>
       <c r="K12" s="35" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="L12" s="35" t="s">
         <v>246</v>
@@ -31634,53 +31625,53 @@
     <row r="13" spans="1:22" s="23" customFormat="1" ht="24" x14ac:dyDescent="0.45">
       <c r="A13" s="103"/>
       <c r="B13" s="56" t="s">
-        <v>1240</v>
+        <v>1237</v>
       </c>
       <c r="C13" s="56"/>
       <c r="D13" s="52">
         <v>10</v>
       </c>
       <c r="E13" s="56" t="s">
-        <v>1126</v>
+        <v>1123</v>
       </c>
       <c r="F13" s="56" t="s">
-        <v>1125</v>
+        <v>1122</v>
       </c>
       <c r="G13" s="56" t="s">
-        <v>1234</v>
+        <v>1231</v>
       </c>
       <c r="H13" s="56" t="s">
-        <v>1127</v>
+        <v>1124</v>
       </c>
       <c r="I13" s="56" t="s">
         <v>11</v>
       </c>
       <c r="J13" s="56" t="s">
-        <v>1127</v>
+        <v>1124</v>
       </c>
       <c r="K13" s="35"/>
       <c r="L13" s="35" t="s">
-        <v>1130</v>
+        <v>1127</v>
       </c>
       <c r="M13" s="35"/>
     </row>
     <row r="14" spans="1:22" s="23" customFormat="1" ht="24" x14ac:dyDescent="0.45">
       <c r="A14" s="103"/>
       <c r="B14" s="56" t="s">
-        <v>1240</v>
+        <v>1237</v>
       </c>
       <c r="C14" s="56"/>
       <c r="D14" s="52">
         <v>11</v>
       </c>
       <c r="E14" s="56" t="s">
-        <v>1129</v>
+        <v>1126</v>
       </c>
       <c r="F14" s="34" t="s">
-        <v>1128</v>
+        <v>1125</v>
       </c>
       <c r="G14" s="34" t="s">
-        <v>1235</v>
+        <v>1232</v>
       </c>
       <c r="H14" s="56" t="s">
         <v>10</v>
@@ -31692,10 +31683,10 @@
         <v>14</v>
       </c>
       <c r="K14" s="107" t="s">
-        <v>1302</v>
+        <v>1298</v>
       </c>
       <c r="L14" s="35" t="s">
-        <v>1132</v>
+        <v>1129</v>
       </c>
       <c r="M14" s="35"/>
     </row>
@@ -31759,7 +31750,7 @@
       <c r="J16" s="56"/>
       <c r="K16" s="35"/>
       <c r="L16" s="35" t="s">
-        <v>1117</v>
+        <v>1114</v>
       </c>
       <c r="M16" s="35"/>
     </row>
@@ -31788,11 +31779,11 @@
       <c r="J17" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="K17" s="35" t="s">
-        <v>1046</v>
+      <c r="K17" s="107" t="s">
+        <v>1298</v>
       </c>
       <c r="L17" s="104" t="s">
-        <v>1116</v>
+        <v>1113</v>
       </c>
       <c r="M17" s="35"/>
     </row>
@@ -32017,10 +32008,10 @@
         <v>2</v>
       </c>
       <c r="E6" s="56" t="s">
-        <v>1108</v>
+        <v>1105</v>
       </c>
       <c r="F6" s="56" t="s">
-        <v>1106</v>
+        <v>1103</v>
       </c>
       <c r="G6" s="56" t="s">
         <v>899</v>
@@ -32034,7 +32025,7 @@
       <c r="J6" s="56"/>
       <c r="K6" s="34"/>
       <c r="L6" s="35" t="s">
-        <v>1107</v>
+        <v>1104</v>
       </c>
       <c r="M6" s="35" t="s">
         <v>189</v>
@@ -32043,20 +32034,20 @@
     <row r="7" spans="1:13" s="51" customFormat="1" ht="47.25" x14ac:dyDescent="0.45">
       <c r="A7" s="35"/>
       <c r="B7" s="56" t="s">
-        <v>1082</v>
+        <v>1079</v>
       </c>
       <c r="C7" s="56"/>
       <c r="D7" s="52">
         <v>3</v>
       </c>
       <c r="E7" s="56" t="s">
-        <v>1111</v>
+        <v>1108</v>
       </c>
       <c r="F7" s="56" t="s">
-        <v>1283</v>
+        <v>1279</v>
       </c>
       <c r="G7" s="56" t="s">
-        <v>1284</v>
+        <v>1280</v>
       </c>
       <c r="H7" s="56" t="s">
         <v>10</v>
@@ -32068,19 +32059,19 @@
         <v>14</v>
       </c>
       <c r="K7" s="111" t="s">
-        <v>1294</v>
+        <v>1290</v>
       </c>
       <c r="L7" s="35" t="s">
-        <v>1135</v>
+        <v>1132</v>
       </c>
       <c r="M7" s="35" t="s">
-        <v>1111</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="51" customFormat="1" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A8" s="35"/>
       <c r="B8" s="56" t="s">
-        <v>1082</v>
+        <v>1079</v>
       </c>
       <c r="C8" s="56"/>
       <c r="D8" s="52">
@@ -32090,10 +32081,10 @@
         <v>22</v>
       </c>
       <c r="F8" s="56" t="s">
-        <v>1133</v>
+        <v>1130</v>
       </c>
       <c r="G8" s="56" t="s">
-        <v>1134</v>
+        <v>1131</v>
       </c>
       <c r="H8" s="56" t="s">
         <v>10</v>
@@ -32108,10 +32099,10 @@
         <v>22</v>
       </c>
       <c r="L8" s="35" t="s">
-        <v>1114</v>
+        <v>1111</v>
       </c>
       <c r="M8" s="35" t="s">
-        <v>1112</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="51" customFormat="1" ht="24" x14ac:dyDescent="0.45">
@@ -32157,7 +32148,7 @@
         <v>6</v>
       </c>
       <c r="E10" s="56" t="s">
-        <v>1209</v>
+        <v>1206</v>
       </c>
       <c r="F10" s="35" t="s">
         <v>760</v>
@@ -32190,13 +32181,13 @@
         <v>7</v>
       </c>
       <c r="E11" s="56" t="s">
-        <v>1230</v>
+        <v>1227</v>
       </c>
       <c r="F11" s="56" t="s">
-        <v>1136</v>
+        <v>1133</v>
       </c>
       <c r="G11" s="56" t="s">
-        <v>1137</v>
+        <v>1134</v>
       </c>
       <c r="H11" s="56" t="s">
         <v>10</v>
@@ -32208,7 +32199,7 @@
         <v>14</v>
       </c>
       <c r="K11" s="106" t="s">
-        <v>1302</v>
+        <v>1298</v>
       </c>
       <c r="L11" s="35" t="s">
         <v>886</v>
@@ -32225,13 +32216,13 @@
         <v>8</v>
       </c>
       <c r="E12" s="56" t="s">
-        <v>1231</v>
+        <v>1228</v>
       </c>
       <c r="F12" s="56" t="s">
-        <v>1138</v>
+        <v>1135</v>
       </c>
       <c r="G12" s="56" t="s">
-        <v>1139</v>
+        <v>1136</v>
       </c>
       <c r="H12" s="56" t="s">
         <v>10</v>
@@ -32256,13 +32247,13 @@
         <v>9</v>
       </c>
       <c r="E13" s="56" t="s">
-        <v>1206</v>
+        <v>1203</v>
       </c>
       <c r="F13" s="56" t="s">
-        <v>1067</v>
+        <v>1064</v>
       </c>
       <c r="G13" s="56" t="s">
-        <v>1068</v>
+        <v>1065</v>
       </c>
       <c r="H13" s="56" t="s">
         <v>10</v>
@@ -32274,13 +32265,13 @@
         <v>14</v>
       </c>
       <c r="K13" s="34" t="s">
-        <v>1298</v>
+        <v>1294</v>
       </c>
       <c r="L13" s="35" t="s">
-        <v>1069</v>
+        <v>1066</v>
       </c>
       <c r="M13" s="56" t="s">
-        <v>1070</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="14" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.45">
@@ -32309,7 +32300,7 @@
         <v>14</v>
       </c>
       <c r="K14" s="106" t="s">
-        <v>1277</v>
+        <v>1273</v>
       </c>
       <c r="L14" s="56" t="s">
         <v>192</v>
@@ -32344,7 +32335,7 @@
         <v>14</v>
       </c>
       <c r="K15" s="106" t="s">
-        <v>1278</v>
+        <v>1274</v>
       </c>
       <c r="L15" s="56" t="s">
         <v>557</v>
@@ -32356,20 +32347,20 @@
     <row r="16" spans="1:13" s="51" customFormat="1" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A16" s="56"/>
       <c r="B16" s="56" t="s">
-        <v>1082</v>
+        <v>1079</v>
       </c>
       <c r="C16" s="56"/>
       <c r="D16" s="52">
         <v>12</v>
       </c>
       <c r="E16" s="56" t="s">
-        <v>1071</v>
+        <v>1068</v>
       </c>
       <c r="F16" s="56" t="s">
-        <v>1072</v>
+        <v>1069</v>
       </c>
       <c r="G16" s="56" t="s">
-        <v>1072</v>
+        <v>1069</v>
       </c>
       <c r="H16" s="56" t="s">
         <v>10</v>
@@ -32381,30 +32372,30 @@
         <v>14</v>
       </c>
       <c r="K16" s="34" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="L16" s="35" t="s">
-        <v>1073</v>
+        <v>1070</v>
       </c>
       <c r="M16" s="56"/>
     </row>
     <row r="17" spans="1:13" s="51" customFormat="1" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A17" s="56"/>
       <c r="B17" s="56" t="s">
-        <v>1082</v>
+        <v>1079</v>
       </c>
       <c r="C17" s="56"/>
       <c r="D17" s="52">
         <v>13</v>
       </c>
       <c r="E17" s="56" t="s">
-        <v>1074</v>
+        <v>1071</v>
       </c>
       <c r="F17" s="56" t="s">
-        <v>1075</v>
+        <v>1072</v>
       </c>
       <c r="G17" s="56" t="s">
-        <v>1076</v>
+        <v>1073</v>
       </c>
       <c r="H17" s="56" t="s">
         <v>10</v>
@@ -32416,30 +32407,30 @@
         <v>14</v>
       </c>
       <c r="K17" s="106" t="s">
-        <v>1290</v>
+        <v>1286</v>
       </c>
       <c r="L17" s="35" t="s">
-        <v>1077</v>
+        <v>1074</v>
       </c>
       <c r="M17" s="56"/>
     </row>
     <row r="18" spans="1:13" s="51" customFormat="1" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="56"/>
       <c r="B18" s="56" t="s">
-        <v>1082</v>
+        <v>1079</v>
       </c>
       <c r="C18" s="56"/>
       <c r="D18" s="52">
         <v>14</v>
       </c>
       <c r="E18" s="56" t="s">
-        <v>1078</v>
+        <v>1075</v>
       </c>
       <c r="F18" s="56" t="s">
-        <v>1238</v>
+        <v>1235</v>
       </c>
       <c r="G18" s="56" t="s">
-        <v>1239</v>
+        <v>1236</v>
       </c>
       <c r="H18" s="56" t="s">
         <v>148</v>
@@ -32450,30 +32441,30 @@
       <c r="J18" s="56"/>
       <c r="K18" s="34"/>
       <c r="L18" s="35" t="s">
-        <v>1079</v>
+        <v>1076</v>
       </c>
       <c r="M18" s="56"/>
     </row>
     <row r="19" spans="1:13" s="51" customFormat="1" ht="24" x14ac:dyDescent="0.45">
       <c r="A19" s="56"/>
       <c r="B19" s="56" t="s">
-        <v>1082</v>
+        <v>1079</v>
       </c>
       <c r="C19" s="56"/>
       <c r="D19" s="52">
         <v>15</v>
       </c>
       <c r="E19" s="56" t="s">
-        <v>1126</v>
+        <v>1123</v>
       </c>
       <c r="F19" s="56" t="s">
-        <v>1140</v>
+        <v>1137</v>
       </c>
       <c r="G19" s="56" t="s">
-        <v>1233</v>
+        <v>1230</v>
       </c>
       <c r="H19" s="56" t="s">
-        <v>1237</v>
+        <v>1234</v>
       </c>
       <c r="I19" s="56" t="s">
         <v>11</v>
@@ -32481,27 +32472,27 @@
       <c r="J19" s="56"/>
       <c r="K19" s="35"/>
       <c r="L19" s="35" t="s">
-        <v>1236</v>
+        <v>1233</v>
       </c>
       <c r="M19" s="35"/>
     </row>
     <row r="20" spans="1:13" s="51" customFormat="1" ht="24" x14ac:dyDescent="0.45">
       <c r="A20" s="56"/>
       <c r="B20" s="56" t="s">
-        <v>1082</v>
+        <v>1079</v>
       </c>
       <c r="C20" s="56"/>
       <c r="D20" s="52">
         <v>16</v>
       </c>
       <c r="E20" s="56" t="s">
-        <v>1129</v>
+        <v>1126</v>
       </c>
       <c r="F20" s="34" t="s">
-        <v>1141</v>
+        <v>1138</v>
       </c>
       <c r="G20" s="34" t="s">
-        <v>1232</v>
+        <v>1229</v>
       </c>
       <c r="H20" s="56" t="s">
         <v>10</v>
@@ -32513,10 +32504,10 @@
         <v>14</v>
       </c>
       <c r="K20" s="106" t="s">
-        <v>1302</v>
+        <v>1298</v>
       </c>
       <c r="L20" s="35" t="s">
-        <v>1132</v>
+        <v>1129</v>
       </c>
       <c r="M20" s="35"/>
     </row>
@@ -32528,7 +32519,7 @@
         <v>17</v>
       </c>
       <c r="E21" s="56" t="s">
-        <v>1207</v>
+        <v>1204</v>
       </c>
       <c r="F21" s="35" t="s">
         <v>828</v>
@@ -32559,7 +32550,7 @@
         <v>18</v>
       </c>
       <c r="E22" s="56" t="s">
-        <v>1208</v>
+        <v>1205</v>
       </c>
       <c r="F22" s="34" t="s">
         <v>782</v>
@@ -32670,7 +32661,7 @@
         <v>14</v>
       </c>
       <c r="K25" s="108" t="s">
-        <v>1286</v>
+        <v>1282</v>
       </c>
       <c r="L25" s="35" t="s">
         <v>196</v>
@@ -32755,7 +32746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
@@ -32915,7 +32906,7 @@
         <v>834</v>
       </c>
       <c r="L4" s="35" t="s">
-        <v>1242</v>
+        <v>1239</v>
       </c>
       <c r="M4" s="35" t="s">
         <v>108</v>
@@ -32947,13 +32938,13 @@
         <v>14</v>
       </c>
       <c r="K5" s="107" t="s">
-        <v>1299</v>
+        <v>1295</v>
       </c>
       <c r="L5" s="50" t="s">
         <v>1012</v>
       </c>
       <c r="M5" s="50" t="s">
-        <v>1243</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="10" customFormat="1" ht="11.65" x14ac:dyDescent="0.35">
@@ -33003,7 +32994,7 @@
         <v>5</v>
       </c>
       <c r="E7" s="35" t="s">
-        <v>1244</v>
+        <v>1241</v>
       </c>
       <c r="F7" s="35" t="s">
         <v>750</v>
@@ -33034,7 +33025,7 @@
         <v>6</v>
       </c>
       <c r="E8" s="35" t="s">
-        <v>1148</v>
+        <v>1145</v>
       </c>
       <c r="F8" s="35" t="s">
         <v>302</v>
@@ -33109,10 +33100,10 @@
         <v>689</v>
       </c>
       <c r="F10" s="34" t="s">
-        <v>1142</v>
+        <v>1139</v>
       </c>
       <c r="G10" s="34" t="s">
-        <v>1144</v>
+        <v>1141</v>
       </c>
       <c r="H10" s="35" t="s">
         <v>10</v>
@@ -33127,7 +33118,7 @@
         <v>1014</v>
       </c>
       <c r="L10" s="35" t="s">
-        <v>1146</v>
+        <v>1143</v>
       </c>
       <c r="M10" s="34"/>
     </row>
@@ -33142,10 +33133,10 @@
         <v>255</v>
       </c>
       <c r="F11" s="35" t="s">
-        <v>1143</v>
+        <v>1140</v>
       </c>
       <c r="G11" s="34" t="s">
-        <v>1145</v>
+        <v>1142</v>
       </c>
       <c r="H11" s="35" t="s">
         <v>10</v>
@@ -33157,7 +33148,7 @@
         <v>14</v>
       </c>
       <c r="K11" s="106" t="s">
-        <v>1301</v>
+        <v>1297</v>
       </c>
       <c r="L11" s="35" t="s">
         <v>255</v>
@@ -34075,7 +34066,7 @@
         <v>5</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>1149</v>
+        <v>1146</v>
       </c>
       <c r="F10" s="35" t="s">
         <v>751</v>
@@ -34092,7 +34083,7 @@
       <c r="J10" s="35"/>
       <c r="K10" s="35"/>
       <c r="L10" s="35" t="s">
-        <v>1245</v>
+        <v>1242</v>
       </c>
       <c r="M10" s="35" t="s">
         <v>120</v>
@@ -34106,7 +34097,7 @@
         <v>6</v>
       </c>
       <c r="E11" s="34" t="s">
-        <v>1150</v>
+        <v>1147</v>
       </c>
       <c r="F11" s="34" t="s">
         <v>315</v>
@@ -34141,7 +34132,7 @@
         <v>7</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>1151</v>
+        <v>1148</v>
       </c>
       <c r="F12" s="34" t="s">
         <v>316</v>
@@ -34207,7 +34198,7 @@
         <v>9</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>1152</v>
+        <v>1149</v>
       </c>
       <c r="F14" s="35" t="s">
         <v>813</v>
@@ -34238,7 +34229,7 @@
         <v>10</v>
       </c>
       <c r="E15" s="35" t="s">
-        <v>1153</v>
+        <v>1150</v>
       </c>
       <c r="F15" s="34" t="s">
         <v>761</v>
@@ -34349,7 +34340,7 @@
         <v>14</v>
       </c>
       <c r="K18" s="107" t="s">
-        <v>1286</v>
+        <v>1282</v>
       </c>
       <c r="L18" s="54" t="s">
         <v>201</v>
@@ -34397,7 +34388,7 @@
         <v>15</v>
       </c>
       <c r="E20" s="58" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
       <c r="F20" s="58" t="s">
         <v>320</v>
@@ -34415,7 +34406,7 @@
         <v>14</v>
       </c>
       <c r="K20" s="107" t="s">
-        <v>1286</v>
+        <v>1282</v>
       </c>
       <c r="L20" s="57" t="s">
         <v>524</v>
@@ -34432,7 +34423,7 @@
         <v>16</v>
       </c>
       <c r="E21" s="34" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
       <c r="F21" s="34" t="s">
         <v>812</v>
@@ -34463,7 +34454,7 @@
         <v>17</v>
       </c>
       <c r="E22" s="34" t="s">
-        <v>1156</v>
+        <v>1153</v>
       </c>
       <c r="F22" s="34" t="s">
         <v>762</v>
@@ -34605,7 +34596,7 @@
         <v>14</v>
       </c>
       <c r="K26" s="108" t="s">
-        <v>1301</v>
+        <v>1297</v>
       </c>
       <c r="L26" s="35" t="s">
         <v>255</v>
@@ -34869,10 +34860,10 @@
         <v>1014</v>
       </c>
       <c r="L6" s="35" t="s">
-        <v>1080</v>
+        <v>1077</v>
       </c>
       <c r="M6" s="35" t="s">
-        <v>1081</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="35.65" x14ac:dyDescent="0.45">
@@ -34883,7 +34874,7 @@
         <v>4</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>1228</v>
+        <v>1225</v>
       </c>
       <c r="F7" s="34" t="s">
         <v>944</v>
@@ -34918,13 +34909,13 @@
         <v>5</v>
       </c>
       <c r="E8" s="35" t="s">
+        <v>1216</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>1217</v>
+      </c>
+      <c r="G8" s="35" t="s">
         <v>1219</v>
-      </c>
-      <c r="F8" s="35" t="s">
-        <v>1220</v>
-      </c>
-      <c r="G8" s="35" t="s">
-        <v>1222</v>
       </c>
       <c r="H8" s="35" t="s">
         <v>10</v>
@@ -34950,13 +34941,13 @@
         <v>6</v>
       </c>
       <c r="E9" s="34" t="s">
-        <v>1227</v>
+        <v>1224</v>
       </c>
       <c r="F9" s="34" t="s">
-        <v>1215</v>
+        <v>1212</v>
       </c>
       <c r="G9" s="34" t="s">
-        <v>1221</v>
+        <v>1218</v>
       </c>
       <c r="H9" s="34" t="s">
         <v>10</v>
@@ -34968,7 +34959,7 @@
         <v>14</v>
       </c>
       <c r="K9" s="102" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="L9" s="59"/>
       <c r="M9" s="59"/>
@@ -34998,10 +34989,10 @@
       <c r="J10" s="35"/>
       <c r="K10" s="35"/>
       <c r="L10" s="35" t="s">
-        <v>1245</v>
+        <v>1242</v>
       </c>
       <c r="M10" s="35" t="s">
-        <v>1093</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="35.65" x14ac:dyDescent="0.45">
@@ -35047,7 +35038,7 @@
         <v>9</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>1158</v>
+        <v>1155</v>
       </c>
       <c r="F12" s="34" t="s">
         <v>350</v>
@@ -35113,7 +35104,7 @@
         <v>11</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>1157</v>
+        <v>1154</v>
       </c>
       <c r="F14" s="35" t="s">
         <v>814</v>
@@ -35144,7 +35135,7 @@
         <v>12</v>
       </c>
       <c r="E15" s="35" t="s">
-        <v>1159</v>
+        <v>1156</v>
       </c>
       <c r="F15" s="34" t="s">
         <v>763</v>
@@ -35255,7 +35246,7 @@
         <v>14</v>
       </c>
       <c r="K18" s="107" t="s">
-        <v>1286</v>
+        <v>1282</v>
       </c>
       <c r="L18" s="35" t="s">
         <v>201</v>
@@ -35303,7 +35294,7 @@
         <v>17</v>
       </c>
       <c r="E20" s="34" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
       <c r="F20" s="34" t="s">
         <v>324</v>
@@ -35321,7 +35312,7 @@
         <v>14</v>
       </c>
       <c r="K20" s="107" t="s">
-        <v>1286</v>
+        <v>1282</v>
       </c>
       <c r="L20" s="35" t="s">
         <v>524</v>
@@ -35338,7 +35329,7 @@
         <v>18</v>
       </c>
       <c r="E21" s="34" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
       <c r="F21" s="34" t="s">
         <v>815</v>
@@ -35369,7 +35360,7 @@
         <v>19</v>
       </c>
       <c r="E22" s="34" t="s">
-        <v>1156</v>
+        <v>1153</v>
       </c>
       <c r="F22" s="34" t="s">
         <v>764</v>
@@ -35511,7 +35502,7 @@
         <v>14</v>
       </c>
       <c r="K26" s="107" t="s">
-        <v>1301</v>
+        <v>1297</v>
       </c>
       <c r="L26" s="35" t="s">
         <v>255</v>
@@ -35774,7 +35765,7 @@
         <v>1003</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>1048</v>
+        <v>1045</v>
       </c>
       <c r="M5" s="6" t="s">
         <v>115</v>
@@ -36106,7 +36097,7 @@
         <v>3</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>1160</v>
+        <v>1157</v>
       </c>
       <c r="F8" s="12" t="s">
         <v>580</v>
@@ -36121,11 +36112,11 @@
         <v>11</v>
       </c>
       <c r="J8" s="35" t="s">
-        <v>1049</v>
+        <v>1046</v>
       </c>
       <c r="K8" s="34"/>
       <c r="L8" s="35" t="s">
-        <v>1050</v>
+        <v>1047</v>
       </c>
       <c r="M8" s="35" t="s">
         <v>577</v>
@@ -36160,10 +36151,10 @@
         <v>1014</v>
       </c>
       <c r="L9" s="35" t="s">
-        <v>1080</v>
+        <v>1077</v>
       </c>
       <c r="M9" s="35" t="s">
-        <v>1081</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.45">
@@ -36174,7 +36165,7 @@
         <v>5</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>1161</v>
+        <v>1158</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>753</v>
@@ -36191,10 +36182,10 @@
       <c r="J10" s="35"/>
       <c r="K10" s="34"/>
       <c r="L10" s="35" t="s">
-        <v>1245</v>
+        <v>1242</v>
       </c>
       <c r="M10" s="35" t="s">
-        <v>1093</v>
+        <v>1090</v>
       </c>
     </row>
     <row r="11" spans="1:13" s="1" customFormat="1" ht="24" x14ac:dyDescent="0.45">
@@ -36240,7 +36231,7 @@
         <v>7</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>1158</v>
+        <v>1155</v>
       </c>
       <c r="F12" s="15" t="s">
         <v>353</v>
@@ -36306,7 +36297,7 @@
         <v>9</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>1152</v>
+        <v>1149</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>691</v>
@@ -36337,7 +36328,7 @@
         <v>10</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>1162</v>
+        <v>1159</v>
       </c>
       <c r="F15" s="15" t="s">
         <v>694</v>
@@ -36448,7 +36439,7 @@
         <v>14</v>
       </c>
       <c r="K18" s="108" t="s">
-        <v>1286</v>
+        <v>1282</v>
       </c>
       <c r="L18" s="12" t="s">
         <v>122</v>
@@ -36496,7 +36487,7 @@
         <v>15</v>
       </c>
       <c r="E20" s="15" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
       <c r="F20" s="15" t="s">
         <v>328</v>
@@ -36514,7 +36505,7 @@
         <v>14</v>
       </c>
       <c r="K20" s="108" t="s">
-        <v>1286</v>
+        <v>1282</v>
       </c>
       <c r="L20" s="12" t="s">
         <v>524</v>
@@ -36531,7 +36522,7 @@
         <v>16</v>
       </c>
       <c r="E21" s="15" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
       <c r="F21" s="15" t="s">
         <v>816</v>
@@ -36562,7 +36553,7 @@
         <v>17</v>
       </c>
       <c r="E22" s="15" t="s">
-        <v>1156</v>
+        <v>1153</v>
       </c>
       <c r="F22" s="15" t="s">
         <v>765</v>
@@ -36704,7 +36695,7 @@
         <v>14</v>
       </c>
       <c r="K26" s="108" t="s">
-        <v>1301</v>
+        <v>1297</v>
       </c>
       <c r="L26" s="12" t="s">
         <v>255</v>
@@ -36746,7 +36737,7 @@
   <dimension ref="A1:N41"/>
   <sheetViews>
     <sheetView topLeftCell="C10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K37" sqref="K37"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -37084,7 +37075,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>1160</v>
+        <v>1157</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>855</v>
@@ -37099,11 +37090,11 @@
         <v>11</v>
       </c>
       <c r="J10" s="12" t="s">
-        <v>1051</v>
+        <v>1048</v>
       </c>
       <c r="K10" s="12"/>
       <c r="L10" s="12" t="s">
-        <v>1052</v>
+        <v>1049</v>
       </c>
       <c r="M10" s="12"/>
     </row>
@@ -37169,10 +37160,10 @@
         <v>1014</v>
       </c>
       <c r="L12" s="35" t="s">
-        <v>1080</v>
+        <v>1077</v>
       </c>
       <c r="M12" s="35" t="s">
-        <v>1081</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.45">
@@ -37183,7 +37174,7 @@
         <v>5</v>
       </c>
       <c r="E13" s="35" t="s">
-        <v>1163</v>
+        <v>1160</v>
       </c>
       <c r="F13" s="35" t="s">
         <v>754</v>
@@ -37200,7 +37191,7 @@
       <c r="J13" s="35"/>
       <c r="K13" s="35"/>
       <c r="L13" s="35" t="s">
-        <v>1245</v>
+        <v>1242</v>
       </c>
       <c r="M13" s="35" t="s">
         <v>120</v>
@@ -37214,7 +37205,7 @@
         <v>6</v>
       </c>
       <c r="E14" s="34" t="s">
-        <v>1164</v>
+        <v>1161</v>
       </c>
       <c r="F14" s="34" t="s">
         <v>279</v>
@@ -37249,7 +37240,7 @@
         <v>7</v>
       </c>
       <c r="E15" s="34" t="s">
-        <v>1165</v>
+        <v>1162</v>
       </c>
       <c r="F15" s="34" t="s">
         <v>280</v>
@@ -37336,10 +37327,10 @@
         <v>1020</v>
       </c>
       <c r="L17" s="52" t="s">
-        <v>1246</v>
+        <v>1243</v>
       </c>
       <c r="M17" s="52" t="s">
-        <v>1246</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="18" spans="1:14" s="2" customFormat="1" ht="35.65" x14ac:dyDescent="0.45">
@@ -37350,10 +37341,10 @@
         <v>10</v>
       </c>
       <c r="E18" s="35" t="s">
-        <v>1247</v>
+        <v>1244</v>
       </c>
       <c r="F18" s="35" t="s">
-        <v>1248</v>
+        <v>1245</v>
       </c>
       <c r="G18" s="35" t="s">
         <v>290</v>
@@ -37369,10 +37360,10 @@
       </c>
       <c r="K18" s="35"/>
       <c r="L18" s="35" t="s">
-        <v>1249</v>
+        <v>1246</v>
       </c>
       <c r="M18" s="35" t="s">
-        <v>1250</v>
+        <v>1247</v>
       </c>
       <c r="N18" s="101"/>
     </row>
@@ -37405,10 +37396,10 @@
         <v>1018</v>
       </c>
       <c r="L19" s="35" t="s">
-        <v>1251</v>
+        <v>1248</v>
       </c>
       <c r="M19" s="35" t="s">
-        <v>1251</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="20" spans="1:14" s="2" customFormat="1" ht="24" x14ac:dyDescent="0.45">
@@ -37467,10 +37458,10 @@
       <c r="J21" s="35"/>
       <c r="K21" s="35"/>
       <c r="L21" s="35" t="s">
-        <v>1252</v>
+        <v>1249</v>
       </c>
       <c r="M21" s="35" t="s">
-        <v>1253</v>
+        <v>1250</v>
       </c>
     </row>
     <row r="22" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.45">
@@ -37520,7 +37511,7 @@
         <v>15</v>
       </c>
       <c r="E23" s="35" t="s">
-        <v>1254</v>
+        <v>1251</v>
       </c>
       <c r="F23" s="35" t="s">
         <v>250</v>
@@ -37568,10 +37559,10 @@
       <c r="J24" s="35"/>
       <c r="K24" s="35"/>
       <c r="L24" s="35" t="s">
-        <v>1255</v>
+        <v>1252</v>
       </c>
       <c r="M24" s="35" t="s">
-        <v>1256</v>
+        <v>1253</v>
       </c>
     </row>
     <row r="25" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.45">
@@ -37582,7 +37573,7 @@
         <v>17</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>1166</v>
+        <v>1163</v>
       </c>
       <c r="F25" s="12" t="s">
         <v>817</v>
@@ -37613,7 +37604,7 @@
         <v>18</v>
       </c>
       <c r="E26" s="15" t="s">
-        <v>1167</v>
+        <v>1164</v>
       </c>
       <c r="F26" s="15" t="s">
         <v>771</v>
@@ -37724,7 +37715,7 @@
         <v>14</v>
       </c>
       <c r="K29" s="109" t="s">
-        <v>1286</v>
+        <v>1282</v>
       </c>
       <c r="L29" s="35" t="s">
         <v>562</v>
@@ -37772,7 +37763,7 @@
         <v>23</v>
       </c>
       <c r="E31" s="34" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
       <c r="F31" s="34" t="s">
         <v>287</v>
@@ -37788,7 +37779,7 @@
         <v>14</v>
       </c>
       <c r="K31" s="109" t="s">
-        <v>1286</v>
+        <v>1282</v>
       </c>
       <c r="L31" s="35" t="s">
         <v>524</v>
@@ -37805,7 +37796,7 @@
         <v>24</v>
       </c>
       <c r="E32" s="34" t="s">
-        <v>1168</v>
+        <v>1165</v>
       </c>
       <c r="F32" s="34" t="s">
         <v>818</v>
@@ -37836,7 +37827,7 @@
         <v>25</v>
       </c>
       <c r="E33" s="34" t="s">
-        <v>1169</v>
+        <v>1166</v>
       </c>
       <c r="F33" s="34" t="s">
         <v>772</v>
@@ -37978,7 +37969,7 @@
         <v>14</v>
       </c>
       <c r="K37" s="109" t="s">
-        <v>1301</v>
+        <v>1297</v>
       </c>
       <c r="L37" s="35" t="s">
         <v>255</v>
@@ -38296,10 +38287,10 @@
         <v>1014</v>
       </c>
       <c r="L6" s="35" t="s">
-        <v>1080</v>
+        <v>1077</v>
       </c>
       <c r="M6" s="35" t="s">
-        <v>1081</v>
+        <v>1078</v>
       </c>
       <c r="N6" s="90"/>
     </row>
@@ -38343,7 +38334,7 @@
         <v>4</v>
       </c>
       <c r="E8" s="34" t="s">
-        <v>1178</v>
+        <v>1175</v>
       </c>
       <c r="F8" s="35" t="s">
         <v>755</v>
@@ -38360,7 +38351,7 @@
       <c r="J8" s="34"/>
       <c r="K8" s="34"/>
       <c r="L8" s="35" t="s">
-        <v>1245</v>
+        <v>1242</v>
       </c>
       <c r="M8" s="35" t="s">
         <v>120</v>
@@ -38411,7 +38402,7 @@
         <v>6</v>
       </c>
       <c r="E10" s="34" t="s">
-        <v>1158</v>
+        <v>1155</v>
       </c>
       <c r="F10" s="34" t="s">
         <v>356</v>
@@ -38587,7 +38578,7 @@
         <v>11</v>
       </c>
       <c r="E15" s="34" t="s">
-        <v>1170</v>
+        <v>1167</v>
       </c>
       <c r="F15" s="34" t="s">
         <v>449</v>
@@ -38604,10 +38595,10 @@
       <c r="J15" s="34"/>
       <c r="K15" s="34"/>
       <c r="L15" s="35" t="s">
-        <v>1091</v>
+        <v>1088</v>
       </c>
       <c r="M15" s="35" t="s">
-        <v>1091</v>
+        <v>1088</v>
       </c>
       <c r="N15" s="90"/>
     </row>
@@ -38619,7 +38610,7 @@
         <v>12</v>
       </c>
       <c r="E16" s="34" t="s">
-        <v>1171</v>
+        <v>1168</v>
       </c>
       <c r="F16" s="34" t="s">
         <v>450</v>
@@ -38636,10 +38627,10 @@
       <c r="J16" s="34"/>
       <c r="K16" s="34"/>
       <c r="L16" s="35" t="s">
-        <v>1092</v>
+        <v>1089</v>
       </c>
       <c r="M16" s="35" t="s">
-        <v>1092</v>
+        <v>1089</v>
       </c>
       <c r="N16" s="90"/>
     </row>
@@ -38651,7 +38642,7 @@
         <v>13</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>1172</v>
+        <v>1169</v>
       </c>
       <c r="F17" s="34" t="s">
         <v>451</v>
@@ -38668,10 +38659,10 @@
       <c r="J17" s="34"/>
       <c r="K17" s="34"/>
       <c r="L17" s="35" t="s">
-        <v>1257</v>
+        <v>1254</v>
       </c>
       <c r="M17" s="35" t="s">
-        <v>1257</v>
+        <v>1254</v>
       </c>
       <c r="N17" s="90"/>
     </row>
@@ -38683,7 +38674,7 @@
         <v>14</v>
       </c>
       <c r="E18" s="34" t="s">
-        <v>1173</v>
+        <v>1170</v>
       </c>
       <c r="F18" s="34" t="s">
         <v>452</v>
@@ -38700,10 +38691,10 @@
       <c r="J18" s="34"/>
       <c r="K18" s="34"/>
       <c r="L18" s="35" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="M18" s="35" t="s">
-        <v>1258</v>
+        <v>1255</v>
       </c>
       <c r="N18" s="90"/>
     </row>
@@ -38732,10 +38723,10 @@
       <c r="J19" s="34"/>
       <c r="K19" s="34"/>
       <c r="L19" s="35" t="s">
-        <v>1259</v>
+        <v>1256</v>
       </c>
       <c r="M19" s="35" t="s">
-        <v>1260</v>
+        <v>1257</v>
       </c>
       <c r="N19" s="90"/>
     </row>
@@ -38744,16 +38735,16 @@
       <c r="B20" s="15"/>
       <c r="C20" s="15"/>
       <c r="D20" s="56" t="s">
+        <v>1079</v>
+      </c>
+      <c r="E20" s="34" t="s">
+        <v>1080</v>
+      </c>
+      <c r="F20" s="34" t="s">
+        <v>1081</v>
+      </c>
+      <c r="G20" s="34" t="s">
         <v>1082</v>
-      </c>
-      <c r="E20" s="34" t="s">
-        <v>1083</v>
-      </c>
-      <c r="F20" s="34" t="s">
-        <v>1084</v>
-      </c>
-      <c r="G20" s="34" t="s">
-        <v>1085</v>
       </c>
       <c r="H20" s="34" t="s">
         <v>10</v>
@@ -38765,13 +38756,13 @@
         <v>14</v>
       </c>
       <c r="K20" s="106" t="s">
-        <v>1296</v>
+        <v>1292</v>
       </c>
       <c r="L20" s="35" t="s">
-        <v>1086</v>
+        <v>1083</v>
       </c>
       <c r="M20" s="35" t="s">
-        <v>1086</v>
+        <v>1083</v>
       </c>
       <c r="N20" s="90"/>
     </row>
@@ -38780,16 +38771,16 @@
       <c r="B21" s="15"/>
       <c r="C21" s="15"/>
       <c r="D21" s="56" t="s">
-        <v>1082</v>
+        <v>1079</v>
       </c>
       <c r="E21" s="34" t="s">
-        <v>1087</v>
+        <v>1084</v>
       </c>
       <c r="F21" s="34" t="s">
-        <v>1088</v>
+        <v>1085</v>
       </c>
       <c r="G21" s="34" t="s">
-        <v>1089</v>
+        <v>1086</v>
       </c>
       <c r="H21" s="34" t="s">
         <v>13</v>
@@ -38800,10 +38791,10 @@
       <c r="J21" s="34"/>
       <c r="K21" s="34"/>
       <c r="L21" s="35" t="s">
-        <v>1090</v>
+        <v>1087</v>
       </c>
       <c r="M21" s="35" t="s">
-        <v>1090</v>
+        <v>1087</v>
       </c>
       <c r="N21" s="90"/>
     </row>
@@ -38943,7 +38934,7 @@
         <v>20</v>
       </c>
       <c r="E26" s="34" t="s">
-        <v>1174</v>
+        <v>1171</v>
       </c>
       <c r="F26" s="34" t="s">
         <v>863</v>
@@ -39036,7 +39027,7 @@
         <v>1026</v>
       </c>
       <c r="L28" s="35" t="s">
-        <v>1053</v>
+        <v>1050</v>
       </c>
       <c r="M28" s="35" t="s">
         <v>139</v>
@@ -39072,10 +39063,10 @@
         <v>1027</v>
       </c>
       <c r="L29" s="35" t="s">
-        <v>1054</v>
+        <v>1051</v>
       </c>
       <c r="M29" s="35" t="s">
-        <v>1054</v>
+        <v>1051</v>
       </c>
       <c r="N29" s="90"/>
     </row>
@@ -39108,10 +39099,10 @@
         <v>1028</v>
       </c>
       <c r="L30" s="35" t="s">
-        <v>1055</v>
+        <v>1052</v>
       </c>
       <c r="M30" s="35" t="s">
-        <v>1055</v>
+        <v>1052</v>
       </c>
       <c r="N30" s="90"/>
     </row>
@@ -39123,7 +39114,7 @@
         <v>25</v>
       </c>
       <c r="E31" s="34" t="s">
-        <v>1261</v>
+        <v>1258</v>
       </c>
       <c r="F31" s="34" t="s">
         <v>466</v>
@@ -39140,7 +39131,7 @@
       <c r="J31" s="34"/>
       <c r="K31" s="34"/>
       <c r="L31" s="35" t="s">
-        <v>1147</v>
+        <v>1144</v>
       </c>
       <c r="M31" s="35" t="s">
         <v>140</v>
@@ -39155,7 +39146,7 @@
         <v>26</v>
       </c>
       <c r="E32" s="34" t="s">
-        <v>1262</v>
+        <v>1259</v>
       </c>
       <c r="F32" s="34" t="s">
         <v>468</v>
@@ -39208,7 +39199,7 @@
         <v>1029</v>
       </c>
       <c r="L33" s="35" t="s">
-        <v>1056</v>
+        <v>1053</v>
       </c>
       <c r="M33" s="35" t="s">
         <v>619</v>
@@ -39381,13 +39372,13 @@
         <v>14</v>
       </c>
       <c r="K38" s="106" t="s">
-        <v>1295</v>
+        <v>1291</v>
       </c>
       <c r="L38" s="35" t="s">
-        <v>1263</v>
+        <v>1260</v>
       </c>
       <c r="M38" s="35" t="s">
-        <v>1264</v>
+        <v>1261</v>
       </c>
       <c r="N38" s="90"/>
     </row>
@@ -39466,13 +39457,13 @@
         <v>35</v>
       </c>
       <c r="E41" s="34" t="s">
-        <v>1265</v>
+        <v>1262</v>
       </c>
       <c r="F41" s="34" t="s">
-        <v>1266</v>
+        <v>1263</v>
       </c>
       <c r="G41" s="34" t="s">
-        <v>1267</v>
+        <v>1264</v>
       </c>
       <c r="H41" s="34" t="s">
         <v>10</v>
@@ -39484,13 +39475,13 @@
         <v>14</v>
       </c>
       <c r="K41" s="106" t="s">
-        <v>1287</v>
+        <v>1283</v>
       </c>
       <c r="L41" s="35" t="s">
-        <v>1211</v>
+        <v>1208</v>
       </c>
       <c r="M41" s="35" t="s">
-        <v>1104</v>
+        <v>1101</v>
       </c>
       <c r="N41" s="98"/>
     </row>
@@ -39499,16 +39490,16 @@
       <c r="B42" s="15"/>
       <c r="C42" s="15"/>
       <c r="D42" s="56" t="s">
-        <v>1082</v>
+        <v>1079</v>
       </c>
       <c r="E42" s="34" t="s">
+        <v>1095</v>
+      </c>
+      <c r="F42" s="34" t="s">
+        <v>1091</v>
+      </c>
+      <c r="G42" s="34" t="s">
         <v>1098</v>
-      </c>
-      <c r="F42" s="34" t="s">
-        <v>1094</v>
-      </c>
-      <c r="G42" s="34" t="s">
-        <v>1101</v>
       </c>
       <c r="H42" s="34" t="s">
         <v>10</v>
@@ -39520,13 +39511,13 @@
         <v>14</v>
       </c>
       <c r="K42" s="106" t="s">
-        <v>1288</v>
+        <v>1284</v>
       </c>
       <c r="L42" s="35" t="s">
-        <v>1212</v>
+        <v>1209</v>
       </c>
       <c r="M42" s="35" t="s">
-        <v>1095</v>
+        <v>1092</v>
       </c>
       <c r="N42" s="97"/>
     </row>
@@ -39535,16 +39526,16 @@
       <c r="B43" s="15"/>
       <c r="C43" s="15"/>
       <c r="D43" s="56" t="s">
-        <v>1082</v>
+        <v>1079</v>
       </c>
       <c r="E43" s="34" t="s">
+        <v>1096</v>
+      </c>
+      <c r="F43" s="34" t="s">
+        <v>1093</v>
+      </c>
+      <c r="G43" s="34" t="s">
         <v>1099</v>
-      </c>
-      <c r="F43" s="34" t="s">
-        <v>1096</v>
-      </c>
-      <c r="G43" s="34" t="s">
-        <v>1102</v>
       </c>
       <c r="H43" s="34" t="s">
         <v>10</v>
@@ -39556,13 +39547,13 @@
         <v>14</v>
       </c>
       <c r="K43" s="106" t="s">
-        <v>1287</v>
+        <v>1283</v>
       </c>
       <c r="L43" s="35" t="s">
-        <v>1210</v>
+        <v>1207</v>
       </c>
       <c r="M43" s="35" t="s">
-        <v>1105</v>
+        <v>1102</v>
       </c>
       <c r="N43" s="98"/>
     </row>
@@ -39571,16 +39562,16 @@
       <c r="B44" s="15"/>
       <c r="C44" s="15"/>
       <c r="D44" s="56" t="s">
-        <v>1082</v>
+        <v>1079</v>
       </c>
       <c r="E44" s="34" t="s">
+        <v>1097</v>
+      </c>
+      <c r="F44" s="34" t="s">
+        <v>1094</v>
+      </c>
+      <c r="G44" s="34" t="s">
         <v>1100</v>
-      </c>
-      <c r="F44" s="34" t="s">
-        <v>1097</v>
-      </c>
-      <c r="G44" s="34" t="s">
-        <v>1103</v>
       </c>
       <c r="H44" s="34" t="s">
         <v>10</v>
@@ -39592,13 +39583,13 @@
         <v>14</v>
       </c>
       <c r="K44" s="106" t="s">
-        <v>1288</v>
+        <v>1284</v>
       </c>
       <c r="L44" s="35" t="s">
-        <v>1213</v>
+        <v>1210</v>
       </c>
       <c r="M44" s="35" t="s">
-        <v>1214</v>
+        <v>1211</v>
       </c>
       <c r="N44" s="97"/>
     </row>
@@ -39639,7 +39630,7 @@
         <v>37</v>
       </c>
       <c r="E46" s="12" t="s">
-        <v>1175</v>
+        <v>1172</v>
       </c>
       <c r="F46" s="12" t="s">
         <v>567</v>
@@ -39657,7 +39648,7 @@
         <v>14</v>
       </c>
       <c r="K46" s="108" t="s">
-        <v>1289</v>
+        <v>1285</v>
       </c>
       <c r="L46" s="12" t="s">
         <v>840</v>
@@ -39674,7 +39665,7 @@
         <v>38</v>
       </c>
       <c r="E47" s="15" t="s">
-        <v>1176</v>
+        <v>1173</v>
       </c>
       <c r="F47" s="12" t="s">
         <v>819</v>
@@ -39705,7 +39696,7 @@
         <v>39</v>
       </c>
       <c r="E48" s="15" t="s">
-        <v>1177</v>
+        <v>1174</v>
       </c>
       <c r="F48" s="15" t="s">
         <v>773</v>
@@ -39722,7 +39713,7 @@
       <c r="J48" s="15"/>
       <c r="K48" s="15"/>
       <c r="L48" s="12" t="s">
-        <v>1057</v>
+        <v>1054</v>
       </c>
       <c r="M48" s="12" t="s">
         <v>1002</v>
@@ -39816,7 +39807,7 @@
         <v>14</v>
       </c>
       <c r="K51" s="108" t="s">
-        <v>1286</v>
+        <v>1282</v>
       </c>
       <c r="L51" s="12" t="s">
         <v>138</v>
@@ -39864,7 +39855,7 @@
         <v>44</v>
       </c>
       <c r="E53" s="15" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
       <c r="F53" s="15" t="s">
         <v>332</v>
@@ -39880,7 +39871,7 @@
         <v>14</v>
       </c>
       <c r="K53" s="108" t="s">
-        <v>1286</v>
+        <v>1282</v>
       </c>
       <c r="L53" s="12" t="s">
         <v>524</v>
@@ -39897,7 +39888,7 @@
         <v>45</v>
       </c>
       <c r="E54" s="15" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
       <c r="F54" s="15" t="s">
         <v>820</v>
@@ -39928,7 +39919,7 @@
         <v>46</v>
       </c>
       <c r="E55" s="15" t="s">
-        <v>1156</v>
+        <v>1153</v>
       </c>
       <c r="F55" s="15" t="s">
         <v>774</v>
@@ -40071,7 +40062,7 @@
         <v>14</v>
       </c>
       <c r="K59" s="108" t="s">
-        <v>1301</v>
+        <v>1297</v>
       </c>
       <c r="L59" s="12" t="s">
         <v>255</v>
@@ -40417,10 +40408,10 @@
         <v>1014</v>
       </c>
       <c r="L6" s="35" t="s">
-        <v>1080</v>
+        <v>1077</v>
       </c>
       <c r="M6" s="35" t="s">
-        <v>1081</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="24" x14ac:dyDescent="0.45">
@@ -40433,7 +40424,7 @@
         <v>4</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>1228</v>
+        <v>1225</v>
       </c>
       <c r="F7" s="34" t="s">
         <v>628</v>
@@ -40472,13 +40463,13 @@
         <v>5</v>
       </c>
       <c r="E8" s="35" t="s">
-        <v>1226</v>
+        <v>1223</v>
       </c>
       <c r="F8" s="34" t="s">
-        <v>1224</v>
+        <v>1221</v>
       </c>
       <c r="G8" s="34" t="s">
-        <v>1225</v>
+        <v>1222</v>
       </c>
       <c r="H8" s="34" t="s">
         <v>10</v>
@@ -40504,7 +40495,7 @@
         <v>6</v>
       </c>
       <c r="E9" s="34" t="s">
-        <v>1227</v>
+        <v>1224</v>
       </c>
       <c r="F9" s="34" t="s">
         <v>432</v>
@@ -40522,7 +40513,7 @@
         <v>14</v>
       </c>
       <c r="K9" s="102" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="L9" s="35" t="s">
         <v>151</v>
@@ -40605,7 +40596,7 @@
         <v>9</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>1179</v>
+        <v>1176</v>
       </c>
       <c r="F12" s="35" t="s">
         <v>756</v>
@@ -40622,7 +40613,7 @@
       <c r="J12" s="34"/>
       <c r="K12" s="34"/>
       <c r="L12" s="35" t="s">
-        <v>1245</v>
+        <v>1242</v>
       </c>
       <c r="M12" s="35" t="s">
         <v>120</v>
@@ -40671,7 +40662,7 @@
         <v>11</v>
       </c>
       <c r="E14" s="34" t="s">
-        <v>1158</v>
+        <v>1155</v>
       </c>
       <c r="F14" s="34" t="s">
         <v>359</v>
@@ -40772,7 +40763,7 @@
         <v>14</v>
       </c>
       <c r="E17" s="34" t="s">
-        <v>1180</v>
+        <v>1177</v>
       </c>
       <c r="F17" s="34" t="s">
         <v>430</v>
@@ -40803,7 +40794,7 @@
         <v>15</v>
       </c>
       <c r="E18" s="34" t="s">
-        <v>1181</v>
+        <v>1178</v>
       </c>
       <c r="F18" s="35" t="s">
         <v>821</v>
@@ -40834,7 +40825,7 @@
         <v>16</v>
       </c>
       <c r="E19" s="34" t="s">
-        <v>1182</v>
+        <v>1179</v>
       </c>
       <c r="F19" s="34" t="s">
         <v>775</v>
@@ -40945,7 +40936,7 @@
         <v>14</v>
       </c>
       <c r="K22" s="106" t="s">
-        <v>1286</v>
+        <v>1282</v>
       </c>
       <c r="L22" s="35" t="s">
         <v>150</v>
@@ -40993,7 +40984,7 @@
         <v>21</v>
       </c>
       <c r="E24" s="34" t="s">
-        <v>1154</v>
+        <v>1151</v>
       </c>
       <c r="F24" s="34" t="s">
         <v>336</v>
@@ -41011,7 +41002,7 @@
         <v>14</v>
       </c>
       <c r="K24" s="106" t="s">
-        <v>1286</v>
+        <v>1282</v>
       </c>
       <c r="L24" s="35" t="s">
         <v>524</v>
@@ -41028,7 +41019,7 @@
         <v>22</v>
       </c>
       <c r="E25" s="34" t="s">
-        <v>1155</v>
+        <v>1152</v>
       </c>
       <c r="F25" s="34" t="s">
         <v>822</v>
@@ -41051,7 +41042,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="2" customFormat="1" ht="24" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:13" s="2" customFormat="1" ht="35.65" x14ac:dyDescent="0.45">
       <c r="A26" s="15"/>
       <c r="B26" s="34"/>
       <c r="C26" s="34"/>
@@ -41059,7 +41050,7 @@
         <v>23</v>
       </c>
       <c r="E26" s="34" t="s">
-        <v>1156</v>
+        <v>1153</v>
       </c>
       <c r="F26" s="34" t="s">
         <v>776</v>
@@ -41171,7 +41162,7 @@
         <v>1014</v>
       </c>
       <c r="L29" s="35" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="M29" s="34"/>
     </row>
@@ -41201,7 +41192,7 @@
         <v>14</v>
       </c>
       <c r="K30" s="106" t="s">
-        <v>1301</v>
+        <v>1297</v>
       </c>
       <c r="L30" s="35" t="s">
         <v>255</v>
@@ -41221,6 +41212,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100584B29A9F606E64BBE0B94B46ABEDBD5" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ad12f995843361ff338b3798f1f5f41c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4d5313c0-c1e6-4122-afa9-da1ccdba405d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8fda66a02b6b5d1f39f2000ab0f58af4" ns2:_="">
     <xsd:import namespace="4d5313c0-c1e6-4122-afa9-da1ccdba405d"/>
@@ -41392,15 +41392,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -41414,6 +41405,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04CD8B6C-25F0-471A-A724-387AC1B5060F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F67F35D-1CDD-4110-B6CE-1A6865489AEE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -41427,14 +41426,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{04CD8B6C-25F0-471A-A724-387AC1B5060F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>